<commit_message>
Update 360 Giving grants files
Update 360 Giving grant CSV and Excel files
</commit_message>
<xml_diff>
--- a/open/grants.xlsx
+++ b/open/grants.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/westsi/Documents/GitHub/zing/open/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2651CE06-BB85-CF4B-94C8-C40141427F76}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A488DA9D-8E4A-FD4C-A0F2-9DBCFE2372C8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1378" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1420" uniqueCount="470">
   <si>
     <t>Identifier</t>
   </si>
@@ -1460,6 +1460,21 @@
   </si>
   <si>
     <t>NE11 0HW</t>
+  </si>
+  <si>
+    <t>360G-zing-68</t>
+  </si>
+  <si>
+    <t>Funding to continue scaling the Village Investor Programme (VIP) which enables communities to economically support vulnerable children for the long term.</t>
+  </si>
+  <si>
+    <t>360G-zing-69</t>
+  </si>
+  <si>
+    <t>Platform analytics development</t>
+  </si>
+  <si>
+    <t>Project funding to expand upon Peace First's platform analytics, building a greater understanding of the participant user journey, including any points of attrition. This work will also enable future A/B testing of different types of intervention/support, and their effectiveness when implemented at different stages of the journey.</t>
   </si>
 </sst>
 </file>
@@ -1979,10 +1994,10 @@
   <dimension ref="A1:AL75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C59" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="G73" sqref="G73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2235,7 +2250,7 @@
       <c r="AJ2" s="6"/>
       <c r="AK2" s="13">
         <f t="shared" ref="AK2:AK60" ca="1" si="0">NOW()</f>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL2" s="14" t="s">
         <v>335</v>
@@ -2332,7 +2347,7 @@
       <c r="AJ3" s="6"/>
       <c r="AK3" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL3" s="14" t="s">
         <v>335</v>
@@ -2429,7 +2444,7 @@
       <c r="AJ4" s="6"/>
       <c r="AK4" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL4" s="14" t="s">
         <v>335</v>
@@ -2526,7 +2541,7 @@
       <c r="AJ5" s="6"/>
       <c r="AK5" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL5" s="14" t="s">
         <v>335</v>
@@ -2623,7 +2638,7 @@
       <c r="AJ6" s="6"/>
       <c r="AK6" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL6" s="14" t="s">
         <v>335</v>
@@ -2720,7 +2735,7 @@
       <c r="AJ7" s="6"/>
       <c r="AK7" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL7" s="14" t="s">
         <v>335</v>
@@ -2817,7 +2832,7 @@
       <c r="AJ8" s="6"/>
       <c r="AK8" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL8" s="14" t="s">
         <v>335</v>
@@ -2912,7 +2927,7 @@
       <c r="AJ9" s="6"/>
       <c r="AK9" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL9" s="14" t="s">
         <v>335</v>
@@ -3009,7 +3024,7 @@
       <c r="AJ10" s="6"/>
       <c r="AK10" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL10" s="14" t="s">
         <v>335</v>
@@ -3104,7 +3119,7 @@
       <c r="AJ11" s="6"/>
       <c r="AK11" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL11" s="14" t="s">
         <v>335</v>
@@ -3201,7 +3216,7 @@
       <c r="AJ12" s="6"/>
       <c r="AK12" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL12" s="14" t="s">
         <v>335</v>
@@ -3296,7 +3311,7 @@
       <c r="AJ13" s="6"/>
       <c r="AK13" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL13" s="14" t="s">
         <v>335</v>
@@ -3393,7 +3408,7 @@
       <c r="AJ14" s="6"/>
       <c r="AK14" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL14" s="14" t="s">
         <v>335</v>
@@ -3488,7 +3503,7 @@
       <c r="AJ15" s="6"/>
       <c r="AK15" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL15" s="14" t="s">
         <v>335</v>
@@ -3583,7 +3598,7 @@
       <c r="AJ16" s="6"/>
       <c r="AK16" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL16" s="14" t="s">
         <v>335</v>
@@ -3680,7 +3695,7 @@
       <c r="AJ17" s="6"/>
       <c r="AK17" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL17" s="14" t="s">
         <v>335</v>
@@ -3777,7 +3792,7 @@
       <c r="AJ18" s="6"/>
       <c r="AK18" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL18" s="14" t="s">
         <v>335</v>
@@ -3872,7 +3887,7 @@
       <c r="AJ19" s="6"/>
       <c r="AK19" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL19" s="14" t="s">
         <v>335</v>
@@ -3967,7 +3982,7 @@
       <c r="AJ20" s="6"/>
       <c r="AK20" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL20" s="14" t="s">
         <v>335</v>
@@ -4064,7 +4079,7 @@
       <c r="AJ21" s="6"/>
       <c r="AK21" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL21" s="14" t="s">
         <v>335</v>
@@ -4159,7 +4174,7 @@
       <c r="AJ22" s="6"/>
       <c r="AK22" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL22" s="14" t="s">
         <v>335</v>
@@ -4256,7 +4271,7 @@
       <c r="AJ23" s="6"/>
       <c r="AK23" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL23" s="14" t="s">
         <v>335</v>
@@ -4353,7 +4368,7 @@
       <c r="AJ24" s="6"/>
       <c r="AK24" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL24" s="14" t="s">
         <v>335</v>
@@ -4448,7 +4463,7 @@
       <c r="AJ25" s="6"/>
       <c r="AK25" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL25" s="14" t="s">
         <v>335</v>
@@ -4545,7 +4560,7 @@
       <c r="AJ26" s="6"/>
       <c r="AK26" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL26" s="14" t="s">
         <v>335</v>
@@ -4642,7 +4657,7 @@
       <c r="AJ27" s="6"/>
       <c r="AK27" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL27" s="14" t="s">
         <v>335</v>
@@ -4737,7 +4752,7 @@
       <c r="AJ28" s="6"/>
       <c r="AK28" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL28" s="14" t="s">
         <v>335</v>
@@ -4834,7 +4849,7 @@
       <c r="AJ29" s="6"/>
       <c r="AK29" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL29" s="14" t="s">
         <v>335</v>
@@ -4929,7 +4944,7 @@
       <c r="AJ30" s="6"/>
       <c r="AK30" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL30" s="14" t="s">
         <v>335</v>
@@ -5026,7 +5041,7 @@
       <c r="AJ31" s="6"/>
       <c r="AK31" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL31" s="14" t="s">
         <v>335</v>
@@ -5123,7 +5138,7 @@
       <c r="AJ32" s="6"/>
       <c r="AK32" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL32" s="14" t="s">
         <v>335</v>
@@ -5220,7 +5235,7 @@
       <c r="AJ33" s="6"/>
       <c r="AK33" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL33" s="14" t="s">
         <v>335</v>
@@ -5317,7 +5332,7 @@
       <c r="AJ34" s="6"/>
       <c r="AK34" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL34" s="14" t="s">
         <v>335</v>
@@ -5412,7 +5427,7 @@
       <c r="AJ35" s="6"/>
       <c r="AK35" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL35" s="14" t="s">
         <v>335</v>
@@ -5509,7 +5524,7 @@
       <c r="AJ36" s="6"/>
       <c r="AK36" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL36" s="14" t="s">
         <v>335</v>
@@ -5604,7 +5619,7 @@
       <c r="AJ37" s="6"/>
       <c r="AK37" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL37" s="14" t="s">
         <v>335</v>
@@ -5701,7 +5716,7 @@
       <c r="AJ38" s="6"/>
       <c r="AK38" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL38" s="14" t="s">
         <v>335</v>
@@ -5798,7 +5813,7 @@
       <c r="AJ39" s="6"/>
       <c r="AK39" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL39" s="14" t="s">
         <v>335</v>
@@ -5895,7 +5910,7 @@
       <c r="AJ40" s="6"/>
       <c r="AK40" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL40" s="14" t="s">
         <v>335</v>
@@ -5992,7 +6007,7 @@
       <c r="AJ41" s="6"/>
       <c r="AK41" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL41" s="14" t="s">
         <v>335</v>
@@ -6089,7 +6104,7 @@
       <c r="AJ42" s="6"/>
       <c r="AK42" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL42" s="14" t="s">
         <v>335</v>
@@ -6186,7 +6201,7 @@
       <c r="AJ43" s="6"/>
       <c r="AK43" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL43" s="14" t="s">
         <v>335</v>
@@ -6281,7 +6296,7 @@
       <c r="AJ44" s="6"/>
       <c r="AK44" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL44" s="14" t="s">
         <v>335</v>
@@ -6378,7 +6393,7 @@
       <c r="AJ45" s="6"/>
       <c r="AK45" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL45" s="14" t="s">
         <v>335</v>
@@ -6473,7 +6488,7 @@
       <c r="AJ46" s="6"/>
       <c r="AK46" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL46" s="14" t="s">
         <v>335</v>
@@ -6570,7 +6585,7 @@
       <c r="AJ47" s="6"/>
       <c r="AK47" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL47" s="14" t="s">
         <v>335</v>
@@ -6665,7 +6680,7 @@
       <c r="AJ48" s="6"/>
       <c r="AK48" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL48" s="14" t="s">
         <v>335</v>
@@ -6762,7 +6777,7 @@
       <c r="AJ49" s="6"/>
       <c r="AK49" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL49" s="14" t="s">
         <v>335</v>
@@ -6859,7 +6874,7 @@
       <c r="AJ50" s="6"/>
       <c r="AK50" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL50" s="14" t="s">
         <v>335</v>
@@ -6954,7 +6969,7 @@
       <c r="AJ51" s="6"/>
       <c r="AK51" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL51" s="14" t="s">
         <v>335</v>
@@ -7051,7 +7066,7 @@
       <c r="AJ52" s="6"/>
       <c r="AK52" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL52" s="14" t="s">
         <v>335</v>
@@ -7148,7 +7163,7 @@
       <c r="AJ53" s="6"/>
       <c r="AK53" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL53" s="14" t="s">
         <v>335</v>
@@ -7242,7 +7257,7 @@
       </c>
       <c r="AK54" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL54" s="14" t="s">
         <v>335</v>
@@ -7337,7 +7352,7 @@
       <c r="AJ55" s="24"/>
       <c r="AK55" s="24">
         <f ca="1">NOW()</f>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL55" s="14" t="s">
         <v>335</v>
@@ -7434,7 +7449,7 @@
       <c r="AJ56" s="24"/>
       <c r="AK56" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL56" s="14" t="s">
         <v>335</v>
@@ -7531,7 +7546,7 @@
       <c r="AJ57" s="6"/>
       <c r="AK57" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL57" s="14" t="s">
         <v>335</v>
@@ -7626,7 +7641,7 @@
       <c r="AJ58" s="6"/>
       <c r="AK58" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL58" s="14" t="s">
         <v>335</v>
@@ -7723,7 +7738,7 @@
       <c r="AJ59" s="6"/>
       <c r="AK59" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL59" s="14" t="s">
         <v>335</v>
@@ -7820,7 +7835,7 @@
       <c r="AJ60" s="6"/>
       <c r="AK60" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL60" s="14" t="s">
         <v>335</v>
@@ -7913,7 +7928,7 @@
       <c r="AJ61" s="6"/>
       <c r="AK61" s="13">
         <f ca="1">NOW()</f>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL61" s="14" t="s">
         <v>335</v>
@@ -8006,7 +8021,7 @@
       <c r="AJ62" s="6"/>
       <c r="AK62" s="13">
         <f ca="1">NOW()</f>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL62" s="14" t="s">
         <v>335</v>
@@ -8099,7 +8114,7 @@
       <c r="AJ63" s="6"/>
       <c r="AK63" s="13">
         <f ca="1">NOW()</f>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL63" s="14" t="s">
         <v>335</v>
@@ -8193,8 +8208,8 @@
       </c>
       <c r="AJ64" s="6"/>
       <c r="AK64" s="13">
-        <f t="shared" ref="AK64:AK66" ca="1" si="1">NOW()</f>
-        <v>43655.517574189813</v>
+        <f t="shared" ref="AK64:AK68" ca="1" si="1">NOW()</f>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL64" s="14" t="s">
         <v>335</v>
@@ -8289,7 +8304,7 @@
       <c r="AJ65" s="6"/>
       <c r="AK65" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL65" s="14" t="s">
         <v>335</v>
@@ -8384,91 +8399,199 @@
       <c r="AJ66" s="6"/>
       <c r="AK66" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>43655.517574189813</v>
+        <v>43707.550085763891</v>
       </c>
       <c r="AL66" s="14" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="67" spans="1:38" ht="14" x14ac:dyDescent="0.15">
-      <c r="A67" s="6"/>
-      <c r="B67" s="6"/>
-      <c r="C67" s="6"/>
-      <c r="D67" s="6"/>
-      <c r="E67" s="8"/>
-      <c r="F67" s="8"/>
-      <c r="G67" s="6"/>
-      <c r="H67" s="9"/>
-      <c r="I67" s="6"/>
-      <c r="J67" s="9"/>
-      <c r="K67" s="9"/>
+    <row r="67" spans="1:38" ht="28" x14ac:dyDescent="0.15">
+      <c r="A67" s="6" t="s">
+        <v>465</v>
+      </c>
+      <c r="B67" s="11" t="s">
+        <v>329</v>
+      </c>
+      <c r="C67" s="7" t="s">
+        <v>466</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E67" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="F67" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="G67" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="H67" s="9">
+        <v>43556</v>
+      </c>
+      <c r="I67" s="14" t="s">
+        <v>332</v>
+      </c>
+      <c r="J67" s="9">
+        <v>43556</v>
+      </c>
+      <c r="K67" s="9">
+        <v>43922</v>
+      </c>
       <c r="L67" s="9"/>
-      <c r="M67" s="6"/>
-      <c r="N67" s="6"/>
-      <c r="O67" s="6"/>
-      <c r="P67" s="26"/>
-      <c r="Q67" s="8"/>
-      <c r="R67" s="6"/>
-      <c r="S67" s="6"/>
-      <c r="T67" s="6"/>
-      <c r="U67" s="7"/>
-      <c r="V67" s="6"/>
+      <c r="M67" s="6">
+        <v>12</v>
+      </c>
+      <c r="N67" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="O67" s="11" t="s">
+        <v>321</v>
+      </c>
+      <c r="P67" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q67" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="R67" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="S67" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="T67" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="U67" s="15" t="s">
+        <v>330</v>
+      </c>
+      <c r="V67" s="14" t="s">
+        <v>331</v>
+      </c>
       <c r="W67" s="6"/>
       <c r="X67" s="6"/>
       <c r="Y67" s="6"/>
       <c r="Z67" s="6"/>
       <c r="AA67" s="6"/>
       <c r="AB67" s="6"/>
-      <c r="AC67" s="6"/>
-      <c r="AD67" s="6"/>
+      <c r="AC67" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD67" s="6" t="s">
+        <v>50</v>
+      </c>
       <c r="AE67" s="6"/>
       <c r="AF67" s="6"/>
-      <c r="AG67" s="6"/>
+      <c r="AG67" s="6" t="s">
+        <v>50</v>
+      </c>
       <c r="AH67" s="6"/>
-      <c r="AI67" s="6"/>
+      <c r="AI67" s="19" t="s">
+        <v>51</v>
+      </c>
       <c r="AJ67" s="6"/>
-      <c r="AK67" s="13"/>
-      <c r="AL67" s="6"/>
+      <c r="AK67" s="13">
+        <f t="shared" ca="1" si="1"/>
+        <v>43707.550085763891</v>
+      </c>
+      <c r="AL67" s="14" t="s">
+        <v>335</v>
+      </c>
     </row>
-    <row r="68" spans="1:38" ht="14" x14ac:dyDescent="0.15">
-      <c r="A68" s="6"/>
-      <c r="B68" s="6"/>
-      <c r="C68" s="6"/>
-      <c r="D68" s="6"/>
-      <c r="E68" s="8"/>
-      <c r="F68" s="8"/>
-      <c r="G68" s="6"/>
-      <c r="H68" s="9"/>
-      <c r="I68" s="6"/>
-      <c r="J68" s="9"/>
-      <c r="K68" s="9"/>
+    <row r="68" spans="1:38" ht="42" x14ac:dyDescent="0.15">
+      <c r="A68" s="6" t="s">
+        <v>467</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>468</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="E68" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="F68" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="G68" s="6">
+        <v>30000</v>
+      </c>
+      <c r="H68" s="9">
+        <v>43677</v>
+      </c>
+      <c r="I68" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="J68" s="9">
+        <v>43677</v>
+      </c>
+      <c r="K68" s="9">
+        <v>44043</v>
+      </c>
       <c r="L68" s="9"/>
-      <c r="M68" s="6"/>
-      <c r="N68" s="6"/>
-      <c r="O68" s="6"/>
-      <c r="P68" s="26"/>
+      <c r="M68" s="6">
+        <v>12</v>
+      </c>
+      <c r="N68" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="O68" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="P68" s="25" t="s">
+        <v>311</v>
+      </c>
       <c r="Q68" s="8"/>
-      <c r="R68" s="6"/>
-      <c r="S68" s="6"/>
-      <c r="T68" s="6"/>
-      <c r="U68" s="7"/>
-      <c r="V68" s="6"/>
+      <c r="R68" s="6" t="s">
+        <v>381</v>
+      </c>
+      <c r="S68" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="T68" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="U68" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="V68" s="14" t="s">
+        <v>380</v>
+      </c>
       <c r="W68" s="6"/>
       <c r="X68" s="6"/>
       <c r="Y68" s="6"/>
       <c r="Z68" s="6"/>
       <c r="AA68" s="6"/>
       <c r="AB68" s="6"/>
-      <c r="AC68" s="6"/>
-      <c r="AD68" s="6"/>
+      <c r="AC68" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD68" s="6" t="s">
+        <v>50</v>
+      </c>
       <c r="AE68" s="6"/>
       <c r="AF68" s="6"/>
-      <c r="AG68" s="6"/>
+      <c r="AG68" s="6" t="s">
+        <v>50</v>
+      </c>
       <c r="AH68" s="6"/>
-      <c r="AI68" s="6"/>
+      <c r="AI68" s="19" t="s">
+        <v>51</v>
+      </c>
       <c r="AJ68" s="6"/>
-      <c r="AK68" s="13"/>
-      <c r="AL68" s="6"/>
+      <c r="AK68" s="13">
+        <f t="shared" ca="1" si="1"/>
+        <v>43707.550085763891</v>
+      </c>
+      <c r="AL68" s="14" t="s">
+        <v>335</v>
+      </c>
     </row>
     <row r="69" spans="1:38" ht="14" x14ac:dyDescent="0.15">
       <c r="A69" s="6"/>
@@ -8758,8 +8881,14 @@
     <hyperlink ref="V64" r:id="rId77" xr:uid="{22C23FB9-7687-CF46-8D88-8B37722E18AE}"/>
     <hyperlink ref="I65" r:id="rId78" xr:uid="{0D3BF5C6-C362-0945-9B82-36EA9151FA12}"/>
     <hyperlink ref="V65" r:id="rId79" xr:uid="{92DB7632-D1CD-E14B-8A29-76F677800927}"/>
+    <hyperlink ref="I67" r:id="rId80" xr:uid="{AD10AF4D-D56C-B24D-8DBB-B86F368813E1}"/>
+    <hyperlink ref="V67" r:id="rId81" xr:uid="{4C6A55CE-5199-8A42-A3B7-CE4B70CC9418}"/>
+    <hyperlink ref="AL67" r:id="rId82" xr:uid="{174C7705-EA16-3646-92C0-FCB355FFE75C}"/>
+    <hyperlink ref="AL68" r:id="rId83" xr:uid="{A901E03A-725E-C741-94C8-61B9D2FAE211}"/>
+    <hyperlink ref="I68" r:id="rId84" xr:uid="{31305DFC-424C-BE4B-A96E-5BFCDE782066}"/>
+    <hyperlink ref="V68" r:id="rId85" xr:uid="{C302D653-12FD-9348-8F28-ACBBFD2EF9F1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId80"/>
+  <legacyDrawing r:id="rId86"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update 360 Giving grants data
Add The Difference and Young Trustees Movement grants to our published data.
</commit_message>
<xml_diff>
--- a/open/grants.xlsx
+++ b/open/grants.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/westsi/Documents/GitHub/zing/open/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A488DA9D-8E4A-FD4C-A0F2-9DBCFE2372C8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C6DBEE-EE56-104B-B563-23B7412E4694}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1420" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1461" uniqueCount="490">
   <si>
     <t>Identifier</t>
   </si>
@@ -1243,9 +1243,6 @@
     <t>Matched core funding for the iWill campaign team</t>
   </si>
   <si>
-    <t>Seed funding to The Difference (incubated within Catch 22): a new career route, creating specialist teaching leaders positioned to drive inclusion in schools, and make the difference for the UK’s most vulnerable young people.</t>
-  </si>
-  <si>
     <t>https://www.catch-22.org.uk</t>
   </si>
   <si>
@@ -1475,6 +1472,69 @@
   </si>
   <si>
     <t>Project funding to expand upon Peace First's platform analytics, building a greater understanding of the participant user journey, including any points of attrition. This work will also enable future A/B testing of different types of intervention/support, and their effectiveness when implemented at different stages of the journey.</t>
+  </si>
+  <si>
+    <t>Core funding for recruitment of a second teacher cohort</t>
+  </si>
+  <si>
+    <t>360G-zing-70</t>
+  </si>
+  <si>
+    <t>360G-zing-71</t>
+  </si>
+  <si>
+    <t>Seed funding toward the recruitment and training of The Difference's second cohort of leaders (now a registered charity). A new career route, creating specialist teaching leaders positioned to drive inclusion in schools, and improve outcomes for the UK’s most vulnerable young people.</t>
+  </si>
+  <si>
+    <t>Seed funding to The Difference (incubated within Catch 22): a new career route, creating specialist teaching leaders positioned to drive inclusion in schools, and improve outcomes for the UK’s most vulnerable young people.</t>
+  </si>
+  <si>
+    <t>1184843</t>
+  </si>
+  <si>
+    <t>GB-CHC-1184843</t>
+  </si>
+  <si>
+    <t>The Difference Education Ltd</t>
+  </si>
+  <si>
+    <t>11426427</t>
+  </si>
+  <si>
+    <t>E5 0RU</t>
+  </si>
+  <si>
+    <t>12 Mildenhall Road</t>
+  </si>
+  <si>
+    <t>https://youngtrusteesmovement.org/</t>
+  </si>
+  <si>
+    <t>Core funding toward the start of movement to increase the diversity of people on charity trustee boards, starting with a focus on doubling the number of young people under 30 on boards in the UK, by 2024 (currently 3%).</t>
+  </si>
+  <si>
+    <t>1164021</t>
+  </si>
+  <si>
+    <t>GB-CHC-1164021</t>
+  </si>
+  <si>
+    <t>The Blagrave Trust</t>
+  </si>
+  <si>
+    <t>4th Floor, 18 St Cross St</t>
+  </si>
+  <si>
+    <t>EC1N 8UN</t>
+  </si>
+  <si>
+    <t>Less than 3% of charity trustees are under 30. The Young Trustees Movements aims to change that, through a movement supporting youth in their preparation to become a trustee; through encouraging greater diversity at the board level; and working with recruiters to bridge between the two. The movement's initial focus is to increase age diversity, with a broader goal of increasing trustee board diversity in general.</t>
+  </si>
+  <si>
+    <t>https://www.blagravetrust.org/</t>
+  </si>
+  <si>
+    <t>Core funding toward the start of the Young Trustee Movement</t>
   </si>
 </sst>
 </file>
@@ -1485,7 +1545,7 @@
     <numFmt numFmtId="164" formatCode="yyyy&quot;-&quot;mm&quot;-&quot;dd"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\Thh:mm:ss\Z"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1550,6 +1610,16 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1578,7 +1648,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1671,6 +1741,9 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1994,10 +2067,10 @@
   <dimension ref="A1:AL75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C59" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C65" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G73" sqref="G73"/>
+      <selection pane="bottomRight" activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2250,7 +2323,7 @@
       <c r="AJ2" s="6"/>
       <c r="AK2" s="13">
         <f t="shared" ref="AK2:AK60" ca="1" si="0">NOW()</f>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL2" s="14" t="s">
         <v>335</v>
@@ -2347,7 +2420,7 @@
       <c r="AJ3" s="6"/>
       <c r="AK3" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL3" s="14" t="s">
         <v>335</v>
@@ -2444,7 +2517,7 @@
       <c r="AJ4" s="6"/>
       <c r="AK4" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL4" s="14" t="s">
         <v>335</v>
@@ -2541,7 +2614,7 @@
       <c r="AJ5" s="6"/>
       <c r="AK5" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL5" s="14" t="s">
         <v>335</v>
@@ -2638,7 +2711,7 @@
       <c r="AJ6" s="6"/>
       <c r="AK6" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL6" s="14" t="s">
         <v>335</v>
@@ -2735,7 +2808,7 @@
       <c r="AJ7" s="6"/>
       <c r="AK7" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL7" s="14" t="s">
         <v>335</v>
@@ -2832,7 +2905,7 @@
       <c r="AJ8" s="6"/>
       <c r="AK8" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL8" s="14" t="s">
         <v>335</v>
@@ -2927,7 +3000,7 @@
       <c r="AJ9" s="6"/>
       <c r="AK9" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL9" s="14" t="s">
         <v>335</v>
@@ -3024,7 +3097,7 @@
       <c r="AJ10" s="6"/>
       <c r="AK10" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL10" s="14" t="s">
         <v>335</v>
@@ -3119,7 +3192,7 @@
       <c r="AJ11" s="6"/>
       <c r="AK11" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL11" s="14" t="s">
         <v>335</v>
@@ -3130,7 +3203,7 @@
         <v>107</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>109</v>
@@ -3151,7 +3224,7 @@
         <v>41244</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="J12" s="9">
         <v>41244</v>
@@ -3190,7 +3263,7 @@
         <v>115</v>
       </c>
       <c r="V12" s="10" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="W12" s="6"/>
       <c r="X12" s="6"/>
@@ -3216,7 +3289,7 @@
       <c r="AJ12" s="6"/>
       <c r="AK12" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL12" s="14" t="s">
         <v>335</v>
@@ -3227,7 +3300,7 @@
         <v>116</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>118</v>
@@ -3248,7 +3321,7 @@
         <v>41456</v>
       </c>
       <c r="I13" s="10" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="J13" s="9">
         <v>41456</v>
@@ -3285,7 +3358,7 @@
         <v>124</v>
       </c>
       <c r="V13" s="10" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="W13" s="6"/>
       <c r="X13" s="6"/>
@@ -3311,7 +3384,7 @@
       <c r="AJ13" s="6"/>
       <c r="AK13" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL13" s="14" t="s">
         <v>335</v>
@@ -3408,7 +3481,7 @@
       <c r="AJ14" s="6"/>
       <c r="AK14" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL14" s="14" t="s">
         <v>335</v>
@@ -3503,7 +3576,7 @@
       <c r="AJ15" s="6"/>
       <c r="AK15" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL15" s="14" t="s">
         <v>335</v>
@@ -3598,7 +3671,7 @@
       <c r="AJ16" s="6"/>
       <c r="AK16" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL16" s="14" t="s">
         <v>335</v>
@@ -3695,7 +3768,7 @@
       <c r="AJ17" s="6"/>
       <c r="AK17" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL17" s="14" t="s">
         <v>335</v>
@@ -3706,7 +3779,7 @@
         <v>135</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>136</v>
@@ -3727,7 +3800,7 @@
         <v>41609</v>
       </c>
       <c r="I18" s="10" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="J18" s="9">
         <v>41609</v>
@@ -3766,7 +3839,7 @@
         <v>115</v>
       </c>
       <c r="V18" s="10" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="W18" s="6"/>
       <c r="X18" s="6"/>
@@ -3792,7 +3865,7 @@
       <c r="AJ18" s="6"/>
       <c r="AK18" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL18" s="14" t="s">
         <v>335</v>
@@ -3887,7 +3960,7 @@
       <c r="AJ19" s="6"/>
       <c r="AK19" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL19" s="14" t="s">
         <v>335</v>
@@ -3982,7 +4055,7 @@
       <c r="AJ20" s="6"/>
       <c r="AK20" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL20" s="14" t="s">
         <v>335</v>
@@ -4079,7 +4152,7 @@
       <c r="AJ21" s="6"/>
       <c r="AK21" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL21" s="14" t="s">
         <v>335</v>
@@ -4174,7 +4247,7 @@
       <c r="AJ22" s="6"/>
       <c r="AK22" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL22" s="14" t="s">
         <v>335</v>
@@ -4271,7 +4344,7 @@
       <c r="AJ23" s="6"/>
       <c r="AK23" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL23" s="14" t="s">
         <v>335</v>
@@ -4368,7 +4441,7 @@
       <c r="AJ24" s="6"/>
       <c r="AK24" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL24" s="14" t="s">
         <v>335</v>
@@ -4463,7 +4536,7 @@
       <c r="AJ25" s="6"/>
       <c r="AK25" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL25" s="14" t="s">
         <v>335</v>
@@ -4474,7 +4547,7 @@
         <v>174</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>175</v>
@@ -4495,7 +4568,7 @@
         <v>42036</v>
       </c>
       <c r="I26" s="10" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="J26" s="9">
         <v>42036</v>
@@ -4534,7 +4607,7 @@
         <v>115</v>
       </c>
       <c r="V26" s="10" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="W26" s="6"/>
       <c r="X26" s="6"/>
@@ -4560,7 +4633,7 @@
       <c r="AJ26" s="6"/>
       <c r="AK26" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL26" s="14" t="s">
         <v>335</v>
@@ -4657,7 +4730,7 @@
       <c r="AJ27" s="6"/>
       <c r="AK27" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL27" s="14" t="s">
         <v>335</v>
@@ -4752,7 +4825,7 @@
       <c r="AJ28" s="6"/>
       <c r="AK28" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL28" s="14" t="s">
         <v>335</v>
@@ -4849,7 +4922,7 @@
       <c r="AJ29" s="6"/>
       <c r="AK29" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL29" s="14" t="s">
         <v>335</v>
@@ -4944,7 +5017,7 @@
       <c r="AJ30" s="6"/>
       <c r="AK30" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL30" s="14" t="s">
         <v>335</v>
@@ -5041,7 +5114,7 @@
       <c r="AJ31" s="6"/>
       <c r="AK31" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL31" s="14" t="s">
         <v>335</v>
@@ -5138,7 +5211,7 @@
       <c r="AJ32" s="6"/>
       <c r="AK32" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL32" s="14" t="s">
         <v>335</v>
@@ -5235,7 +5308,7 @@
       <c r="AJ33" s="6"/>
       <c r="AK33" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL33" s="14" t="s">
         <v>335</v>
@@ -5332,7 +5405,7 @@
       <c r="AJ34" s="6"/>
       <c r="AK34" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL34" s="14" t="s">
         <v>335</v>
@@ -5427,7 +5500,7 @@
       <c r="AJ35" s="6"/>
       <c r="AK35" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL35" s="14" t="s">
         <v>335</v>
@@ -5524,7 +5597,7 @@
       <c r="AJ36" s="6"/>
       <c r="AK36" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL36" s="14" t="s">
         <v>335</v>
@@ -5619,7 +5692,7 @@
       <c r="AJ37" s="6"/>
       <c r="AK37" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL37" s="14" t="s">
         <v>335</v>
@@ -5716,7 +5789,7 @@
       <c r="AJ38" s="6"/>
       <c r="AK38" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL38" s="14" t="s">
         <v>335</v>
@@ -5813,7 +5886,7 @@
       <c r="AJ39" s="6"/>
       <c r="AK39" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL39" s="14" t="s">
         <v>335</v>
@@ -5910,7 +5983,7 @@
       <c r="AJ40" s="6"/>
       <c r="AK40" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL40" s="14" t="s">
         <v>335</v>
@@ -6007,7 +6080,7 @@
       <c r="AJ41" s="6"/>
       <c r="AK41" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL41" s="14" t="s">
         <v>335</v>
@@ -6104,7 +6177,7 @@
       <c r="AJ42" s="6"/>
       <c r="AK42" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL42" s="14" t="s">
         <v>335</v>
@@ -6201,7 +6274,7 @@
       <c r="AJ43" s="6"/>
       <c r="AK43" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL43" s="14" t="s">
         <v>335</v>
@@ -6296,7 +6369,7 @@
       <c r="AJ44" s="6"/>
       <c r="AK44" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL44" s="14" t="s">
         <v>335</v>
@@ -6393,7 +6466,7 @@
       <c r="AJ45" s="6"/>
       <c r="AK45" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL45" s="14" t="s">
         <v>335</v>
@@ -6488,7 +6561,7 @@
       <c r="AJ46" s="6"/>
       <c r="AK46" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL46" s="14" t="s">
         <v>335</v>
@@ -6585,7 +6658,7 @@
       <c r="AJ47" s="6"/>
       <c r="AK47" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL47" s="14" t="s">
         <v>335</v>
@@ -6680,7 +6753,7 @@
       <c r="AJ48" s="6"/>
       <c r="AK48" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL48" s="14" t="s">
         <v>335</v>
@@ -6777,7 +6850,7 @@
       <c r="AJ49" s="6"/>
       <c r="AK49" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL49" s="14" t="s">
         <v>335</v>
@@ -6874,7 +6947,7 @@
       <c r="AJ50" s="6"/>
       <c r="AK50" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL50" s="14" t="s">
         <v>335</v>
@@ -6969,7 +7042,7 @@
       <c r="AJ51" s="6"/>
       <c r="AK51" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL51" s="14" t="s">
         <v>335</v>
@@ -7066,7 +7139,7 @@
       <c r="AJ52" s="6"/>
       <c r="AK52" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL52" s="14" t="s">
         <v>335</v>
@@ -7163,7 +7236,7 @@
       <c r="AJ53" s="6"/>
       <c r="AK53" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL53" s="14" t="s">
         <v>335</v>
@@ -7257,7 +7330,7 @@
       </c>
       <c r="AK54" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL54" s="14" t="s">
         <v>335</v>
@@ -7352,7 +7425,7 @@
       <c r="AJ55" s="24"/>
       <c r="AK55" s="24">
         <f ca="1">NOW()</f>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL55" s="14" t="s">
         <v>335</v>
@@ -7449,7 +7522,7 @@
       <c r="AJ56" s="24"/>
       <c r="AK56" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL56" s="14" t="s">
         <v>335</v>
@@ -7546,7 +7619,7 @@
       <c r="AJ57" s="6"/>
       <c r="AK57" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL57" s="14" t="s">
         <v>335</v>
@@ -7641,7 +7714,7 @@
       <c r="AJ58" s="6"/>
       <c r="AK58" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL58" s="14" t="s">
         <v>335</v>
@@ -7652,10 +7725,10 @@
         <v>315</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>392</v>
+        <v>473</v>
       </c>
       <c r="D59" s="6" t="s">
         <v>40</v>
@@ -7688,16 +7761,16 @@
         <v>10</v>
       </c>
       <c r="N59" s="6" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="O59" s="11" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="P59" s="25" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="Q59" s="8" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="R59" s="6" t="s">
         <v>317</v>
@@ -7712,7 +7785,7 @@
         <v>319</v>
       </c>
       <c r="V59" s="17" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="W59" s="6"/>
       <c r="X59" s="6"/>
@@ -7738,7 +7811,7 @@
       <c r="AJ59" s="6"/>
       <c r="AK59" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL59" s="14" t="s">
         <v>335</v>
@@ -7835,7 +7908,7 @@
       <c r="AJ60" s="6"/>
       <c r="AK60" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL60" s="14" t="s">
         <v>335</v>
@@ -7843,13 +7916,13 @@
     </row>
     <row r="61" spans="1:38" ht="14" x14ac:dyDescent="0.15">
       <c r="A61" s="6" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B61" s="11" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C61" s="15" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D61" s="6" t="s">
         <v>40</v>
@@ -7867,7 +7940,7 @@
         <v>43252</v>
       </c>
       <c r="I61" s="14" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="J61" s="9">
         <v>43252</v>
@@ -7875,34 +7948,36 @@
       <c r="K61" s="9">
         <v>43617</v>
       </c>
-      <c r="L61" s="9"/>
+      <c r="L61" s="9">
+        <v>43617</v>
+      </c>
       <c r="M61" s="6">
         <v>12</v>
       </c>
       <c r="N61" s="11" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="O61" s="11" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="P61" s="26"/>
       <c r="Q61" s="12" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="R61" s="11" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="S61" s="11" t="s">
         <v>46</v>
       </c>
       <c r="T61" s="11" t="s">
+        <v>411</v>
+      </c>
+      <c r="U61" s="15" t="s">
         <v>412</v>
       </c>
-      <c r="U61" s="15" t="s">
+      <c r="V61" s="14" t="s">
         <v>413</v>
-      </c>
-      <c r="V61" s="14" t="s">
-        <v>414</v>
       </c>
       <c r="W61" s="6"/>
       <c r="X61" s="6"/>
@@ -7928,7 +8003,7 @@
       <c r="AJ61" s="6"/>
       <c r="AK61" s="13">
         <f ca="1">NOW()</f>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL61" s="14" t="s">
         <v>335</v>
@@ -7936,13 +8011,13 @@
     </row>
     <row r="62" spans="1:38" ht="56" x14ac:dyDescent="0.15">
       <c r="A62" s="11" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B62" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C62" s="15" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D62" s="6" t="s">
         <v>40</v>
@@ -7960,7 +8035,7 @@
         <v>43496</v>
       </c>
       <c r="I62" s="14" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="J62" s="9">
         <v>43496</v>
@@ -7973,29 +8048,29 @@
         <v>12</v>
       </c>
       <c r="N62" s="11" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="O62" s="11" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="P62" s="26"/>
       <c r="Q62" s="12" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="R62" s="11" t="s">
+        <v>418</v>
+      </c>
+      <c r="S62" s="11" t="s">
         <v>419</v>
       </c>
-      <c r="S62" s="11" t="s">
+      <c r="T62" s="11" t="s">
         <v>420</v>
       </c>
-      <c r="T62" s="11" t="s">
-        <v>421</v>
-      </c>
       <c r="U62" s="15" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="V62" s="14" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="W62" s="6"/>
       <c r="X62" s="6"/>
@@ -8021,7 +8096,7 @@
       <c r="AJ62" s="6"/>
       <c r="AK62" s="13">
         <f ca="1">NOW()</f>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL62" s="14" t="s">
         <v>335</v>
@@ -8029,13 +8104,13 @@
     </row>
     <row r="63" spans="1:38" ht="56" x14ac:dyDescent="0.15">
       <c r="A63" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B63" s="11" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C63" s="15" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D63" s="6" t="s">
         <v>40</v>
@@ -8053,7 +8128,7 @@
         <v>43497</v>
       </c>
       <c r="I63" s="14" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="J63" s="9">
         <v>43497</v>
@@ -8066,29 +8141,29 @@
         <v>12</v>
       </c>
       <c r="N63" s="11" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="O63" s="11" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="P63" s="26"/>
       <c r="Q63" s="12" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="R63" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="S63" s="11" t="s">
         <v>46</v>
       </c>
       <c r="T63" s="11" t="s">
+        <v>431</v>
+      </c>
+      <c r="U63" s="15" t="s">
         <v>432</v>
       </c>
-      <c r="U63" s="15" t="s">
-        <v>433</v>
-      </c>
       <c r="V63" s="14" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="W63" s="6"/>
       <c r="X63" s="6"/>
@@ -8114,7 +8189,7 @@
       <c r="AJ63" s="6"/>
       <c r="AK63" s="13">
         <f ca="1">NOW()</f>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL63" s="14" t="s">
         <v>335</v>
@@ -8122,13 +8197,13 @@
     </row>
     <row r="64" spans="1:38" ht="28" x14ac:dyDescent="0.15">
       <c r="A64" s="6" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C64" s="28" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D64" s="6" t="s">
         <v>40</v>
@@ -8146,7 +8221,7 @@
         <v>43542</v>
       </c>
       <c r="I64" s="14" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="J64" s="9">
         <v>43542</v>
@@ -8159,31 +8234,31 @@
         <v>12</v>
       </c>
       <c r="N64" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="O64" s="6" t="s">
         <v>447</v>
       </c>
-      <c r="O64" s="6" t="s">
+      <c r="P64" s="26" t="s">
         <v>448</v>
       </c>
-      <c r="P64" s="26" t="s">
+      <c r="Q64" s="8" t="s">
         <v>449</v>
       </c>
-      <c r="Q64" s="8" t="s">
+      <c r="R64" s="6" t="s">
         <v>450</v>
-      </c>
-      <c r="R64" s="6" t="s">
-        <v>451</v>
       </c>
       <c r="S64" s="6" t="s">
         <v>46</v>
       </c>
       <c r="T64" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="U64" s="7" t="s">
         <v>452</v>
       </c>
-      <c r="U64" s="7" t="s">
-        <v>453</v>
-      </c>
       <c r="V64" s="14" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="W64" s="6"/>
       <c r="X64" s="6"/>
@@ -8208,8 +8283,8 @@
       </c>
       <c r="AJ64" s="6"/>
       <c r="AK64" s="13">
-        <f t="shared" ref="AK64:AK68" ca="1" si="1">NOW()</f>
-        <v>43707.550085763891</v>
+        <f t="shared" ref="AK64:AK70" ca="1" si="1">NOW()</f>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL64" s="14" t="s">
         <v>335</v>
@@ -8217,13 +8292,13 @@
     </row>
     <row r="65" spans="1:38" ht="84" x14ac:dyDescent="0.15">
       <c r="A65" s="6" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B65" s="11" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C65" s="15" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D65" s="6" t="s">
         <v>40</v>
@@ -8241,7 +8316,7 @@
         <v>43543</v>
       </c>
       <c r="I65" s="14" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="J65" s="9">
         <v>43543</v>
@@ -8254,31 +8329,31 @@
         <v>12</v>
       </c>
       <c r="N65" s="11" t="s">
+        <v>456</v>
+      </c>
+      <c r="O65" s="11" t="s">
+        <v>437</v>
+      </c>
+      <c r="P65" s="29" t="s">
         <v>457</v>
       </c>
-      <c r="O65" s="11" t="s">
-        <v>438</v>
-      </c>
-      <c r="P65" s="29" t="s">
+      <c r="Q65" s="12" t="s">
         <v>458</v>
       </c>
-      <c r="Q65" s="12" t="s">
-        <v>459</v>
-      </c>
       <c r="R65" s="11" t="s">
+        <v>461</v>
+      </c>
+      <c r="S65" s="11" t="s">
         <v>462</v>
       </c>
-      <c r="S65" s="11" t="s">
+      <c r="T65" s="11" t="s">
         <v>463</v>
       </c>
-      <c r="T65" s="11" t="s">
-        <v>464</v>
-      </c>
       <c r="U65" s="15" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="V65" s="14" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="W65" s="6"/>
       <c r="X65" s="6"/>
@@ -8304,7 +8379,7 @@
       <c r="AJ65" s="6"/>
       <c r="AK65" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL65" s="14" t="s">
         <v>335</v>
@@ -8312,13 +8387,13 @@
     </row>
     <row r="66" spans="1:38" ht="56" x14ac:dyDescent="0.15">
       <c r="A66" s="6" t="s">
+        <v>440</v>
+      </c>
+      <c r="B66" s="6" t="s">
         <v>441</v>
       </c>
-      <c r="B66" s="6" t="s">
-        <v>442</v>
-      </c>
       <c r="C66" s="6" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D66" s="6" t="s">
         <v>40</v>
@@ -8336,7 +8411,7 @@
         <v>43607</v>
       </c>
       <c r="I66" s="14" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="J66" s="9">
         <v>43607</v>
@@ -8349,16 +8424,16 @@
         <v>12</v>
       </c>
       <c r="N66" s="6" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="O66" s="11" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="P66" s="25" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="Q66" s="8" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="R66" s="6" t="s">
         <v>317</v>
@@ -8370,10 +8445,10 @@
         <v>318</v>
       </c>
       <c r="U66" s="7" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="V66" s="30" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="W66" s="6"/>
       <c r="X66" s="6"/>
@@ -8399,7 +8474,7 @@
       <c r="AJ66" s="6"/>
       <c r="AK66" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL66" s="14" t="s">
         <v>335</v>
@@ -8407,13 +8482,13 @@
     </row>
     <row r="67" spans="1:38" ht="28" x14ac:dyDescent="0.15">
       <c r="A67" s="6" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B67" s="11" t="s">
         <v>329</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D67" s="6" t="s">
         <v>40</v>
@@ -8494,7 +8569,7 @@
       <c r="AJ67" s="6"/>
       <c r="AK67" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL67" s="14" t="s">
         <v>335</v>
@@ -8502,13 +8577,13 @@
     </row>
     <row r="68" spans="1:38" ht="42" x14ac:dyDescent="0.15">
       <c r="A68" s="6" t="s">
+        <v>466</v>
+      </c>
+      <c r="B68" s="6" t="s">
         <v>467</v>
       </c>
-      <c r="B68" s="6" t="s">
+      <c r="C68" s="7" t="s">
         <v>468</v>
-      </c>
-      <c r="C68" s="7" t="s">
-        <v>469</v>
       </c>
       <c r="D68" s="6" t="s">
         <v>100</v>
@@ -8587,91 +8662,198 @@
       <c r="AJ68" s="6"/>
       <c r="AK68" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>43707.550085763891</v>
+        <v>43753.663857175925</v>
       </c>
       <c r="AL68" s="14" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="69" spans="1:38" ht="14" x14ac:dyDescent="0.15">
-      <c r="A69" s="6"/>
-      <c r="B69" s="6"/>
-      <c r="C69" s="6"/>
-      <c r="D69" s="6"/>
-      <c r="E69" s="8"/>
-      <c r="F69" s="8"/>
-      <c r="G69" s="6"/>
-      <c r="H69" s="9"/>
-      <c r="I69" s="6"/>
-      <c r="J69" s="9"/>
-      <c r="K69" s="9"/>
+    <row r="69" spans="1:38" ht="42" x14ac:dyDescent="0.15">
+      <c r="A69" s="6" t="s">
+        <v>470</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>489</v>
+      </c>
+      <c r="C69" s="15" t="s">
+        <v>481</v>
+      </c>
+      <c r="D69" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E69" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="F69" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="G69" s="6">
+        <v>10000</v>
+      </c>
+      <c r="H69" s="9">
+        <v>43709</v>
+      </c>
+      <c r="I69" s="14" t="s">
+        <v>480</v>
+      </c>
+      <c r="J69" s="9">
+        <v>43709</v>
+      </c>
+      <c r="K69" s="9">
+        <v>44075</v>
+      </c>
       <c r="L69" s="9"/>
-      <c r="M69" s="6"/>
-      <c r="N69" s="6"/>
-      <c r="O69" s="6"/>
-      <c r="P69" s="26"/>
-      <c r="Q69" s="8"/>
-      <c r="R69" s="6"/>
-      <c r="S69" s="6"/>
-      <c r="T69" s="6"/>
-      <c r="U69" s="7"/>
-      <c r="V69" s="6"/>
+      <c r="M69" s="6">
+        <v>12</v>
+      </c>
+      <c r="N69" s="11" t="s">
+        <v>483</v>
+      </c>
+      <c r="O69" s="11" t="s">
+        <v>484</v>
+      </c>
+      <c r="P69" s="29" t="s">
+        <v>482</v>
+      </c>
+      <c r="R69" s="12" t="s">
+        <v>485</v>
+      </c>
+      <c r="S69" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="T69" s="11" t="s">
+        <v>486</v>
+      </c>
+      <c r="U69" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="V69" s="14" t="s">
+        <v>488</v>
+      </c>
       <c r="W69" s="6"/>
       <c r="X69" s="6"/>
       <c r="Y69" s="6"/>
       <c r="Z69" s="6"/>
       <c r="AA69" s="6"/>
       <c r="AB69" s="6"/>
-      <c r="AC69" s="6"/>
-      <c r="AD69" s="6"/>
+      <c r="AC69" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD69" s="6" t="s">
+        <v>50</v>
+      </c>
       <c r="AE69" s="6"/>
       <c r="AF69" s="6"/>
-      <c r="AG69" s="6"/>
+      <c r="AG69" s="6" t="s">
+        <v>50</v>
+      </c>
       <c r="AH69" s="6"/>
-      <c r="AI69" s="6"/>
+      <c r="AI69" s="19" t="s">
+        <v>51</v>
+      </c>
       <c r="AJ69" s="6"/>
-      <c r="AK69" s="13"/>
-      <c r="AL69" s="6"/>
+      <c r="AK69" s="13">
+        <f t="shared" ca="1" si="1"/>
+        <v>43753.663857175925</v>
+      </c>
+      <c r="AL69" s="14" t="s">
+        <v>335</v>
+      </c>
     </row>
-    <row r="70" spans="1:38" ht="14" x14ac:dyDescent="0.15">
-      <c r="A70" s="6"/>
-      <c r="B70" s="6"/>
-      <c r="C70" s="6"/>
-      <c r="D70" s="6"/>
-      <c r="E70" s="8"/>
-      <c r="F70" s="8"/>
-      <c r="G70" s="6"/>
-      <c r="H70" s="9"/>
-      <c r="I70" s="6"/>
-      <c r="J70" s="9"/>
-      <c r="K70" s="9"/>
+    <row r="70" spans="1:38" ht="56" x14ac:dyDescent="0.15">
+      <c r="A70" s="6" t="s">
+        <v>471</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>469</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>472</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E70" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="F70" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="G70" s="6">
+        <v>30000</v>
+      </c>
+      <c r="H70" s="9">
+        <v>43709</v>
+      </c>
+      <c r="I70" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="J70" s="9">
+        <v>43709</v>
+      </c>
+      <c r="K70" s="9">
+        <v>44075</v>
+      </c>
       <c r="L70" s="9"/>
-      <c r="M70" s="6"/>
-      <c r="N70" s="6"/>
-      <c r="O70" s="6"/>
-      <c r="P70" s="26"/>
-      <c r="Q70" s="8"/>
-      <c r="R70" s="6"/>
-      <c r="S70" s="6"/>
-      <c r="T70" s="6"/>
-      <c r="U70" s="7"/>
-      <c r="V70" s="6"/>
+      <c r="M70" s="6">
+        <v>12</v>
+      </c>
+      <c r="N70" s="11" t="s">
+        <v>475</v>
+      </c>
+      <c r="O70" s="11" t="s">
+        <v>476</v>
+      </c>
+      <c r="P70" s="32" t="s">
+        <v>474</v>
+      </c>
+      <c r="Q70" s="12" t="s">
+        <v>477</v>
+      </c>
+      <c r="R70" s="11" t="s">
+        <v>479</v>
+      </c>
+      <c r="S70" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="T70" s="11" t="s">
+        <v>478</v>
+      </c>
+      <c r="U70" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="V70" s="14" t="s">
+        <v>316</v>
+      </c>
       <c r="W70" s="6"/>
       <c r="X70" s="6"/>
       <c r="Y70" s="6"/>
       <c r="Z70" s="6"/>
       <c r="AA70" s="6"/>
       <c r="AB70" s="6"/>
-      <c r="AC70" s="6"/>
-      <c r="AD70" s="6"/>
+      <c r="AC70" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD70" s="6" t="s">
+        <v>50</v>
+      </c>
       <c r="AE70" s="6"/>
       <c r="AF70" s="6"/>
-      <c r="AG70" s="6"/>
+      <c r="AG70" s="6" t="s">
+        <v>50</v>
+      </c>
       <c r="AH70" s="6"/>
-      <c r="AI70" s="6"/>
+      <c r="AI70" s="19" t="s">
+        <v>51</v>
+      </c>
       <c r="AJ70" s="6"/>
-      <c r="AK70" s="13"/>
-      <c r="AL70" s="6"/>
+      <c r="AK70" s="13">
+        <f t="shared" ca="1" si="1"/>
+        <v>43753.663857175925</v>
+      </c>
+      <c r="AL70" s="14" t="s">
+        <v>335</v>
+      </c>
     </row>
     <row r="71" spans="1:38" ht="14" x14ac:dyDescent="0.15">
       <c r="A71" s="6"/>
@@ -8801,6 +8983,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:AL60" xr:uid="{AE487DEF-5BC5-C74D-81B1-9FC54E50B3DD}"/>
+  <phoneticPr fontId="12" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="AL2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="I4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
@@ -8887,8 +9070,14 @@
     <hyperlink ref="AL68" r:id="rId83" xr:uid="{A901E03A-725E-C741-94C8-61B9D2FAE211}"/>
     <hyperlink ref="I68" r:id="rId84" xr:uid="{31305DFC-424C-BE4B-A96E-5BFCDE782066}"/>
     <hyperlink ref="V68" r:id="rId85" xr:uid="{C302D653-12FD-9348-8F28-ACBBFD2EF9F1}"/>
+    <hyperlink ref="I70" r:id="rId86" xr:uid="{F95C4425-40C1-D54E-97D9-DC400BCA326C}"/>
+    <hyperlink ref="V70" r:id="rId87" xr:uid="{05AE4D1C-6B5F-CD45-85D1-D2FE8753C986}"/>
+    <hyperlink ref="AL69" r:id="rId88" xr:uid="{E07D8CF3-886E-A64A-B9CC-C7C1CB712E97}"/>
+    <hyperlink ref="AL70" r:id="rId89" xr:uid="{C3A29FC7-45A2-BD49-9F66-F3362975B416}"/>
+    <hyperlink ref="I69" r:id="rId90" xr:uid="{A9F19546-10EA-864C-A6F1-A65365EE36C4}"/>
+    <hyperlink ref="V69" r:id="rId91" xr:uid="{3F9D190E-30DD-A149-B311-DD2FE463FED7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId86"/>
+  <legacyDrawing r:id="rId92"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update sitemap and grants data
</commit_message>
<xml_diff>
--- a/open/grants.xlsx
+++ b/open/grants.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/westsi/Documents/GitHub/zing/open/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C6DBEE-EE56-104B-B563-23B7412E4694}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F630A17-6298-1045-B6E2-DC0A8F209CDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1461" uniqueCount="490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1481" uniqueCount="502">
   <si>
     <t>Identifier</t>
   </si>
@@ -1535,6 +1535,42 @@
   </si>
   <si>
     <t>Core funding toward the start of the Young Trustee Movement</t>
+  </si>
+  <si>
+    <t>360G-zing-72</t>
+  </si>
+  <si>
+    <t>Core funding for staff, to replicate the Really NEET model in London</t>
+  </si>
+  <si>
+    <t>The Really NEET Project was founded to meet the unique needs of NEET young people (aged 16-24) to learn in a supportive and specially tailored environment. Their projects are about much more than simply getting a job or passing a course; they hope to empower positive change in young people by giving them the tools to create stability and security in their lives that will enable them to achieve their future goals and become contributing members of wider society. They are an Award-winning South Yorkshire based Social Enterprise working with some of society’s most vulnerable young people. Their founder, Sophie Maxwell, set up the project due to her own life experiences (dropping out of school, domestic violence and homelessness) leading to her wanting to set up a college for young people who had been through similar circumstances to her, ensuring they had the right kind of support in place at such a crucial age, enabling them to achieve their dreams despite their challenges. Their 37 week "Inspiring Change" programme supports disadvantaged youth through: Maths and English, highly practical vocational qualifications, Personal Social Development sessions, employability sessions, home-pickups, enrichment activities, a leadership residential, and quality onsite youth work.</t>
+  </si>
+  <si>
+    <t>https://reallyneet.co.uk/</t>
+  </si>
+  <si>
+    <t>Core funding to cover staff costs, supporting the development of a project in London, which will replicate and adapt the Really NEET model outside of South Yorkshire.</t>
+  </si>
+  <si>
+    <t>36000</t>
+  </si>
+  <si>
+    <t>07583111</t>
+  </si>
+  <si>
+    <t>The Really NEET Project</t>
+  </si>
+  <si>
+    <t>GB-COH-07583111</t>
+  </si>
+  <si>
+    <t>Unit One, Chemist Lane</t>
+  </si>
+  <si>
+    <t>Rotherham</t>
+  </si>
+  <si>
+    <t>S60 1NA</t>
   </si>
 </sst>
 </file>
@@ -2064,13 +2100,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AL75"/>
+  <dimension ref="A1:AL74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C65" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B72" sqref="B72"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2322,8 +2358,8 @@
       </c>
       <c r="AJ2" s="6"/>
       <c r="AK2" s="13">
-        <f t="shared" ref="AK2:AK60" ca="1" si="0">NOW()</f>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL2" s="14" t="s">
         <v>335</v>
@@ -2419,8 +2455,8 @@
       </c>
       <c r="AJ3" s="6"/>
       <c r="AK3" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL3" s="14" t="s">
         <v>335</v>
@@ -2516,8 +2552,8 @@
       </c>
       <c r="AJ4" s="6"/>
       <c r="AK4" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL4" s="14" t="s">
         <v>335</v>
@@ -2613,8 +2649,8 @@
       </c>
       <c r="AJ5" s="6"/>
       <c r="AK5" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL5" s="14" t="s">
         <v>335</v>
@@ -2710,8 +2746,8 @@
       </c>
       <c r="AJ6" s="6"/>
       <c r="AK6" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL6" s="14" t="s">
         <v>335</v>
@@ -2807,8 +2843,8 @@
       </c>
       <c r="AJ7" s="6"/>
       <c r="AK7" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL7" s="14" t="s">
         <v>335</v>
@@ -2904,8 +2940,8 @@
       </c>
       <c r="AJ8" s="6"/>
       <c r="AK8" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL8" s="14" t="s">
         <v>335</v>
@@ -2999,8 +3035,8 @@
       </c>
       <c r="AJ9" s="6"/>
       <c r="AK9" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL9" s="14" t="s">
         <v>335</v>
@@ -3096,8 +3132,8 @@
       </c>
       <c r="AJ10" s="6"/>
       <c r="AK10" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL10" s="14" t="s">
         <v>335</v>
@@ -3191,8 +3227,8 @@
       </c>
       <c r="AJ11" s="6"/>
       <c r="AK11" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL11" s="14" t="s">
         <v>335</v>
@@ -3288,8 +3324,8 @@
       </c>
       <c r="AJ12" s="6"/>
       <c r="AK12" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL12" s="14" t="s">
         <v>335</v>
@@ -3383,8 +3419,8 @@
       </c>
       <c r="AJ13" s="6"/>
       <c r="AK13" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL13" s="14" t="s">
         <v>335</v>
@@ -3480,8 +3516,8 @@
       </c>
       <c r="AJ14" s="6"/>
       <c r="AK14" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL14" s="14" t="s">
         <v>335</v>
@@ -3575,8 +3611,8 @@
       </c>
       <c r="AJ15" s="6"/>
       <c r="AK15" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL15" s="14" t="s">
         <v>335</v>
@@ -3670,8 +3706,8 @@
       </c>
       <c r="AJ16" s="6"/>
       <c r="AK16" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL16" s="14" t="s">
         <v>335</v>
@@ -3767,8 +3803,8 @@
       </c>
       <c r="AJ17" s="6"/>
       <c r="AK17" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL17" s="14" t="s">
         <v>335</v>
@@ -3864,8 +3900,8 @@
       </c>
       <c r="AJ18" s="6"/>
       <c r="AK18" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL18" s="14" t="s">
         <v>335</v>
@@ -3959,8 +3995,8 @@
       </c>
       <c r="AJ19" s="6"/>
       <c r="AK19" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL19" s="14" t="s">
         <v>335</v>
@@ -4054,8 +4090,8 @@
       </c>
       <c r="AJ20" s="6"/>
       <c r="AK20" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL20" s="14" t="s">
         <v>335</v>
@@ -4151,8 +4187,8 @@
       </c>
       <c r="AJ21" s="6"/>
       <c r="AK21" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL21" s="14" t="s">
         <v>335</v>
@@ -4246,8 +4282,8 @@
       </c>
       <c r="AJ22" s="6"/>
       <c r="AK22" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL22" s="14" t="s">
         <v>335</v>
@@ -4343,8 +4379,8 @@
       </c>
       <c r="AJ23" s="6"/>
       <c r="AK23" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL23" s="14" t="s">
         <v>335</v>
@@ -4440,8 +4476,8 @@
       </c>
       <c r="AJ24" s="6"/>
       <c r="AK24" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL24" s="14" t="s">
         <v>335</v>
@@ -4535,8 +4571,8 @@
       </c>
       <c r="AJ25" s="6"/>
       <c r="AK25" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL25" s="14" t="s">
         <v>335</v>
@@ -4632,8 +4668,8 @@
       </c>
       <c r="AJ26" s="6"/>
       <c r="AK26" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL26" s="14" t="s">
         <v>335</v>
@@ -4729,8 +4765,8 @@
       </c>
       <c r="AJ27" s="6"/>
       <c r="AK27" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL27" s="14" t="s">
         <v>335</v>
@@ -4824,8 +4860,8 @@
       </c>
       <c r="AJ28" s="6"/>
       <c r="AK28" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL28" s="14" t="s">
         <v>335</v>
@@ -4921,8 +4957,8 @@
       </c>
       <c r="AJ29" s="6"/>
       <c r="AK29" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL29" s="14" t="s">
         <v>335</v>
@@ -5016,8 +5052,8 @@
       </c>
       <c r="AJ30" s="6"/>
       <c r="AK30" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL30" s="14" t="s">
         <v>335</v>
@@ -5113,8 +5149,8 @@
       </c>
       <c r="AJ31" s="6"/>
       <c r="AK31" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL31" s="14" t="s">
         <v>335</v>
@@ -5210,8 +5246,8 @@
       </c>
       <c r="AJ32" s="6"/>
       <c r="AK32" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL32" s="14" t="s">
         <v>335</v>
@@ -5307,8 +5343,8 @@
       </c>
       <c r="AJ33" s="6"/>
       <c r="AK33" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL33" s="14" t="s">
         <v>335</v>
@@ -5404,8 +5440,8 @@
       </c>
       <c r="AJ34" s="6"/>
       <c r="AK34" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL34" s="14" t="s">
         <v>335</v>
@@ -5499,8 +5535,8 @@
       </c>
       <c r="AJ35" s="6"/>
       <c r="AK35" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL35" s="14" t="s">
         <v>335</v>
@@ -5596,8 +5632,8 @@
       </c>
       <c r="AJ36" s="6"/>
       <c r="AK36" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL36" s="14" t="s">
         <v>335</v>
@@ -5691,8 +5727,8 @@
       </c>
       <c r="AJ37" s="6"/>
       <c r="AK37" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL37" s="14" t="s">
         <v>335</v>
@@ -5788,8 +5824,8 @@
       </c>
       <c r="AJ38" s="6"/>
       <c r="AK38" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL38" s="14" t="s">
         <v>335</v>
@@ -5885,8 +5921,8 @@
       </c>
       <c r="AJ39" s="6"/>
       <c r="AK39" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL39" s="14" t="s">
         <v>335</v>
@@ -5982,8 +6018,8 @@
       </c>
       <c r="AJ40" s="6"/>
       <c r="AK40" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL40" s="14" t="s">
         <v>335</v>
@@ -6079,8 +6115,8 @@
       </c>
       <c r="AJ41" s="6"/>
       <c r="AK41" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL41" s="14" t="s">
         <v>335</v>
@@ -6176,8 +6212,8 @@
       </c>
       <c r="AJ42" s="6"/>
       <c r="AK42" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL42" s="14" t="s">
         <v>335</v>
@@ -6273,8 +6309,8 @@
       </c>
       <c r="AJ43" s="6"/>
       <c r="AK43" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL43" s="14" t="s">
         <v>335</v>
@@ -6368,8 +6404,8 @@
       </c>
       <c r="AJ44" s="6"/>
       <c r="AK44" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL44" s="14" t="s">
         <v>335</v>
@@ -6465,8 +6501,8 @@
       </c>
       <c r="AJ45" s="6"/>
       <c r="AK45" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL45" s="14" t="s">
         <v>335</v>
@@ -6560,8 +6596,8 @@
       </c>
       <c r="AJ46" s="6"/>
       <c r="AK46" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL46" s="14" t="s">
         <v>335</v>
@@ -6657,8 +6693,8 @@
       </c>
       <c r="AJ47" s="6"/>
       <c r="AK47" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL47" s="14" t="s">
         <v>335</v>
@@ -6752,8 +6788,8 @@
       </c>
       <c r="AJ48" s="6"/>
       <c r="AK48" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL48" s="14" t="s">
         <v>335</v>
@@ -6849,8 +6885,8 @@
       </c>
       <c r="AJ49" s="6"/>
       <c r="AK49" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL49" s="14" t="s">
         <v>335</v>
@@ -6946,8 +6982,8 @@
       </c>
       <c r="AJ50" s="6"/>
       <c r="AK50" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL50" s="14" t="s">
         <v>335</v>
@@ -7041,8 +7077,8 @@
       </c>
       <c r="AJ51" s="6"/>
       <c r="AK51" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL51" s="14" t="s">
         <v>335</v>
@@ -7138,8 +7174,8 @@
       </c>
       <c r="AJ52" s="6"/>
       <c r="AK52" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL52" s="14" t="s">
         <v>335</v>
@@ -7235,8 +7271,8 @@
       </c>
       <c r="AJ53" s="6"/>
       <c r="AK53" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL53" s="14" t="s">
         <v>335</v>
@@ -7329,8 +7365,8 @@
         <v>51</v>
       </c>
       <c r="AK54" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL54" s="14" t="s">
         <v>335</v>
@@ -7425,7 +7461,7 @@
       <c r="AJ55" s="24"/>
       <c r="AK55" s="24">
         <f ca="1">NOW()</f>
-        <v>43753.663857175925</v>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL55" s="14" t="s">
         <v>335</v>
@@ -7521,8 +7557,8 @@
       </c>
       <c r="AJ56" s="24"/>
       <c r="AK56" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL56" s="14" t="s">
         <v>335</v>
@@ -7618,8 +7654,8 @@
       </c>
       <c r="AJ57" s="6"/>
       <c r="AK57" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL57" s="14" t="s">
         <v>335</v>
@@ -7713,8 +7749,8 @@
       </c>
       <c r="AJ58" s="6"/>
       <c r="AK58" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL58" s="14" t="s">
         <v>335</v>
@@ -7810,8 +7846,8 @@
       </c>
       <c r="AJ59" s="6"/>
       <c r="AK59" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL59" s="14" t="s">
         <v>335</v>
@@ -7907,8 +7943,8 @@
       </c>
       <c r="AJ60" s="6"/>
       <c r="AK60" s="13">
-        <f t="shared" ca="1" si="0"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL60" s="14" t="s">
         <v>335</v>
@@ -8003,7 +8039,7 @@
       <c r="AJ61" s="6"/>
       <c r="AK61" s="13">
         <f ca="1">NOW()</f>
-        <v>43753.663857175925</v>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL61" s="14" t="s">
         <v>335</v>
@@ -8096,7 +8132,7 @@
       <c r="AJ62" s="6"/>
       <c r="AK62" s="13">
         <f ca="1">NOW()</f>
-        <v>43753.663857175925</v>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL62" s="14" t="s">
         <v>335</v>
@@ -8189,7 +8225,7 @@
       <c r="AJ63" s="6"/>
       <c r="AK63" s="13">
         <f ca="1">NOW()</f>
-        <v>43753.663857175925</v>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL63" s="14" t="s">
         <v>335</v>
@@ -8283,8 +8319,8 @@
       </c>
       <c r="AJ64" s="6"/>
       <c r="AK64" s="13">
-        <f t="shared" ref="AK64:AK70" ca="1" si="1">NOW()</f>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL64" s="14" t="s">
         <v>335</v>
@@ -8378,8 +8414,8 @@
       </c>
       <c r="AJ65" s="6"/>
       <c r="AK65" s="13">
-        <f t="shared" ca="1" si="1"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL65" s="14" t="s">
         <v>335</v>
@@ -8473,8 +8509,8 @@
       </c>
       <c r="AJ66" s="6"/>
       <c r="AK66" s="13">
-        <f t="shared" ca="1" si="1"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL66" s="14" t="s">
         <v>335</v>
@@ -8568,8 +8604,8 @@
       </c>
       <c r="AJ67" s="6"/>
       <c r="AK67" s="13">
-        <f t="shared" ca="1" si="1"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL67" s="14" t="s">
         <v>335</v>
@@ -8661,8 +8697,8 @@
       </c>
       <c r="AJ68" s="6"/>
       <c r="AK68" s="13">
-        <f t="shared" ca="1" si="1"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL68" s="14" t="s">
         <v>335</v>
@@ -8753,8 +8789,8 @@
       </c>
       <c r="AJ69" s="6"/>
       <c r="AK69" s="13">
-        <f t="shared" ca="1" si="1"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL69" s="14" t="s">
         <v>335</v>
@@ -8848,52 +8884,105 @@
       </c>
       <c r="AJ70" s="6"/>
       <c r="AK70" s="13">
-        <f t="shared" ca="1" si="1"/>
-        <v>43753.663857175925</v>
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
       </c>
       <c r="AL70" s="14" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="71" spans="1:38" ht="14" x14ac:dyDescent="0.15">
-      <c r="A71" s="6"/>
-      <c r="B71" s="6"/>
-      <c r="C71" s="6"/>
-      <c r="D71" s="6"/>
-      <c r="E71" s="8"/>
-      <c r="F71" s="8"/>
-      <c r="G71" s="6"/>
-      <c r="H71" s="9"/>
-      <c r="I71" s="6"/>
-      <c r="J71" s="9"/>
-      <c r="K71" s="9"/>
+    <row r="71" spans="1:38" ht="126" x14ac:dyDescent="0.15">
+      <c r="A71" s="6" t="s">
+        <v>490</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>491</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>494</v>
+      </c>
+      <c r="D71" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E71" s="8" t="s">
+        <v>495</v>
+      </c>
+      <c r="F71" s="8" t="s">
+        <v>495</v>
+      </c>
+      <c r="G71" s="6">
+        <v>36000</v>
+      </c>
+      <c r="H71" s="9">
+        <v>43800</v>
+      </c>
+      <c r="I71" s="14" t="s">
+        <v>493</v>
+      </c>
+      <c r="J71" s="9">
+        <v>43800</v>
+      </c>
+      <c r="K71" s="9">
+        <v>44166</v>
+      </c>
       <c r="L71" s="9"/>
-      <c r="M71" s="6"/>
-      <c r="N71" s="6"/>
-      <c r="O71" s="6"/>
+      <c r="M71" s="6">
+        <v>12</v>
+      </c>
+      <c r="N71" s="6" t="s">
+        <v>498</v>
+      </c>
+      <c r="O71" s="6" t="s">
+        <v>497</v>
+      </c>
       <c r="P71" s="26"/>
-      <c r="Q71" s="8"/>
-      <c r="R71" s="6"/>
-      <c r="S71" s="6"/>
-      <c r="T71" s="6"/>
-      <c r="U71" s="7"/>
-      <c r="V71" s="6"/>
+      <c r="Q71" s="8" t="s">
+        <v>496</v>
+      </c>
+      <c r="R71" s="6" t="s">
+        <v>499</v>
+      </c>
+      <c r="S71" s="6" t="s">
+        <v>500</v>
+      </c>
+      <c r="T71" s="6" t="s">
+        <v>501</v>
+      </c>
+      <c r="U71" s="7" t="s">
+        <v>492</v>
+      </c>
+      <c r="V71" s="14" t="s">
+        <v>493</v>
+      </c>
       <c r="W71" s="6"/>
       <c r="X71" s="6"/>
       <c r="Y71" s="6"/>
       <c r="Z71" s="6"/>
       <c r="AA71" s="6"/>
       <c r="AB71" s="6"/>
-      <c r="AC71" s="6"/>
-      <c r="AD71" s="6"/>
+      <c r="AC71" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD71" s="6" t="s">
+        <v>50</v>
+      </c>
       <c r="AE71" s="6"/>
       <c r="AF71" s="6"/>
-      <c r="AG71" s="6"/>
+      <c r="AG71" s="6" t="s">
+        <v>50</v>
+      </c>
       <c r="AH71" s="6"/>
-      <c r="AI71" s="6"/>
+      <c r="AI71" s="6" t="s">
+        <v>51</v>
+      </c>
       <c r="AJ71" s="6"/>
-      <c r="AK71" s="13"/>
-      <c r="AL71" s="6"/>
+      <c r="AK71" s="13">
+        <f ca="1">NOW()</f>
+        <v>43816.726411574076</v>
+      </c>
+      <c r="AL71" s="14" t="s">
+        <v>335</v>
+      </c>
     </row>
     <row r="72" spans="1:38" ht="14" x14ac:dyDescent="0.15">
       <c r="A72" s="6"/>
@@ -8935,51 +9024,11 @@
       <c r="AK72" s="13"/>
       <c r="AL72" s="6"/>
     </row>
-    <row r="73" spans="1:38" ht="14" x14ac:dyDescent="0.15">
-      <c r="A73" s="6"/>
-      <c r="B73" s="6"/>
-      <c r="C73" s="6"/>
-      <c r="D73" s="6"/>
-      <c r="E73" s="8"/>
-      <c r="F73" s="8"/>
-      <c r="G73" s="6"/>
-      <c r="H73" s="9"/>
-      <c r="I73" s="6"/>
-      <c r="J73" s="9"/>
-      <c r="K73" s="9"/>
-      <c r="L73" s="9"/>
-      <c r="M73" s="6"/>
-      <c r="N73" s="6"/>
-      <c r="O73" s="6"/>
-      <c r="P73" s="26"/>
-      <c r="Q73" s="8"/>
-      <c r="R73" s="6"/>
-      <c r="S73" s="6"/>
-      <c r="T73" s="6"/>
-      <c r="U73" s="7"/>
-      <c r="V73" s="6"/>
-      <c r="W73" s="6"/>
-      <c r="X73" s="6"/>
-      <c r="Y73" s="6"/>
-      <c r="Z73" s="6"/>
-      <c r="AA73" s="6"/>
-      <c r="AB73" s="6"/>
-      <c r="AC73" s="6"/>
-      <c r="AD73" s="6"/>
-      <c r="AE73" s="6"/>
-      <c r="AF73" s="6"/>
-      <c r="AG73" s="6"/>
-      <c r="AH73" s="6"/>
-      <c r="AI73" s="6"/>
-      <c r="AJ73" s="6"/>
-      <c r="AK73" s="13"/>
-      <c r="AL73" s="6"/>
+    <row r="73" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="P73" s="31"/>
     </row>
     <row r="74" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="P74" s="31"/>
-    </row>
-    <row r="75" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="P75" s="31"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AL60" xr:uid="{AE487DEF-5BC5-C74D-81B1-9FC54E50B3DD}"/>
@@ -9076,8 +9125,11 @@
     <hyperlink ref="AL70" r:id="rId89" xr:uid="{C3A29FC7-45A2-BD49-9F66-F3362975B416}"/>
     <hyperlink ref="I69" r:id="rId90" xr:uid="{A9F19546-10EA-864C-A6F1-A65365EE36C4}"/>
     <hyperlink ref="V69" r:id="rId91" xr:uid="{3F9D190E-30DD-A149-B311-DD2FE463FED7}"/>
+    <hyperlink ref="V71" r:id="rId92" xr:uid="{E71ED7BD-E5E9-ED45-9956-D79CB4FB1410}"/>
+    <hyperlink ref="I71" r:id="rId93" xr:uid="{491B3049-EF60-354B-AC90-AA0512B6FB72}"/>
+    <hyperlink ref="AL71" r:id="rId94" xr:uid="{37973771-8508-B24C-8A43-D902FF3DE69F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId92"/>
+  <legacyDrawing r:id="rId95"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update grants and add COVID-19 statement
</commit_message>
<xml_diff>
--- a/open/grants.xlsx
+++ b/open/grants.xlsx
@@ -1,29 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/westsi/Documents/GitHub/zing/open/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F630A17-6298-1045-B6E2-DC0A8F209CDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{7A421DAB-A5F7-574D-AD7B-D769D5D483FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Grants" sheetId="1" r:id="rId1"/>
+    <sheet name="grants2" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Grants!$A$1:$AL$60</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">grants2!$A$1:$AL$60</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -62,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1481" uniqueCount="502">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1597" uniqueCount="538">
   <si>
     <t>Identifier</t>
   </si>
@@ -1571,6 +1573,116 @@
   </si>
   <si>
     <t>S60 1NA</t>
+  </si>
+  <si>
+    <t>360G-zing-78</t>
+  </si>
+  <si>
+    <t>360G-zing-79</t>
+  </si>
+  <si>
+    <t>360G-zing-80</t>
+  </si>
+  <si>
+    <t>360G-zing-81</t>
+  </si>
+  <si>
+    <t>360G-zing-82</t>
+  </si>
+  <si>
+    <t>360G-zing-83</t>
+  </si>
+  <si>
+    <t>Whatever It Takes</t>
+  </si>
+  <si>
+    <t>Fair Education Alliance</t>
+  </si>
+  <si>
+    <t>Learning with Parents</t>
+  </si>
+  <si>
+    <t>Funding toward a Head of Programmes and Partnerships role</t>
+  </si>
+  <si>
+    <t>Funding to cover a Head of Programmes and Partnership role, freeing up capacity from programme delivery onto sales, fundraising and strategy.</t>
+  </si>
+  <si>
+    <t>GB-CHC-1188042</t>
+  </si>
+  <si>
+    <t>6 Mitre Passage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE10 0ER
+</t>
+  </si>
+  <si>
+    <t>https://www.faireducation.org.uk/</t>
+  </si>
+  <si>
+    <t>The Fair Education Alliance is a coalition of over 160 organisations working to end educational inequality. Together they drive lasting change at a local and national level, monitoring the gap between the most disadvantaged children and their wealthier peers, and using their collective voice and resources to end educational inequality.</t>
+  </si>
+  <si>
+    <t>Digital transformation programme</t>
+  </si>
+  <si>
+    <t>Funding and digital support toward the roll out of a digital transformation programme, as the Fair Education Alliance becomes independent from Teach First. This strand covers the auditing of the FEA membership, regularly gathering membership data for both the secretariat and members, and the piloting of tools to effectively leverage this data, aiming to improve collaboration across the membership. This core funding covers the role of a project manager in 2020, who will manage the execution of a digital transformation plan, including member audit and digital FEA member services.</t>
+  </si>
+  <si>
+    <t>Whatever It Takes (WIT) exists to break the destructive cycle of offending behaviours in children enabling them to enjoy lives of choice and opportunity. Highly skilled WIT Guides work alongside young people who are involved in – or are at risk of - criminal behaviours. WIT gives the young people a chance to take control over their lives and break the destructive cycle which causes deep trauma, as well as costing the taxpayer millions of pounds.</t>
+  </si>
+  <si>
+    <t>11928188</t>
+  </si>
+  <si>
+    <t>GB-COH-11928188</t>
+  </si>
+  <si>
+    <t>Funding toward a pilot of the WIT's model over 18 months in five local authority areas. WIT will work alongside 25 young people and their families per area, building relationships so that the 18 months of intensive work is outcome focussed and impactful.</t>
+  </si>
+  <si>
+    <t>Funding toward a pilot of WIT's model in five local authorities</t>
+  </si>
+  <si>
+    <t>COVID19 response funding. Funding to support the launching of a rapid response grant process to help young people around the world lead projects that address community impacts of COVID-19, from providing meals to elderly neighbors, to launching digital mental health campaigns to support youth feeling isolated.</t>
+  </si>
+  <si>
+    <t>Platform development in response to COVID19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In response to COVID19, Learning with Parents has seen an overwhelming increase in demand for their parental engagement tool Maths with Parents. To cope with increased demand on the platform across the UK, and the roll out of improvements to the service, we have given core funding toward the salary of an interim CTO, and the back end platform, and digital support/ connections toward the rebuilding of their front-end website.
+</t>
+  </si>
+  <si>
+    <t>Core funding for an interim CTO and platform improvements in response to COVID19</t>
+  </si>
+  <si>
+    <t>https://www.learningwithparents.com/</t>
+  </si>
+  <si>
+    <t>GB-COH-09622195</t>
+  </si>
+  <si>
+    <t>09622195</t>
+  </si>
+  <si>
+    <t>59 Church Lane</t>
+  </si>
+  <si>
+    <t>Wareham</t>
+  </si>
+  <si>
+    <t>BH20 6DD</t>
+  </si>
+  <si>
+    <t>Learning with Parent's mission is to motivate and empower families to have enjoyable learning experiences together. Through their programmes, they partner with schools to drive and monitor effective parental engagement and to support disadvantaged families,  and partner with organisations to champion parental engagement as a means to narrow the disadvantage gap.</t>
+  </si>
+  <si>
+    <t>Core funding in response to COVID19, toward coverage of a shortage in event fundraising, which was due to run during the UK lockdown.</t>
+  </si>
+  <si>
+    <t>Core funding in response to COVID19</t>
   </si>
 </sst>
 </file>
@@ -1684,7 +1796,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1780,6 +1892,12 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -2100,13 +2218,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AL74"/>
+  <dimension ref="A1:AL79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2358,8 +2476,8 @@
       </c>
       <c r="AJ2" s="6"/>
       <c r="AK2" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ref="AK2:AK33" ca="1" si="0">NOW()</f>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL2" s="14" t="s">
         <v>335</v>
@@ -2455,8 +2573,8 @@
       </c>
       <c r="AJ3" s="6"/>
       <c r="AK3" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL3" s="14" t="s">
         <v>335</v>
@@ -2552,8 +2670,8 @@
       </c>
       <c r="AJ4" s="6"/>
       <c r="AK4" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL4" s="14" t="s">
         <v>335</v>
@@ -2649,8 +2767,8 @@
       </c>
       <c r="AJ5" s="6"/>
       <c r="AK5" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL5" s="14" t="s">
         <v>335</v>
@@ -2746,8 +2864,8 @@
       </c>
       <c r="AJ6" s="6"/>
       <c r="AK6" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL6" s="14" t="s">
         <v>335</v>
@@ -2843,8 +2961,8 @@
       </c>
       <c r="AJ7" s="6"/>
       <c r="AK7" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL7" s="14" t="s">
         <v>335</v>
@@ -2940,8 +3058,8 @@
       </c>
       <c r="AJ8" s="6"/>
       <c r="AK8" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL8" s="14" t="s">
         <v>335</v>
@@ -3035,8 +3153,8 @@
       </c>
       <c r="AJ9" s="6"/>
       <c r="AK9" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL9" s="14" t="s">
         <v>335</v>
@@ -3132,8 +3250,8 @@
       </c>
       <c r="AJ10" s="6"/>
       <c r="AK10" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL10" s="14" t="s">
         <v>335</v>
@@ -3227,8 +3345,8 @@
       </c>
       <c r="AJ11" s="6"/>
       <c r="AK11" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL11" s="14" t="s">
         <v>335</v>
@@ -3324,8 +3442,8 @@
       </c>
       <c r="AJ12" s="6"/>
       <c r="AK12" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL12" s="14" t="s">
         <v>335</v>
@@ -3419,8 +3537,8 @@
       </c>
       <c r="AJ13" s="6"/>
       <c r="AK13" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL13" s="14" t="s">
         <v>335</v>
@@ -3516,8 +3634,8 @@
       </c>
       <c r="AJ14" s="6"/>
       <c r="AK14" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL14" s="14" t="s">
         <v>335</v>
@@ -3611,8 +3729,8 @@
       </c>
       <c r="AJ15" s="6"/>
       <c r="AK15" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL15" s="14" t="s">
         <v>335</v>
@@ -3706,8 +3824,8 @@
       </c>
       <c r="AJ16" s="6"/>
       <c r="AK16" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL16" s="14" t="s">
         <v>335</v>
@@ -3803,8 +3921,8 @@
       </c>
       <c r="AJ17" s="6"/>
       <c r="AK17" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL17" s="14" t="s">
         <v>335</v>
@@ -3900,8 +4018,8 @@
       </c>
       <c r="AJ18" s="6"/>
       <c r="AK18" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL18" s="14" t="s">
         <v>335</v>
@@ -3995,8 +4113,8 @@
       </c>
       <c r="AJ19" s="6"/>
       <c r="AK19" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL19" s="14" t="s">
         <v>335</v>
@@ -4090,8 +4208,8 @@
       </c>
       <c r="AJ20" s="6"/>
       <c r="AK20" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL20" s="14" t="s">
         <v>335</v>
@@ -4187,8 +4305,8 @@
       </c>
       <c r="AJ21" s="6"/>
       <c r="AK21" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL21" s="14" t="s">
         <v>335</v>
@@ -4282,8 +4400,8 @@
       </c>
       <c r="AJ22" s="6"/>
       <c r="AK22" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL22" s="14" t="s">
         <v>335</v>
@@ -4379,8 +4497,8 @@
       </c>
       <c r="AJ23" s="6"/>
       <c r="AK23" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL23" s="14" t="s">
         <v>335</v>
@@ -4476,8 +4594,8 @@
       </c>
       <c r="AJ24" s="6"/>
       <c r="AK24" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL24" s="14" t="s">
         <v>335</v>
@@ -4571,8 +4689,8 @@
       </c>
       <c r="AJ25" s="6"/>
       <c r="AK25" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL25" s="14" t="s">
         <v>335</v>
@@ -4668,8 +4786,8 @@
       </c>
       <c r="AJ26" s="6"/>
       <c r="AK26" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL26" s="14" t="s">
         <v>335</v>
@@ -4765,8 +4883,8 @@
       </c>
       <c r="AJ27" s="6"/>
       <c r="AK27" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL27" s="14" t="s">
         <v>335</v>
@@ -4860,8 +4978,8 @@
       </c>
       <c r="AJ28" s="6"/>
       <c r="AK28" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL28" s="14" t="s">
         <v>335</v>
@@ -4957,8 +5075,8 @@
       </c>
       <c r="AJ29" s="6"/>
       <c r="AK29" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL29" s="14" t="s">
         <v>335</v>
@@ -5052,8 +5170,8 @@
       </c>
       <c r="AJ30" s="6"/>
       <c r="AK30" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL30" s="14" t="s">
         <v>335</v>
@@ -5149,8 +5267,8 @@
       </c>
       <c r="AJ31" s="6"/>
       <c r="AK31" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL31" s="14" t="s">
         <v>335</v>
@@ -5246,8 +5364,8 @@
       </c>
       <c r="AJ32" s="6"/>
       <c r="AK32" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL32" s="14" t="s">
         <v>335</v>
@@ -5343,8 +5461,8 @@
       </c>
       <c r="AJ33" s="6"/>
       <c r="AK33" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL33" s="14" t="s">
         <v>335</v>
@@ -5440,8 +5558,8 @@
       </c>
       <c r="AJ34" s="6"/>
       <c r="AK34" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ref="AK34:AK65" ca="1" si="1">NOW()</f>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL34" s="14" t="s">
         <v>335</v>
@@ -5535,8 +5653,8 @@
       </c>
       <c r="AJ35" s="6"/>
       <c r="AK35" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL35" s="14" t="s">
         <v>335</v>
@@ -5632,8 +5750,8 @@
       </c>
       <c r="AJ36" s="6"/>
       <c r="AK36" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL36" s="14" t="s">
         <v>335</v>
@@ -5727,8 +5845,8 @@
       </c>
       <c r="AJ37" s="6"/>
       <c r="AK37" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL37" s="14" t="s">
         <v>335</v>
@@ -5824,8 +5942,8 @@
       </c>
       <c r="AJ38" s="6"/>
       <c r="AK38" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL38" s="14" t="s">
         <v>335</v>
@@ -5921,8 +6039,8 @@
       </c>
       <c r="AJ39" s="6"/>
       <c r="AK39" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL39" s="14" t="s">
         <v>335</v>
@@ -6018,8 +6136,8 @@
       </c>
       <c r="AJ40" s="6"/>
       <c r="AK40" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL40" s="14" t="s">
         <v>335</v>
@@ -6115,8 +6233,8 @@
       </c>
       <c r="AJ41" s="6"/>
       <c r="AK41" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL41" s="14" t="s">
         <v>335</v>
@@ -6212,8 +6330,8 @@
       </c>
       <c r="AJ42" s="6"/>
       <c r="AK42" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL42" s="14" t="s">
         <v>335</v>
@@ -6309,8 +6427,8 @@
       </c>
       <c r="AJ43" s="6"/>
       <c r="AK43" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL43" s="14" t="s">
         <v>335</v>
@@ -6404,8 +6522,8 @@
       </c>
       <c r="AJ44" s="6"/>
       <c r="AK44" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL44" s="14" t="s">
         <v>335</v>
@@ -6501,8 +6619,8 @@
       </c>
       <c r="AJ45" s="6"/>
       <c r="AK45" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL45" s="14" t="s">
         <v>335</v>
@@ -6596,8 +6714,8 @@
       </c>
       <c r="AJ46" s="6"/>
       <c r="AK46" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL46" s="14" t="s">
         <v>335</v>
@@ -6693,8 +6811,8 @@
       </c>
       <c r="AJ47" s="6"/>
       <c r="AK47" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL47" s="14" t="s">
         <v>335</v>
@@ -6788,8 +6906,8 @@
       </c>
       <c r="AJ48" s="6"/>
       <c r="AK48" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL48" s="14" t="s">
         <v>335</v>
@@ -6885,8 +7003,8 @@
       </c>
       <c r="AJ49" s="6"/>
       <c r="AK49" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL49" s="14" t="s">
         <v>335</v>
@@ -6982,8 +7100,8 @@
       </c>
       <c r="AJ50" s="6"/>
       <c r="AK50" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL50" s="14" t="s">
         <v>335</v>
@@ -7077,8 +7195,8 @@
       </c>
       <c r="AJ51" s="6"/>
       <c r="AK51" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL51" s="14" t="s">
         <v>335</v>
@@ -7174,8 +7292,8 @@
       </c>
       <c r="AJ52" s="6"/>
       <c r="AK52" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL52" s="14" t="s">
         <v>335</v>
@@ -7271,8 +7389,8 @@
       </c>
       <c r="AJ53" s="6"/>
       <c r="AK53" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL53" s="14" t="s">
         <v>335</v>
@@ -7365,8 +7483,8 @@
         <v>51</v>
       </c>
       <c r="AK54" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL54" s="14" t="s">
         <v>335</v>
@@ -7460,8 +7578,8 @@
       </c>
       <c r="AJ55" s="24"/>
       <c r="AK55" s="24">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL55" s="14" t="s">
         <v>335</v>
@@ -7557,8 +7675,8 @@
       </c>
       <c r="AJ56" s="24"/>
       <c r="AK56" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL56" s="14" t="s">
         <v>335</v>
@@ -7654,8 +7772,8 @@
       </c>
       <c r="AJ57" s="6"/>
       <c r="AK57" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL57" s="14" t="s">
         <v>335</v>
@@ -7749,8 +7867,8 @@
       </c>
       <c r="AJ58" s="6"/>
       <c r="AK58" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL58" s="14" t="s">
         <v>335</v>
@@ -7846,8 +7964,8 @@
       </c>
       <c r="AJ59" s="6"/>
       <c r="AK59" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL59" s="14" t="s">
         <v>335</v>
@@ -7943,8 +8061,8 @@
       </c>
       <c r="AJ60" s="6"/>
       <c r="AK60" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL60" s="14" t="s">
         <v>335</v>
@@ -8038,8 +8156,8 @@
       </c>
       <c r="AJ61" s="6"/>
       <c r="AK61" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL61" s="14" t="s">
         <v>335</v>
@@ -8079,7 +8197,9 @@
       <c r="K62" s="9">
         <v>43861</v>
       </c>
-      <c r="L62" s="9"/>
+      <c r="L62" s="9">
+        <v>43861</v>
+      </c>
       <c r="M62" s="6">
         <v>12</v>
       </c>
@@ -8131,8 +8251,8 @@
       </c>
       <c r="AJ62" s="6"/>
       <c r="AK62" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL62" s="14" t="s">
         <v>335</v>
@@ -8172,7 +8292,9 @@
       <c r="K63" s="9">
         <v>43862</v>
       </c>
-      <c r="L63" s="9"/>
+      <c r="L63" s="9">
+        <v>43862</v>
+      </c>
       <c r="M63" s="6">
         <v>12</v>
       </c>
@@ -8224,8 +8346,8 @@
       </c>
       <c r="AJ63" s="6"/>
       <c r="AK63" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL63" s="14" t="s">
         <v>335</v>
@@ -8265,7 +8387,9 @@
       <c r="K64" s="9">
         <v>43908</v>
       </c>
-      <c r="L64" s="9"/>
+      <c r="L64" s="9">
+        <v>43908</v>
+      </c>
       <c r="M64" s="6">
         <v>12</v>
       </c>
@@ -8319,8 +8443,8 @@
       </c>
       <c r="AJ64" s="6"/>
       <c r="AK64" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL64" s="14" t="s">
         <v>335</v>
@@ -8360,7 +8484,9 @@
       <c r="K65" s="9">
         <v>43909</v>
       </c>
-      <c r="L65" s="9"/>
+      <c r="L65" s="9">
+        <v>43909</v>
+      </c>
       <c r="M65" s="6">
         <v>12</v>
       </c>
@@ -8414,8 +8540,8 @@
       </c>
       <c r="AJ65" s="6"/>
       <c r="AK65" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL65" s="14" t="s">
         <v>335</v>
@@ -8509,8 +8635,8 @@
       </c>
       <c r="AJ66" s="6"/>
       <c r="AK66" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ref="AK66:AK71" ca="1" si="2">NOW()</f>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL66" s="14" t="s">
         <v>335</v>
@@ -8550,7 +8676,9 @@
       <c r="K67" s="9">
         <v>43922</v>
       </c>
-      <c r="L67" s="9"/>
+      <c r="L67" s="9">
+        <v>43922</v>
+      </c>
       <c r="M67" s="6">
         <v>12</v>
       </c>
@@ -8604,8 +8732,8 @@
       </c>
       <c r="AJ67" s="6"/>
       <c r="AK67" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL67" s="14" t="s">
         <v>335</v>
@@ -8697,8 +8825,8 @@
       </c>
       <c r="AJ68" s="6"/>
       <c r="AK68" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL68" s="14" t="s">
         <v>335</v>
@@ -8789,8 +8917,8 @@
       </c>
       <c r="AJ69" s="6"/>
       <c r="AK69" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL69" s="14" t="s">
         <v>335</v>
@@ -8884,8 +9012,8 @@
       </c>
       <c r="AJ70" s="6"/>
       <c r="AK70" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL70" s="14" t="s">
         <v>335</v>
@@ -8977,35 +9105,71 @@
       </c>
       <c r="AJ71" s="6"/>
       <c r="AK71" s="13">
-        <f ca="1">NOW()</f>
-        <v>43816.726411574076</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>43930.97215671296</v>
       </c>
       <c r="AL71" s="14" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="72" spans="1:38" ht="14" x14ac:dyDescent="0.15">
-      <c r="A72" s="6"/>
-      <c r="B72" s="6"/>
-      <c r="C72" s="6"/>
-      <c r="D72" s="6"/>
-      <c r="E72" s="8"/>
-      <c r="F72" s="8"/>
-      <c r="G72" s="6"/>
-      <c r="H72" s="9"/>
+    <row r="72" spans="1:38" ht="42" x14ac:dyDescent="0.15">
+      <c r="A72" s="6" t="s">
+        <v>502</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>524</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>523</v>
+      </c>
+      <c r="D72" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E72" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="F72" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="G72" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="H72" s="9">
+        <v>43831</v>
+      </c>
       <c r="I72" s="6"/>
-      <c r="J72" s="9"/>
-      <c r="K72" s="9"/>
+      <c r="J72" s="9">
+        <v>43831</v>
+      </c>
+      <c r="K72" s="9">
+        <v>44197</v>
+      </c>
       <c r="L72" s="9"/>
-      <c r="M72" s="6"/>
-      <c r="N72" s="6"/>
-      <c r="O72" s="6"/>
+      <c r="M72" s="6">
+        <v>12</v>
+      </c>
+      <c r="N72" s="34" t="s">
+        <v>522</v>
+      </c>
+      <c r="O72" s="6" t="s">
+        <v>508</v>
+      </c>
       <c r="P72" s="26"/>
-      <c r="Q72" s="8"/>
-      <c r="R72" s="6"/>
-      <c r="S72" s="6"/>
-      <c r="T72" s="6"/>
-      <c r="U72" s="7"/>
+      <c r="Q72" s="8" t="s">
+        <v>521</v>
+      </c>
+      <c r="R72" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="S72" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="T72" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="U72" s="7" t="s">
+        <v>520</v>
+      </c>
       <c r="V72" s="6"/>
       <c r="W72" s="6"/>
       <c r="X72" s="6"/>
@@ -9013,22 +9177,486 @@
       <c r="Z72" s="6"/>
       <c r="AA72" s="6"/>
       <c r="AB72" s="6"/>
-      <c r="AC72" s="6"/>
-      <c r="AD72" s="6"/>
+      <c r="AC72" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD72" s="6" t="s">
+        <v>50</v>
+      </c>
       <c r="AE72" s="6"/>
       <c r="AF72" s="6"/>
-      <c r="AG72" s="6"/>
+      <c r="AG72" s="6" t="s">
+        <v>50</v>
+      </c>
       <c r="AH72" s="6"/>
-      <c r="AI72" s="6"/>
+      <c r="AI72" s="19" t="s">
+        <v>51</v>
+      </c>
       <c r="AJ72" s="6"/>
-      <c r="AK72" s="13"/>
-      <c r="AL72" s="6"/>
+      <c r="AK72" s="13">
+        <f t="shared" ref="AK72:AK77" ca="1" si="3">NOW()</f>
+        <v>43930.97215671296</v>
+      </c>
+      <c r="AL72" s="14" t="s">
+        <v>335</v>
+      </c>
     </row>
-    <row r="73" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="P73" s="31"/>
+    <row r="73" spans="1:38" ht="70" x14ac:dyDescent="0.15">
+      <c r="A73" s="6" t="s">
+        <v>503</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>518</v>
+      </c>
+      <c r="C73" s="33" t="s">
+        <v>519</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E73" s="5">
+        <v>35000</v>
+      </c>
+      <c r="F73" s="5">
+        <v>35000</v>
+      </c>
+      <c r="G73" s="5">
+        <v>35000</v>
+      </c>
+      <c r="H73" s="9">
+        <v>43831</v>
+      </c>
+      <c r="I73" s="14" t="s">
+        <v>516</v>
+      </c>
+      <c r="J73" s="9">
+        <v>43831</v>
+      </c>
+      <c r="K73" s="9">
+        <v>44197</v>
+      </c>
+      <c r="M73" s="5">
+        <v>12</v>
+      </c>
+      <c r="N73" s="5" t="s">
+        <v>513</v>
+      </c>
+      <c r="O73" s="5" t="s">
+        <v>509</v>
+      </c>
+      <c r="P73" s="31">
+        <v>1188042</v>
+      </c>
+      <c r="Q73" s="5">
+        <v>11884952</v>
+      </c>
+      <c r="R73" s="5" t="s">
+        <v>514</v>
+      </c>
+      <c r="S73" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="T73" s="33" t="s">
+        <v>515</v>
+      </c>
+      <c r="U73" s="33" t="s">
+        <v>517</v>
+      </c>
+      <c r="V73" s="14" t="s">
+        <v>516</v>
+      </c>
+      <c r="AC73" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD73" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE73" s="6"/>
+      <c r="AF73" s="6"/>
+      <c r="AG73" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH73" s="6"/>
+      <c r="AI73" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ73" s="6"/>
+      <c r="AK73" s="13">
+        <f t="shared" ca="1" si="3"/>
+        <v>43930.97215671296</v>
+      </c>
+      <c r="AL73" s="14" t="s">
+        <v>335</v>
+      </c>
     </row>
-    <row r="74" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="P74" s="31"/>
+    <row r="74" spans="1:38" ht="56" x14ac:dyDescent="0.15">
+      <c r="A74" s="11" t="s">
+        <v>504</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>511</v>
+      </c>
+      <c r="C74" s="33" t="s">
+        <v>512</v>
+      </c>
+      <c r="D74" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E74" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="F74" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="G74" s="6">
+        <v>25000</v>
+      </c>
+      <c r="H74" s="9">
+        <v>43862</v>
+      </c>
+      <c r="I74" s="14" t="s">
+        <v>426</v>
+      </c>
+      <c r="J74" s="9">
+        <v>43862</v>
+      </c>
+      <c r="K74" s="9">
+        <v>43862</v>
+      </c>
+      <c r="L74" s="9"/>
+      <c r="M74" s="6">
+        <v>12</v>
+      </c>
+      <c r="N74" s="11" t="s">
+        <v>429</v>
+      </c>
+      <c r="O74" s="11" t="s">
+        <v>427</v>
+      </c>
+      <c r="P74" s="26"/>
+      <c r="Q74" s="12" t="s">
+        <v>428</v>
+      </c>
+      <c r="R74" s="11" t="s">
+        <v>430</v>
+      </c>
+      <c r="S74" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="T74" s="11" t="s">
+        <v>431</v>
+      </c>
+      <c r="U74" s="15" t="s">
+        <v>432</v>
+      </c>
+      <c r="V74" s="14" t="s">
+        <v>426</v>
+      </c>
+      <c r="W74" s="6"/>
+      <c r="X74" s="6"/>
+      <c r="Y74" s="6"/>
+      <c r="Z74" s="6"/>
+      <c r="AA74" s="6"/>
+      <c r="AB74" s="6"/>
+      <c r="AC74" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD74" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE74" s="6"/>
+      <c r="AF74" s="6"/>
+      <c r="AG74" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH74" s="6"/>
+      <c r="AI74" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ74" s="6"/>
+      <c r="AK74" s="13">
+        <f t="shared" ca="1" si="3"/>
+        <v>43930.97215671296</v>
+      </c>
+      <c r="AL74" s="14" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="75" spans="1:38" ht="42" x14ac:dyDescent="0.15">
+      <c r="A75" s="6" t="s">
+        <v>505</v>
+      </c>
+      <c r="B75" s="6" t="s">
+        <v>526</v>
+      </c>
+      <c r="C75" s="7" t="s">
+        <v>525</v>
+      </c>
+      <c r="D75" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="E75" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="F75" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="G75" s="6">
+        <v>32500</v>
+      </c>
+      <c r="H75" s="9">
+        <v>43922</v>
+      </c>
+      <c r="I75" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="J75" s="9">
+        <v>43922</v>
+      </c>
+      <c r="K75" s="9">
+        <v>44287</v>
+      </c>
+      <c r="L75" s="9"/>
+      <c r="M75" s="6">
+        <v>12</v>
+      </c>
+      <c r="N75" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="O75" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="P75" s="25" t="s">
+        <v>311</v>
+      </c>
+      <c r="Q75" s="8"/>
+      <c r="R75" s="6" t="s">
+        <v>381</v>
+      </c>
+      <c r="S75" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="T75" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="U75" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="V75" s="14" t="s">
+        <v>380</v>
+      </c>
+      <c r="W75" s="6"/>
+      <c r="X75" s="6"/>
+      <c r="Y75" s="6"/>
+      <c r="Z75" s="6"/>
+      <c r="AA75" s="6"/>
+      <c r="AB75" s="6"/>
+      <c r="AC75" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD75" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE75" s="6"/>
+      <c r="AF75" s="6"/>
+      <c r="AG75" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH75" s="6"/>
+      <c r="AI75" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ75" s="6"/>
+      <c r="AK75" s="13">
+        <f t="shared" ca="1" si="3"/>
+        <v>43930.97215671296</v>
+      </c>
+      <c r="AL75" s="14" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="76" spans="1:38" ht="70" x14ac:dyDescent="0.15">
+      <c r="A76" s="5" t="s">
+        <v>506</v>
+      </c>
+      <c r="B76" s="33" t="s">
+        <v>528</v>
+      </c>
+      <c r="C76" s="33" t="s">
+        <v>527</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E76" s="5">
+        <v>35000</v>
+      </c>
+      <c r="F76" s="5">
+        <v>35000</v>
+      </c>
+      <c r="G76" s="5">
+        <v>35000</v>
+      </c>
+      <c r="H76" s="9">
+        <v>43922</v>
+      </c>
+      <c r="I76" s="14" t="s">
+        <v>529</v>
+      </c>
+      <c r="J76" s="9">
+        <v>43922</v>
+      </c>
+      <c r="K76" s="9">
+        <v>43922</v>
+      </c>
+      <c r="M76" s="5">
+        <v>12</v>
+      </c>
+      <c r="N76" s="5" t="s">
+        <v>530</v>
+      </c>
+      <c r="O76" s="5" t="s">
+        <v>510</v>
+      </c>
+      <c r="Q76" s="8" t="s">
+        <v>531</v>
+      </c>
+      <c r="R76" s="5" t="s">
+        <v>532</v>
+      </c>
+      <c r="S76" s="5" t="s">
+        <v>533</v>
+      </c>
+      <c r="T76" s="5" t="s">
+        <v>534</v>
+      </c>
+      <c r="U76" s="33" t="s">
+        <v>535</v>
+      </c>
+      <c r="V76" s="14" t="s">
+        <v>529</v>
+      </c>
+      <c r="AC76" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD76" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE76" s="6"/>
+      <c r="AF76" s="6"/>
+      <c r="AG76" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH76" s="6"/>
+      <c r="AI76" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ76" s="6"/>
+      <c r="AK76" s="13">
+        <f t="shared" ca="1" si="3"/>
+        <v>43930.97215671296</v>
+      </c>
+      <c r="AL76" s="14" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="77" spans="1:38" ht="28" x14ac:dyDescent="0.15">
+      <c r="A77" s="6" t="s">
+        <v>507</v>
+      </c>
+      <c r="B77" s="11" t="s">
+        <v>537</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>536</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E77" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="F77" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="G77" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="H77" s="9">
+        <v>43922</v>
+      </c>
+      <c r="I77" s="14" t="s">
+        <v>332</v>
+      </c>
+      <c r="J77" s="9">
+        <v>43922</v>
+      </c>
+      <c r="K77" s="9">
+        <v>44287</v>
+      </c>
+      <c r="L77" s="9"/>
+      <c r="M77" s="6">
+        <v>12</v>
+      </c>
+      <c r="N77" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="O77" s="11" t="s">
+        <v>321</v>
+      </c>
+      <c r="P77" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q77" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="R77" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="S77" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="T77" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="U77" s="15" t="s">
+        <v>330</v>
+      </c>
+      <c r="V77" s="14" t="s">
+        <v>331</v>
+      </c>
+      <c r="W77" s="6"/>
+      <c r="X77" s="6"/>
+      <c r="Y77" s="6"/>
+      <c r="Z77" s="6"/>
+      <c r="AA77" s="6"/>
+      <c r="AB77" s="6"/>
+      <c r="AC77" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD77" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE77" s="6"/>
+      <c r="AF77" s="6"/>
+      <c r="AG77" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH77" s="6"/>
+      <c r="AI77" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ77" s="6"/>
+      <c r="AK77" s="13">
+        <f t="shared" ca="1" si="3"/>
+        <v>43930.97215671296</v>
+      </c>
+      <c r="AL77" s="14" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="79" spans="1:38" ht="13" x14ac:dyDescent="0.15">
+      <c r="C79" s="33"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AL60" xr:uid="{AE487DEF-5BC5-C74D-81B1-9FC54E50B3DD}"/>
@@ -9128,8 +9756,22 @@
     <hyperlink ref="V71" r:id="rId92" xr:uid="{E71ED7BD-E5E9-ED45-9956-D79CB4FB1410}"/>
     <hyperlink ref="I71" r:id="rId93" xr:uid="{491B3049-EF60-354B-AC90-AA0512B6FB72}"/>
     <hyperlink ref="AL71" r:id="rId94" xr:uid="{37973771-8508-B24C-8A43-D902FF3DE69F}"/>
+    <hyperlink ref="AL74" r:id="rId95" xr:uid="{813A9767-5A5C-1E4B-8CAC-481513D92A4B}"/>
+    <hyperlink ref="I73" r:id="rId96" xr:uid="{1D988DBE-E222-9043-861D-A4E21AF8826D}"/>
+    <hyperlink ref="V73" r:id="rId97" xr:uid="{E3FFE7F8-67F0-7443-8179-22E2D934944E}"/>
+    <hyperlink ref="AL73" r:id="rId98" xr:uid="{7081D0A4-B78D-8F41-9487-B7773A37DAE5}"/>
+    <hyperlink ref="AL72" r:id="rId99" xr:uid="{2D382975-D5B2-5B41-AA68-D8D6D1D7C7C4}"/>
+    <hyperlink ref="AL76" r:id="rId100" xr:uid="{40A95119-13E8-9D40-9DA6-CF3430DF851A}"/>
+    <hyperlink ref="AL75" r:id="rId101" xr:uid="{85EE67B9-1258-8C40-B222-6918288E2D62}"/>
+    <hyperlink ref="I75" r:id="rId102" xr:uid="{4F2FD5F2-07BB-F344-B03C-C531B6301030}"/>
+    <hyperlink ref="V75" r:id="rId103" xr:uid="{1D6E0862-68FC-E84D-A816-48A59F6F2190}"/>
+    <hyperlink ref="I76" r:id="rId104" xr:uid="{629C2154-EA93-2F4C-9BC6-6C84DE5DC933}"/>
+    <hyperlink ref="V76" r:id="rId105" xr:uid="{07E9327F-BD85-B440-96AF-413EC0A70775}"/>
+    <hyperlink ref="I77" r:id="rId106" xr:uid="{A4F9853C-1EE6-4346-9E22-97719CE9CFC7}"/>
+    <hyperlink ref="V77" r:id="rId107" xr:uid="{D6D00EB7-DDFD-A64B-8062-E149826074F6}"/>
+    <hyperlink ref="AL77" r:id="rId108" xr:uid="{A023ACBB-504F-B640-A1C5-0A5B79E91403}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId95"/>
+  <legacyDrawing r:id="rId109"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update 360 Giving Data
</commit_message>
<xml_diff>
--- a/open/grants.xlsx
+++ b/open/grants.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/westsi/Documents/GitHub/zing/open/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF9FADBF-0556-9540-B1E9-612BF5AFF7EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F86F2A7-83C9-584D-A789-C1F26425EC70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="grants2" sheetId="1" r:id="rId1"/>
+    <sheet name="grants" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">grants2!$A$1:$BJ$77</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">grants!$A$1:$BJ$77</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1903" uniqueCount="593">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1968" uniqueCount="618">
   <si>
     <t>Identifier</t>
   </si>
@@ -1848,6 +1848,81 @@
   </si>
   <si>
     <t>https://www.whateverittakesuk.com/</t>
+  </si>
+  <si>
+    <t>360G-zing-84</t>
+  </si>
+  <si>
+    <t>https://unloc.org.uk/</t>
+  </si>
+  <si>
+    <t>Unloc</t>
+  </si>
+  <si>
+    <t>GB-COH-08578126</t>
+  </si>
+  <si>
+    <t>08578126</t>
+  </si>
+  <si>
+    <t>Funding toward a digital lead role for unloc.online</t>
+  </si>
+  <si>
+    <t>1190809</t>
+  </si>
+  <si>
+    <t>360G-zing-85</t>
+  </si>
+  <si>
+    <t>Core funding toward year two of the Young Trustee Movement</t>
+  </si>
+  <si>
+    <t>Core funding for continuing the Young Trustee's Movement to increase the diversity of people on charity trustee boards, starting with a focus on doubling the number of young people under 30 on boards in the UK, by 2024 (currently 3%).</t>
+  </si>
+  <si>
+    <t>The Social Change Nest CIC</t>
+  </si>
+  <si>
+    <t>GB-COH-12611737</t>
+  </si>
+  <si>
+    <t>237 Pentonville Road</t>
+  </si>
+  <si>
+    <t>N1 9NG</t>
+  </si>
+  <si>
+    <t>https://thesocialchangeagency.org/nest-supporting-new-movements/</t>
+  </si>
+  <si>
+    <t>Portsmouth</t>
+  </si>
+  <si>
+    <t>PO3 6PZ</t>
+  </si>
+  <si>
+    <t>Portsmouth College, Tangier Rd</t>
+  </si>
+  <si>
+    <t>Unloc was founded in 2013 by award-winning young leaders and advocates Hayden Taylor and Ben Dowling. Their mission is to empower young people to be innovative changemakers who seek to build stronger communities and sustainable businesses. Unloc develops young people’s skills, enhances their potential and boosts their determination to succeed, through delivering inspiring educational programmes to a growing network of schools and colleges. Their programmes focus on developing: Leadership Skills, Entrepreneurial Skills, Student Voice, Career Pathways.</t>
+  </si>
+  <si>
+    <t>COVID19 response funding. In response to the April 2020 UK lockdown, Unloc rapidly built and launched Unloc.online, a new interactive e-learning platform, providing a series of online short courses designed to encourage students aged 11-19 to explore entrepreneurship, employability, leadership and career pathways from the comfort of their own home. The team is iterating the platform and addding new content with partners, driven by a desire to support the development of young people’s aspirations, skills and career prospects coming out of COVID-19 and into the fast changing labour market.</t>
+  </si>
+  <si>
+    <t>360G-zing-86</t>
+  </si>
+  <si>
+    <t>Funding for recipients of the Challenge and Change Fund</t>
+  </si>
+  <si>
+    <t>https://www.blagravetrust.org/challenge-and-change/</t>
+  </si>
+  <si>
+    <t>Challenge and Change is a fund dedicated to supporting the limitless energy of young people affected by injustices who are working tirelessly across England to create positive change. This fund was available to applicants 18-25 years old, working at the hard edge of injustice, and who have radical ideas, dreams, visions, and imaginations for a just and fair world for all. The fund offerred a package of mentoring and network support to help take their work to the next level.</t>
+  </si>
+  <si>
+    <t>The Blagrave Trust's mission is to bring lasting change to the lives of young people aged 14-25 who are facing significant challenges, to enable them to make a positive transition to adulthood. Their core ambitions are: to promote and empower young people as powerful forces for change, and ensure their voices are heard in matters than affect them; and to achieve social impact beyond our immediate partners in pursuit of a fair and just society.</t>
   </si>
 </sst>
 </file>
@@ -1961,7 +2036,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -2072,6 +2147,12 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2392,13 +2473,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:BJ79"/>
+  <dimension ref="A1:BJ80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="120" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="U80" sqref="U80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2411,7 +2492,7 @@
     <col min="6" max="6" width="15.33203125" style="5" customWidth="1"/>
     <col min="7" max="7" width="16.33203125" style="5" customWidth="1"/>
     <col min="8" max="8" width="33.33203125" style="5" customWidth="1"/>
-    <col min="9" max="9" width="28.6640625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="80.6640625" style="5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23.1640625" style="5" customWidth="1"/>
     <col min="11" max="11" width="22.5" style="5" customWidth="1"/>
     <col min="12" max="12" width="27.33203125" style="5" customWidth="1"/>
@@ -2766,7 +2847,7 @@
       <c r="BH2" s="6"/>
       <c r="BI2" s="13">
         <f t="shared" ref="BI2:BI33" ca="1" si="0">NOW()</f>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ2" s="14" t="s">
         <v>327</v>
@@ -2891,7 +2972,7 @@
       <c r="BH3" s="6"/>
       <c r="BI3" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ3" s="14" t="s">
         <v>327</v>
@@ -3019,7 +3100,7 @@
       <c r="BH4" s="6"/>
       <c r="BI4" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ4" s="14" t="s">
         <v>327</v>
@@ -3143,7 +3224,7 @@
       <c r="BH5" s="6"/>
       <c r="BI5" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ5" s="14" t="s">
         <v>327</v>
@@ -3271,7 +3352,7 @@
       <c r="BH6" s="6"/>
       <c r="BI6" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ6" s="14" t="s">
         <v>327</v>
@@ -3399,7 +3480,7 @@
       <c r="BH7" s="6"/>
       <c r="BI7" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ7" s="14" t="s">
         <v>327</v>
@@ -3528,7 +3609,7 @@
       <c r="BH8" s="6"/>
       <c r="BI8" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ8" s="14" t="s">
         <v>327</v>
@@ -3653,7 +3734,7 @@
       <c r="BH9" s="6"/>
       <c r="BI9" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ9" s="14" t="s">
         <v>327</v>
@@ -3758,7 +3839,7 @@
       <c r="BH10" s="6"/>
       <c r="BI10" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ10" s="14" t="s">
         <v>327</v>
@@ -3879,7 +3960,7 @@
       <c r="BH11" s="6"/>
       <c r="BI11" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ11" s="14" t="s">
         <v>327</v>
@@ -4006,7 +4087,7 @@
       <c r="BH12" s="6"/>
       <c r="BI12" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ12" s="14" t="s">
         <v>327</v>
@@ -4133,7 +4214,7 @@
       <c r="BH13" s="6"/>
       <c r="BI13" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ13" s="14" t="s">
         <v>327</v>
@@ -4262,7 +4343,7 @@
       <c r="BH14" s="6"/>
       <c r="BI14" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ14" s="14" t="s">
         <v>327</v>
@@ -4387,7 +4468,7 @@
       <c r="BH15" s="6"/>
       <c r="BI15" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ15" s="14" t="s">
         <v>327</v>
@@ -4512,7 +4593,7 @@
       <c r="BH16" s="6"/>
       <c r="BI16" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ16" s="14" t="s">
         <v>327</v>
@@ -4641,7 +4722,7 @@
       <c r="BH17" s="6"/>
       <c r="BI17" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ17" s="14" t="s">
         <v>327</v>
@@ -4770,7 +4851,7 @@
       <c r="BH18" s="6"/>
       <c r="BI18" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ18" s="14" t="s">
         <v>327</v>
@@ -4891,7 +4972,7 @@
       <c r="BH19" s="6"/>
       <c r="BI19" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ19" s="14" t="s">
         <v>327</v>
@@ -5018,7 +5099,7 @@
       <c r="BH20" s="6"/>
       <c r="BI20" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ20" s="14" t="s">
         <v>327</v>
@@ -5147,7 +5228,7 @@
       <c r="BH21" s="6"/>
       <c r="BI21" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ21" s="14" t="s">
         <v>327</v>
@@ -5274,7 +5355,7 @@
       <c r="BH22" s="6"/>
       <c r="BI22" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ22" s="14" t="s">
         <v>327</v>
@@ -5403,7 +5484,7 @@
       <c r="BH23" s="6"/>
       <c r="BI23" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ23" s="14" t="s">
         <v>327</v>
@@ -5528,7 +5609,7 @@
       <c r="BH24" s="6"/>
       <c r="BI24" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ24" s="14" t="s">
         <v>327</v>
@@ -5649,7 +5730,7 @@
       <c r="BH25" s="6"/>
       <c r="BI25" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ25" s="14" t="s">
         <v>327</v>
@@ -5776,7 +5857,7 @@
       <c r="BH26" s="6"/>
       <c r="BI26" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ26" s="14" t="s">
         <v>327</v>
@@ -5905,7 +5986,7 @@
       <c r="BH27" s="6"/>
       <c r="BI27" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ27" s="14" t="s">
         <v>327</v>
@@ -6030,7 +6111,7 @@
       <c r="BH28" s="6"/>
       <c r="BI28" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ28" s="14" t="s">
         <v>327</v>
@@ -6157,7 +6238,7 @@
       <c r="BH29" s="6"/>
       <c r="BI29" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ29" s="14" t="s">
         <v>327</v>
@@ -6282,7 +6363,7 @@
       <c r="BH30" s="6"/>
       <c r="BI30" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ30" s="14" t="s">
         <v>327</v>
@@ -6409,7 +6490,7 @@
       <c r="BH31" s="6"/>
       <c r="BI31" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ31" s="14" t="s">
         <v>327</v>
@@ -6536,7 +6617,7 @@
       <c r="BH32" s="6"/>
       <c r="BI32" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ32" s="14" t="s">
         <v>327</v>
@@ -6663,7 +6744,7 @@
       <c r="BH33" s="6"/>
       <c r="BI33" s="13">
         <f t="shared" ca="1" si="0"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ33" s="14" t="s">
         <v>327</v>
@@ -6804,7 +6885,7 @@
       <c r="BH34" s="6"/>
       <c r="BI34" s="13">
         <f t="shared" ref="BI34:BI65" ca="1" si="1">NOW()</f>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ34" s="14" t="s">
         <v>327</v>
@@ -6925,7 +7006,7 @@
       <c r="BH35" s="6"/>
       <c r="BI35" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ35" s="14" t="s">
         <v>327</v>
@@ -7050,7 +7131,7 @@
       <c r="BH36" s="6"/>
       <c r="BI36" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ36" s="14" t="s">
         <v>327</v>
@@ -7181,7 +7262,7 @@
       <c r="BH37" s="6"/>
       <c r="BI37" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ37" s="14" t="s">
         <v>327</v>
@@ -7308,7 +7389,7 @@
       <c r="BH38" s="6"/>
       <c r="BI38" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ38" s="14" t="s">
         <v>327</v>
@@ -7437,7 +7518,7 @@
       <c r="BH39" s="6"/>
       <c r="BI39" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ39" s="14" t="s">
         <v>327</v>
@@ -7566,7 +7647,7 @@
       <c r="BH40" s="6"/>
       <c r="BI40" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ40" s="14" t="s">
         <v>327</v>
@@ -7693,7 +7774,7 @@
       <c r="BH41" s="6"/>
       <c r="BI41" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ41" s="14" t="s">
         <v>327</v>
@@ -7830,7 +7911,7 @@
       <c r="BH42" s="6"/>
       <c r="BI42" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ42" s="14" t="s">
         <v>327</v>
@@ -7949,7 +8030,7 @@
       <c r="BH43" s="6"/>
       <c r="BI43" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ43" s="14" t="s">
         <v>327</v>
@@ -8069,7 +8150,7 @@
       <c r="BH44" s="6"/>
       <c r="BI44" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ44" s="14" t="s">
         <v>327</v>
@@ -8191,7 +8272,7 @@
       <c r="BH45" s="6"/>
       <c r="BI45" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ45" s="14" t="s">
         <v>327</v>
@@ -8311,7 +8392,7 @@
       <c r="BH46" s="6"/>
       <c r="BI46" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ46" s="14" t="s">
         <v>327</v>
@@ -8433,7 +8514,7 @@
       <c r="BH47" s="6"/>
       <c r="BI47" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ47" s="14" t="s">
         <v>327</v>
@@ -8553,7 +8634,7 @@
       <c r="BH48" s="6"/>
       <c r="BI48" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ48" s="14" t="s">
         <v>327</v>
@@ -8675,7 +8756,7 @@
       <c r="BH49" s="6"/>
       <c r="BI49" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ49" s="14" t="s">
         <v>327</v>
@@ -8797,7 +8878,7 @@
       <c r="BH50" s="6"/>
       <c r="BI50" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ50" s="14" t="s">
         <v>327</v>
@@ -8917,7 +8998,7 @@
       <c r="BH51" s="6"/>
       <c r="BI51" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ51" s="14" t="s">
         <v>327</v>
@@ -9039,7 +9120,7 @@
       <c r="BH52" s="6"/>
       <c r="BI52" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ52" s="14" t="s">
         <v>327</v>
@@ -9161,7 +9242,7 @@
       <c r="BH53" s="6"/>
       <c r="BI53" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ53" s="14" t="s">
         <v>327</v>
@@ -9287,7 +9368,7 @@
       </c>
       <c r="BI54" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ54" s="14" t="s">
         <v>327</v>
@@ -9414,7 +9495,7 @@
       <c r="BH55" s="23"/>
       <c r="BI55" s="23">
         <f t="shared" ca="1" si="1"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ55" s="14" t="s">
         <v>327</v>
@@ -9551,7 +9632,7 @@
       <c r="BH56" s="23"/>
       <c r="BI56" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ56" s="14" t="s">
         <v>327</v>
@@ -9673,7 +9754,7 @@
       <c r="BH57" s="6"/>
       <c r="BI57" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ57" s="14" t="s">
         <v>327</v>
@@ -9793,7 +9874,7 @@
       <c r="BH58" s="6"/>
       <c r="BI58" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ58" s="14" t="s">
         <v>327</v>
@@ -9915,7 +9996,7 @@
       <c r="BH59" s="6"/>
       <c r="BI59" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ59" s="14" t="s">
         <v>327</v>
@@ -10052,7 +10133,7 @@
       <c r="BH60" s="6"/>
       <c r="BI60" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ60" s="14" t="s">
         <v>327</v>
@@ -10167,7 +10248,7 @@
       <c r="BH61" s="6"/>
       <c r="BI61" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ61" s="14" t="s">
         <v>327</v>
@@ -10287,7 +10368,7 @@
       <c r="BH62" s="6"/>
       <c r="BI62" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ62" s="14" t="s">
         <v>327</v>
@@ -10407,7 +10488,7 @@
       <c r="BH63" s="6"/>
       <c r="BI63" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ63" s="14" t="s">
         <v>327</v>
@@ -10529,7 +10610,7 @@
       <c r="BH64" s="6"/>
       <c r="BI64" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ64" s="14" t="s">
         <v>327</v>
@@ -10654,7 +10735,7 @@
       <c r="BH65" s="6"/>
       <c r="BI65" s="13">
         <f t="shared" ca="1" si="1"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ65" s="14" t="s">
         <v>327</v>
@@ -10774,7 +10855,7 @@
       <c r="BH66" s="6"/>
       <c r="BI66" s="13">
         <f t="shared" ref="BI66:BI71" ca="1" si="2">NOW()</f>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ66" s="14" t="s">
         <v>327</v>
@@ -10911,7 +10992,7 @@
       <c r="BH67" s="6"/>
       <c r="BI67" s="13">
         <f t="shared" ca="1" si="2"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ67" s="14" t="s">
         <v>327</v>
@@ -11024,7 +11105,7 @@
       <c r="BH68" s="6"/>
       <c r="BI68" s="13">
         <f t="shared" ca="1" si="2"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ68" s="14" t="s">
         <v>327</v>
@@ -11141,7 +11222,7 @@
       <c r="BH69" s="6"/>
       <c r="BI69" s="13">
         <f t="shared" ca="1" si="2"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ69" s="14" t="s">
         <v>327</v>
@@ -11261,7 +11342,7 @@
       <c r="BH70" s="6"/>
       <c r="BI70" s="13">
         <f t="shared" ca="1" si="2"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ70" s="14" t="s">
         <v>327</v>
@@ -11390,7 +11471,7 @@
       <c r="BH71" s="6"/>
       <c r="BI71" s="13">
         <f t="shared" ca="1" si="2"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ71" s="14" t="s">
         <v>327</v>
@@ -11421,7 +11502,9 @@
       <c r="H72" s="9">
         <v>43831</v>
       </c>
-      <c r="I72" s="6"/>
+      <c r="I72" s="14" t="s">
+        <v>592</v>
+      </c>
       <c r="J72" s="9">
         <v>43831</v>
       </c>
@@ -11505,8 +11588,8 @@
       </c>
       <c r="BH72" s="6"/>
       <c r="BI72" s="13">
-        <f t="shared" ref="BI72:BI77" ca="1" si="3">NOW()</f>
-        <v>44033.538023379631</v>
+        <f t="shared" ref="BI72:BI80" ca="1" si="3">NOW()</f>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ72" s="14" t="s">
         <v>327</v>
@@ -11603,7 +11686,7 @@
       <c r="BH73" s="6"/>
       <c r="BI73" s="13">
         <f t="shared" ca="1" si="3"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ73" s="14" t="s">
         <v>327</v>
@@ -11653,7 +11736,9 @@
       <c r="O74" s="11" t="s">
         <v>419</v>
       </c>
-      <c r="P74" s="25"/>
+      <c r="P74" s="25" t="s">
+        <v>599</v>
+      </c>
       <c r="Q74" s="12" t="s">
         <v>420</v>
       </c>
@@ -11721,7 +11806,7 @@
       <c r="BH74" s="6"/>
       <c r="BI74" s="13">
         <f t="shared" ca="1" si="3"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ74" s="14" t="s">
         <v>327</v>
@@ -11834,7 +11919,7 @@
       <c r="BH75" s="6"/>
       <c r="BI75" s="13">
         <f t="shared" ca="1" si="3"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ75" s="14" t="s">
         <v>327</v>
@@ -11928,7 +12013,7 @@
       <c r="BH76" s="6"/>
       <c r="BI76" s="13">
         <f t="shared" ca="1" si="3"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ76" s="14" t="s">
         <v>327</v>
@@ -12063,17 +12148,315 @@
       <c r="BH77" s="6"/>
       <c r="BI77" s="13">
         <f t="shared" ca="1" si="3"/>
-        <v>44033.538023379631</v>
+        <v>44097.539150578705</v>
       </c>
       <c r="BJ77" s="14" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="78" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="AA78" s="6"/>
+    <row r="78" spans="1:62" ht="70" x14ac:dyDescent="0.15">
+      <c r="A78" s="6" t="s">
+        <v>593</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>598</v>
+      </c>
+      <c r="C78" s="39" t="s">
+        <v>612</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E78" s="5">
+        <v>30000</v>
+      </c>
+      <c r="F78" s="5">
+        <v>30000</v>
+      </c>
+      <c r="G78" s="5">
+        <v>30000</v>
+      </c>
+      <c r="H78" s="9">
+        <v>44075</v>
+      </c>
+      <c r="I78" s="14" t="s">
+        <v>594</v>
+      </c>
+      <c r="J78" s="9">
+        <v>44075</v>
+      </c>
+      <c r="K78" s="9">
+        <v>44440</v>
+      </c>
+      <c r="M78" s="5">
+        <v>12</v>
+      </c>
+      <c r="N78" s="5" t="s">
+        <v>596</v>
+      </c>
+      <c r="O78" s="5" t="s">
+        <v>595</v>
+      </c>
+      <c r="Q78" s="38" t="s">
+        <v>597</v>
+      </c>
+      <c r="R78" s="31" t="s">
+        <v>610</v>
+      </c>
+      <c r="S78" s="5" t="s">
+        <v>608</v>
+      </c>
+      <c r="T78" s="5" t="s">
+        <v>609</v>
+      </c>
+      <c r="U78" s="31" t="s">
+        <v>611</v>
+      </c>
+      <c r="V78" s="34" t="s">
+        <v>594</v>
+      </c>
+      <c r="W78" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="X78" s="6" t="s">
+        <v>531</v>
+      </c>
+      <c r="AA78" s="6" t="s">
+        <v>537</v>
+      </c>
+      <c r="BA78" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="BB78" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="BE78" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="BF78" s="6"/>
+      <c r="BG78" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="BH78" s="6"/>
+      <c r="BI78" s="13">
+        <f t="shared" ca="1" si="3"/>
+        <v>44097.539150578705</v>
+      </c>
+      <c r="BJ78" s="14" t="s">
+        <v>327</v>
+      </c>
     </row>
-    <row r="79" spans="1:62" ht="13" x14ac:dyDescent="0.15">
-      <c r="C79" s="31"/>
+    <row r="79" spans="1:62" ht="42" x14ac:dyDescent="0.15">
+      <c r="A79" s="5" t="s">
+        <v>600</v>
+      </c>
+      <c r="B79" s="6" t="s">
+        <v>601</v>
+      </c>
+      <c r="C79" s="15" t="s">
+        <v>602</v>
+      </c>
+      <c r="D79" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E79" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="F79" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="G79" s="6">
+        <v>10000</v>
+      </c>
+      <c r="H79" s="9">
+        <v>44075</v>
+      </c>
+      <c r="I79" s="14" t="s">
+        <v>472</v>
+      </c>
+      <c r="J79" s="9">
+        <v>44075</v>
+      </c>
+      <c r="K79" s="9">
+        <v>44440</v>
+      </c>
+      <c r="L79" s="9"/>
+      <c r="M79" s="6">
+        <v>12</v>
+      </c>
+      <c r="N79" s="11" t="s">
+        <v>604</v>
+      </c>
+      <c r="O79" s="11" t="s">
+        <v>603</v>
+      </c>
+      <c r="P79" s="28"/>
+      <c r="Q79" s="5">
+        <v>12611737</v>
+      </c>
+      <c r="R79" s="12" t="s">
+        <v>605</v>
+      </c>
+      <c r="S79" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="T79" s="11" t="s">
+        <v>606</v>
+      </c>
+      <c r="U79" s="15" t="s">
+        <v>479</v>
+      </c>
+      <c r="V79" s="34" t="s">
+        <v>607</v>
+      </c>
+      <c r="W79" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="X79" s="6" t="s">
+        <v>531</v>
+      </c>
+      <c r="Y79" s="6"/>
+      <c r="Z79" s="6"/>
+      <c r="AA79" s="6" t="s">
+        <v>542</v>
+      </c>
+      <c r="AC79" s="6"/>
+      <c r="AD79" s="6"/>
+      <c r="AE79" s="6"/>
+      <c r="AF79" s="6"/>
+      <c r="AG79" s="6"/>
+      <c r="AH79" s="6"/>
+      <c r="AK79" s="6"/>
+      <c r="AL79" s="6"/>
+      <c r="AO79" s="6"/>
+      <c r="AP79" s="6"/>
+      <c r="AQ79" s="6"/>
+      <c r="AR79" s="6"/>
+      <c r="AS79" s="6"/>
+      <c r="AT79" s="6"/>
+      <c r="AU79" s="6"/>
+      <c r="AV79" s="6"/>
+      <c r="AW79" s="6"/>
+      <c r="AX79" s="6"/>
+      <c r="AY79" s="6"/>
+      <c r="AZ79" s="6"/>
+      <c r="BA79" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="BB79" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="BC79" s="6"/>
+      <c r="BD79" s="6"/>
+      <c r="BE79" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="BF79" s="6"/>
+      <c r="BG79" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="BH79" s="6"/>
+      <c r="BI79" s="13">
+        <f t="shared" ca="1" si="3"/>
+        <v>44097.539150578705</v>
+      </c>
+      <c r="BJ79" s="14" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="80" spans="1:62" ht="56" x14ac:dyDescent="0.15">
+      <c r="A80" s="5" t="s">
+        <v>613</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>614</v>
+      </c>
+      <c r="C80" s="31" t="s">
+        <v>616</v>
+      </c>
+      <c r="D80" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E80" s="5">
+        <v>35000</v>
+      </c>
+      <c r="F80" s="5">
+        <v>35000</v>
+      </c>
+      <c r="G80" s="5">
+        <v>35000</v>
+      </c>
+      <c r="H80" s="9">
+        <v>44075</v>
+      </c>
+      <c r="I80" s="14" t="s">
+        <v>615</v>
+      </c>
+      <c r="J80" s="9">
+        <v>44075</v>
+      </c>
+      <c r="K80" s="9">
+        <v>44440</v>
+      </c>
+      <c r="M80" s="6">
+        <v>12</v>
+      </c>
+      <c r="N80" s="5" t="s">
+        <v>475</v>
+      </c>
+      <c r="O80" s="5" t="s">
+        <v>476</v>
+      </c>
+      <c r="P80" s="5">
+        <v>1164021</v>
+      </c>
+      <c r="R80" s="31" t="s">
+        <v>477</v>
+      </c>
+      <c r="S80" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="T80" s="5" t="s">
+        <v>478</v>
+      </c>
+      <c r="U80" s="31" t="s">
+        <v>617</v>
+      </c>
+      <c r="V80" s="34" t="s">
+        <v>480</v>
+      </c>
+      <c r="W80" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="X80" s="6" t="s">
+        <v>531</v>
+      </c>
+      <c r="AA80" s="6" t="s">
+        <v>537</v>
+      </c>
+      <c r="BA80" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="BB80" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="BC80" s="6"/>
+      <c r="BD80" s="6"/>
+      <c r="BE80" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="BF80" s="6"/>
+      <c r="BG80" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="BH80" s="6"/>
+      <c r="BI80" s="13">
+        <f t="shared" ca="1" si="3"/>
+        <v>44097.539150578705</v>
+      </c>
+      <c r="BJ80" s="14" t="s">
+        <v>327</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:BJ77" xr:uid="{AE487DEF-5BC5-C74D-81B1-9FC54E50B3DD}"/>
@@ -12188,8 +12571,18 @@
     <hyperlink ref="V77" r:id="rId107" xr:uid="{D6D00EB7-DDFD-A64B-8062-E149826074F6}"/>
     <hyperlink ref="BJ77" r:id="rId108" xr:uid="{A023ACBB-504F-B640-A1C5-0A5B79E91403}"/>
     <hyperlink ref="V72" r:id="rId109" xr:uid="{C02293C4-4667-6E44-8C7F-C4E4A5031761}"/>
+    <hyperlink ref="I78" r:id="rId110" xr:uid="{CDDF4B46-A7BD-C84F-984B-5D034786A844}"/>
+    <hyperlink ref="BJ78" r:id="rId111" xr:uid="{06B6D7C5-69AE-114E-9D14-5996D5312EF5}"/>
+    <hyperlink ref="I72" r:id="rId112" xr:uid="{0CEF14E7-E2E7-9C4F-9C4B-772B11C4EFF9}"/>
+    <hyperlink ref="BJ79" r:id="rId113" xr:uid="{2D2057F1-C09F-1547-9544-AF3EE83B9D68}"/>
+    <hyperlink ref="I79" r:id="rId114" xr:uid="{4F488052-9000-7E4E-832E-D1587AD242D1}"/>
+    <hyperlink ref="V79" r:id="rId115" xr:uid="{1E0742AD-3F3C-B54D-A360-9CF363257003}"/>
+    <hyperlink ref="V78" r:id="rId116" xr:uid="{F14A319E-D4E0-0748-B429-2DF8D61E490B}"/>
+    <hyperlink ref="I80" r:id="rId117" xr:uid="{C1793103-2F4B-604A-8D3A-446777DE1912}"/>
+    <hyperlink ref="V80" r:id="rId118" xr:uid="{6A84CF0E-CE2E-904A-8851-D4D90B970386}"/>
+    <hyperlink ref="BJ80" r:id="rId119" xr:uid="{FF417C2C-75CE-6347-B7BA-2A02C14CB6B4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId110"/>
+  <legacyDrawing r:id="rId120"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Tweak grant data for The Difference
360 Giving data update
</commit_message>
<xml_diff>
--- a/open/grants.xlsx
+++ b/open/grants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/westsi/Documents/GitHub/zing/open/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52EFFDF4-C958-6745-9B58-DD34BD937F1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC06D275-0C43-6A42-A694-C794819EC039}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1949,10 +1949,10 @@
     <t>360G-zing-88</t>
   </si>
   <si>
-    <t>Core funding for recruitment of a third teacher cohort</t>
-  </si>
-  <si>
-    <t>Seed funding toward the recruitment and training of The Difference's third cohort of leaders. A new career route, creating specialist teaching leaders positioned to drive inclusion in schools, and improve outcomes for the UK’s most vulnerable young people.</t>
+    <t>Seed funding toward year two of The Difference's school leadership programme, and the recruitment and training of The Difference's third cohort of leaders. This is a new career route, creating specialist teaching leaders positioned to drive inclusion in schools, and improve outcomes for the UK’s most vulnerable young people.</t>
+  </si>
+  <si>
+    <t>Core funding for years two and three of The Difference's school leadership programme</t>
   </si>
 </sst>
 </file>
@@ -2503,10 +2503,10 @@
   <dimension ref="A1:BJ82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C76" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2874,7 +2874,7 @@
       <c r="BH2" s="2"/>
       <c r="BI2" s="18">
         <f t="shared" ref="BI2:BI33" ca="1" si="0">NOW()</f>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ2" s="8" t="s">
         <v>327</v>
@@ -2999,7 +2999,7 @@
       <c r="BH3" s="2"/>
       <c r="BI3" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ3" s="8" t="s">
         <v>327</v>
@@ -3127,7 +3127,7 @@
       <c r="BH4" s="2"/>
       <c r="BI4" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ4" s="8" t="s">
         <v>327</v>
@@ -3251,7 +3251,7 @@
       <c r="BH5" s="2"/>
       <c r="BI5" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ5" s="8" t="s">
         <v>327</v>
@@ -3379,7 +3379,7 @@
       <c r="BH6" s="2"/>
       <c r="BI6" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ6" s="8" t="s">
         <v>327</v>
@@ -3507,7 +3507,7 @@
       <c r="BH7" s="2"/>
       <c r="BI7" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ7" s="8" t="s">
         <v>327</v>
@@ -3636,7 +3636,7 @@
       <c r="BH8" s="2"/>
       <c r="BI8" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ8" s="8" t="s">
         <v>327</v>
@@ -3761,7 +3761,7 @@
       <c r="BH9" s="2"/>
       <c r="BI9" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ9" s="8" t="s">
         <v>327</v>
@@ -3866,7 +3866,7 @@
       <c r="BH10" s="2"/>
       <c r="BI10" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ10" s="8" t="s">
         <v>327</v>
@@ -3987,7 +3987,7 @@
       <c r="BH11" s="2"/>
       <c r="BI11" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ11" s="8" t="s">
         <v>327</v>
@@ -4114,7 +4114,7 @@
       <c r="BH12" s="2"/>
       <c r="BI12" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ12" s="8" t="s">
         <v>327</v>
@@ -4241,7 +4241,7 @@
       <c r="BH13" s="2"/>
       <c r="BI13" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ13" s="8" t="s">
         <v>327</v>
@@ -4370,7 +4370,7 @@
       <c r="BH14" s="2"/>
       <c r="BI14" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ14" s="8" t="s">
         <v>327</v>
@@ -4495,7 +4495,7 @@
       <c r="BH15" s="2"/>
       <c r="BI15" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ15" s="8" t="s">
         <v>327</v>
@@ -4620,7 +4620,7 @@
       <c r="BH16" s="2"/>
       <c r="BI16" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ16" s="8" t="s">
         <v>327</v>
@@ -4749,7 +4749,7 @@
       <c r="BH17" s="2"/>
       <c r="BI17" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ17" s="8" t="s">
         <v>327</v>
@@ -4878,7 +4878,7 @@
       <c r="BH18" s="2"/>
       <c r="BI18" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ18" s="8" t="s">
         <v>327</v>
@@ -4999,7 +4999,7 @@
       <c r="BH19" s="2"/>
       <c r="BI19" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ19" s="8" t="s">
         <v>327</v>
@@ -5126,7 +5126,7 @@
       <c r="BH20" s="2"/>
       <c r="BI20" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ20" s="8" t="s">
         <v>327</v>
@@ -5255,7 +5255,7 @@
       <c r="BH21" s="2"/>
       <c r="BI21" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ21" s="8" t="s">
         <v>327</v>
@@ -5382,7 +5382,7 @@
       <c r="BH22" s="2"/>
       <c r="BI22" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ22" s="8" t="s">
         <v>327</v>
@@ -5511,7 +5511,7 @@
       <c r="BH23" s="2"/>
       <c r="BI23" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ23" s="8" t="s">
         <v>327</v>
@@ -5636,7 +5636,7 @@
       <c r="BH24" s="2"/>
       <c r="BI24" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ24" s="8" t="s">
         <v>327</v>
@@ -5757,7 +5757,7 @@
       <c r="BH25" s="2"/>
       <c r="BI25" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ25" s="8" t="s">
         <v>327</v>
@@ -5884,7 +5884,7 @@
       <c r="BH26" s="2"/>
       <c r="BI26" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ26" s="8" t="s">
         <v>327</v>
@@ -6013,7 +6013,7 @@
       <c r="BH27" s="2"/>
       <c r="BI27" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ27" s="8" t="s">
         <v>327</v>
@@ -6138,7 +6138,7 @@
       <c r="BH28" s="2"/>
       <c r="BI28" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ28" s="8" t="s">
         <v>327</v>
@@ -6265,7 +6265,7 @@
       <c r="BH29" s="2"/>
       <c r="BI29" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ29" s="8" t="s">
         <v>327</v>
@@ -6390,7 +6390,7 @@
       <c r="BH30" s="2"/>
       <c r="BI30" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ30" s="8" t="s">
         <v>327</v>
@@ -6517,7 +6517,7 @@
       <c r="BH31" s="2"/>
       <c r="BI31" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ31" s="8" t="s">
         <v>327</v>
@@ -6644,7 +6644,7 @@
       <c r="BH32" s="2"/>
       <c r="BI32" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ32" s="8" t="s">
         <v>327</v>
@@ -6771,7 +6771,7 @@
       <c r="BH33" s="2"/>
       <c r="BI33" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ33" s="8" t="s">
         <v>327</v>
@@ -6912,7 +6912,7 @@
       <c r="BH34" s="2"/>
       <c r="BI34" s="18">
         <f t="shared" ref="BI34:BI65" ca="1" si="1">NOW()</f>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ34" s="8" t="s">
         <v>327</v>
@@ -7033,7 +7033,7 @@
       <c r="BH35" s="2"/>
       <c r="BI35" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ35" s="8" t="s">
         <v>327</v>
@@ -7158,7 +7158,7 @@
       <c r="BH36" s="2"/>
       <c r="BI36" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ36" s="8" t="s">
         <v>327</v>
@@ -7289,7 +7289,7 @@
       <c r="BH37" s="2"/>
       <c r="BI37" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ37" s="8" t="s">
         <v>327</v>
@@ -7416,7 +7416,7 @@
       <c r="BH38" s="2"/>
       <c r="BI38" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ38" s="8" t="s">
         <v>327</v>
@@ -7545,7 +7545,7 @@
       <c r="BH39" s="2"/>
       <c r="BI39" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ39" s="8" t="s">
         <v>327</v>
@@ -7674,7 +7674,7 @@
       <c r="BH40" s="2"/>
       <c r="BI40" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ40" s="8" t="s">
         <v>327</v>
@@ -7801,7 +7801,7 @@
       <c r="BH41" s="2"/>
       <c r="BI41" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ41" s="8" t="s">
         <v>327</v>
@@ -7938,7 +7938,7 @@
       <c r="BH42" s="2"/>
       <c r="BI42" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ42" s="8" t="s">
         <v>327</v>
@@ -8057,7 +8057,7 @@
       <c r="BH43" s="2"/>
       <c r="BI43" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ43" s="8" t="s">
         <v>327</v>
@@ -8177,7 +8177,7 @@
       <c r="BH44" s="2"/>
       <c r="BI44" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ44" s="8" t="s">
         <v>327</v>
@@ -8299,7 +8299,7 @@
       <c r="BH45" s="2"/>
       <c r="BI45" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ45" s="8" t="s">
         <v>327</v>
@@ -8419,7 +8419,7 @@
       <c r="BH46" s="2"/>
       <c r="BI46" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ46" s="8" t="s">
         <v>327</v>
@@ -8541,7 +8541,7 @@
       <c r="BH47" s="2"/>
       <c r="BI47" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ47" s="8" t="s">
         <v>327</v>
@@ -8661,7 +8661,7 @@
       <c r="BH48" s="2"/>
       <c r="BI48" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ48" s="8" t="s">
         <v>327</v>
@@ -8783,7 +8783,7 @@
       <c r="BH49" s="2"/>
       <c r="BI49" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ49" s="8" t="s">
         <v>327</v>
@@ -8905,7 +8905,7 @@
       <c r="BH50" s="2"/>
       <c r="BI50" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ50" s="8" t="s">
         <v>327</v>
@@ -9025,7 +9025,7 @@
       <c r="BH51" s="2"/>
       <c r="BI51" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ51" s="8" t="s">
         <v>327</v>
@@ -9147,7 +9147,7 @@
       <c r="BH52" s="2"/>
       <c r="BI52" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ52" s="8" t="s">
         <v>327</v>
@@ -9269,7 +9269,7 @@
       <c r="BH53" s="2"/>
       <c r="BI53" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ53" s="8" t="s">
         <v>327</v>
@@ -9395,7 +9395,7 @@
       </c>
       <c r="BI54" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ54" s="8" t="s">
         <v>327</v>
@@ -9522,7 +9522,7 @@
       <c r="BH55" s="24"/>
       <c r="BI55" s="24">
         <f t="shared" ca="1" si="1"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ55" s="8" t="s">
         <v>327</v>
@@ -9659,7 +9659,7 @@
       <c r="BH56" s="24"/>
       <c r="BI56" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ56" s="8" t="s">
         <v>327</v>
@@ -9781,7 +9781,7 @@
       <c r="BH57" s="2"/>
       <c r="BI57" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ57" s="8" t="s">
         <v>327</v>
@@ -9901,7 +9901,7 @@
       <c r="BH58" s="2"/>
       <c r="BI58" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ58" s="8" t="s">
         <v>327</v>
@@ -10023,7 +10023,7 @@
       <c r="BH59" s="2"/>
       <c r="BI59" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ59" s="8" t="s">
         <v>327</v>
@@ -10160,7 +10160,7 @@
       <c r="BH60" s="2"/>
       <c r="BI60" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ60" s="8" t="s">
         <v>327</v>
@@ -10275,7 +10275,7 @@
       <c r="BH61" s="2"/>
       <c r="BI61" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ61" s="8" t="s">
         <v>327</v>
@@ -10395,7 +10395,7 @@
       <c r="BH62" s="2"/>
       <c r="BI62" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ62" s="8" t="s">
         <v>327</v>
@@ -10515,7 +10515,7 @@
       <c r="BH63" s="2"/>
       <c r="BI63" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ63" s="8" t="s">
         <v>327</v>
@@ -10637,7 +10637,7 @@
       <c r="BH64" s="2"/>
       <c r="BI64" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ64" s="8" t="s">
         <v>327</v>
@@ -10762,7 +10762,7 @@
       <c r="BH65" s="2"/>
       <c r="BI65" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ65" s="8" t="s">
         <v>327</v>
@@ -10882,7 +10882,7 @@
       <c r="BH66" s="2"/>
       <c r="BI66" s="18">
         <f t="shared" ref="BI66:BI71" ca="1" si="2">NOW()</f>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ66" s="8" t="s">
         <v>327</v>
@@ -11019,7 +11019,7 @@
       <c r="BH67" s="2"/>
       <c r="BI67" s="18">
         <f t="shared" ca="1" si="2"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ67" s="8" t="s">
         <v>327</v>
@@ -11132,7 +11132,7 @@
       <c r="BH68" s="2"/>
       <c r="BI68" s="18">
         <f t="shared" ca="1" si="2"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ68" s="8" t="s">
         <v>327</v>
@@ -11249,7 +11249,7 @@
       <c r="BH69" s="2"/>
       <c r="BI69" s="18">
         <f t="shared" ca="1" si="2"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ69" s="8" t="s">
         <v>327</v>
@@ -11369,7 +11369,7 @@
       <c r="BH70" s="19"/>
       <c r="BI70" s="33">
         <f t="shared" ca="1" si="2"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ70" s="34" t="s">
         <v>327</v>
@@ -11498,7 +11498,7 @@
       <c r="BH71" s="19"/>
       <c r="BI71" s="33">
         <f t="shared" ca="1" si="2"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ71" s="34" t="s">
         <v>327</v>
@@ -11616,7 +11616,7 @@
       <c r="BH72" s="2"/>
       <c r="BI72" s="18">
         <f t="shared" ref="BI72:BI82" ca="1" si="3">NOW()</f>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ72" s="8" t="s">
         <v>327</v>
@@ -11713,7 +11713,7 @@
       <c r="BH73" s="2"/>
       <c r="BI73" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ73" s="8" t="s">
         <v>327</v>
@@ -11833,7 +11833,7 @@
       <c r="BH74" s="2"/>
       <c r="BI74" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ74" s="8" t="s">
         <v>327</v>
@@ -11946,7 +11946,7 @@
       <c r="BH75" s="2"/>
       <c r="BI75" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ75" s="8" t="s">
         <v>327</v>
@@ -12040,7 +12040,7 @@
       <c r="BH76" s="2"/>
       <c r="BI76" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ76" s="8" t="s">
         <v>327</v>
@@ -12175,7 +12175,7 @@
       <c r="BH77" s="2"/>
       <c r="BI77" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ77" s="8" t="s">
         <v>327</v>
@@ -12267,7 +12267,7 @@
       <c r="BH78" s="2"/>
       <c r="BI78" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ78" s="8" t="s">
         <v>327</v>
@@ -12385,7 +12385,7 @@
       <c r="BH79" s="2"/>
       <c r="BI79" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ79" s="8" t="s">
         <v>327</v>
@@ -12479,7 +12479,7 @@
       <c r="BH80" s="2"/>
       <c r="BI80" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ80" s="8" t="s">
         <v>327</v>
@@ -12613,7 +12613,7 @@
       </c>
       <c r="BI81" s="33">
         <f t="shared" ca="1" si="3"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ81" s="34" t="s">
         <v>327</v>
@@ -12624,10 +12624,10 @@
         <v>625</v>
       </c>
       <c r="B82" s="32" t="s">
+        <v>627</v>
+      </c>
+      <c r="C82" s="32" t="s">
         <v>626</v>
-      </c>
-      <c r="C82" s="32" t="s">
-        <v>627</v>
       </c>
       <c r="D82" s="32" t="s">
         <v>34</v>
@@ -12712,7 +12712,7 @@
       <c r="BH82" s="19"/>
       <c r="BI82" s="33">
         <f t="shared" ca="1" si="3"/>
-        <v>44166.638098263888</v>
+        <v>44167.426704745369</v>
       </c>
       <c r="BJ82" s="34" t="s">
         <v>327</v>

</xml_diff>

<commit_message>
Update 360G Grants data
Add missing July 2020 grants
</commit_message>
<xml_diff>
--- a/open/grants.xlsx
+++ b/open/grants.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/westsi/Documents/GitHub/zing/open/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F0A06F-1FBD-5848-849D-5C230E87E03A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C8BA1C-F9CD-7B4F-BFD2-3F965DC0DE6B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="460" yWindow="700" windowWidth="33140" windowHeight="20300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="grants" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">grants!$A$1:$BJ$83</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">grants!$A$1:$BJ$87</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2068" uniqueCount="636">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2149" uniqueCount="641">
   <si>
     <t>Identifier</t>
   </si>
@@ -1977,6 +1977,22 @@
   </si>
   <si>
     <t>Funding and in-kind digital support toward the roll out of a digital transformation programme. This strand covers the auditing of the FEA membership, regularly gathering membership data for both the secretariat and members, and the piloting of tools to effectively leverage this data, aiming to improve collaboration across the membership. This is core funding toward covering the role of a digital project manager, and the piloting of tools with the membership.</t>
+  </si>
+  <si>
+    <t>360G-zing-91</t>
+  </si>
+  <si>
+    <t>360G-zing-92</t>
+  </si>
+  <si>
+    <t>360G-zing-93</t>
+  </si>
+  <si>
+    <t>Funding toward prototyping solutions identified through the "My Best Life" digital priorities research</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paul Hamlyn Foundation are covering Phase 2 of the MyBestLife project, running design sprints with young people from the user base of UK Youth, The Mix, Leap and Princes Trust. Founders and Coders are the digital partner on this project, and the next phase will be to prototype the most compelling solutions and build through to MVP. This funding is toward the development of these prototypes.
+</t>
   </si>
 </sst>
 </file>
@@ -2090,7 +2106,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2204,6 +2220,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2524,7 +2543,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:BJ84"/>
+  <dimension ref="A1:BJ88"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="120" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -2572,8 +2591,10 @@
     <col min="37" max="38" width="37.5" style="6" hidden="1" customWidth="1"/>
     <col min="39" max="42" width="37.5" style="6" customWidth="1"/>
     <col min="43" max="44" width="37.5" style="6" hidden="1" customWidth="1"/>
-    <col min="45" max="48" width="37.5" style="6" customWidth="1"/>
-    <col min="49" max="50" width="37.5" style="6" hidden="1" customWidth="1"/>
+    <col min="45" max="47" width="37.5" style="6" customWidth="1"/>
+    <col min="48" max="48" width="34" style="6" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="37.5" style="6" customWidth="1"/>
+    <col min="50" max="50" width="31" style="6" bestFit="1" customWidth="1"/>
     <col min="51" max="52" width="37.5" style="6" customWidth="1"/>
     <col min="53" max="53" width="19" style="6" customWidth="1"/>
     <col min="54" max="54" width="16.83203125" style="6" customWidth="1"/>
@@ -2898,7 +2919,7 @@
       <c r="BH2" s="2"/>
       <c r="BI2" s="18">
         <f t="shared" ref="BI2:BI33" ca="1" si="0">NOW()</f>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ2" s="8" t="s">
         <v>327</v>
@@ -3023,7 +3044,7 @@
       <c r="BH3" s="2"/>
       <c r="BI3" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ3" s="8" t="s">
         <v>327</v>
@@ -3151,7 +3172,7 @@
       <c r="BH4" s="2"/>
       <c r="BI4" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ4" s="8" t="s">
         <v>327</v>
@@ -3275,7 +3296,7 @@
       <c r="BH5" s="2"/>
       <c r="BI5" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ5" s="8" t="s">
         <v>327</v>
@@ -3403,7 +3424,7 @@
       <c r="BH6" s="2"/>
       <c r="BI6" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ6" s="8" t="s">
         <v>327</v>
@@ -3531,7 +3552,7 @@
       <c r="BH7" s="2"/>
       <c r="BI7" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ7" s="8" t="s">
         <v>327</v>
@@ -3660,7 +3681,7 @@
       <c r="BH8" s="2"/>
       <c r="BI8" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ8" s="8" t="s">
         <v>327</v>
@@ -3785,7 +3806,7 @@
       <c r="BH9" s="2"/>
       <c r="BI9" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ9" s="8" t="s">
         <v>327</v>
@@ -3890,7 +3911,7 @@
       <c r="BH10" s="2"/>
       <c r="BI10" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ10" s="8" t="s">
         <v>327</v>
@@ -4011,7 +4032,7 @@
       <c r="BH11" s="2"/>
       <c r="BI11" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ11" s="8" t="s">
         <v>327</v>
@@ -4138,7 +4159,7 @@
       <c r="BH12" s="2"/>
       <c r="BI12" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ12" s="8" t="s">
         <v>327</v>
@@ -4265,7 +4286,7 @@
       <c r="BH13" s="2"/>
       <c r="BI13" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ13" s="8" t="s">
         <v>327</v>
@@ -4394,7 +4415,7 @@
       <c r="BH14" s="2"/>
       <c r="BI14" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ14" s="8" t="s">
         <v>327</v>
@@ -4519,7 +4540,7 @@
       <c r="BH15" s="2"/>
       <c r="BI15" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ15" s="8" t="s">
         <v>327</v>
@@ -4644,7 +4665,7 @@
       <c r="BH16" s="2"/>
       <c r="BI16" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ16" s="8" t="s">
         <v>327</v>
@@ -4773,7 +4794,7 @@
       <c r="BH17" s="2"/>
       <c r="BI17" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ17" s="8" t="s">
         <v>327</v>
@@ -4902,7 +4923,7 @@
       <c r="BH18" s="2"/>
       <c r="BI18" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ18" s="8" t="s">
         <v>327</v>
@@ -5023,7 +5044,7 @@
       <c r="BH19" s="2"/>
       <c r="BI19" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ19" s="8" t="s">
         <v>327</v>
@@ -5150,7 +5171,7 @@
       <c r="BH20" s="2"/>
       <c r="BI20" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ20" s="8" t="s">
         <v>327</v>
@@ -5279,7 +5300,7 @@
       <c r="BH21" s="2"/>
       <c r="BI21" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ21" s="8" t="s">
         <v>327</v>
@@ -5406,7 +5427,7 @@
       <c r="BH22" s="2"/>
       <c r="BI22" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ22" s="8" t="s">
         <v>327</v>
@@ -5535,7 +5556,7 @@
       <c r="BH23" s="2"/>
       <c r="BI23" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ23" s="8" t="s">
         <v>327</v>
@@ -5660,7 +5681,7 @@
       <c r="BH24" s="2"/>
       <c r="BI24" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ24" s="8" t="s">
         <v>327</v>
@@ -5781,7 +5802,7 @@
       <c r="BH25" s="2"/>
       <c r="BI25" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ25" s="8" t="s">
         <v>327</v>
@@ -5908,7 +5929,7 @@
       <c r="BH26" s="2"/>
       <c r="BI26" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ26" s="8" t="s">
         <v>327</v>
@@ -6037,7 +6058,7 @@
       <c r="BH27" s="2"/>
       <c r="BI27" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ27" s="8" t="s">
         <v>327</v>
@@ -6162,7 +6183,7 @@
       <c r="BH28" s="2"/>
       <c r="BI28" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ28" s="8" t="s">
         <v>327</v>
@@ -6289,7 +6310,7 @@
       <c r="BH29" s="2"/>
       <c r="BI29" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ29" s="8" t="s">
         <v>327</v>
@@ -6414,7 +6435,7 @@
       <c r="BH30" s="2"/>
       <c r="BI30" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ30" s="8" t="s">
         <v>327</v>
@@ -6541,7 +6562,7 @@
       <c r="BH31" s="2"/>
       <c r="BI31" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ31" s="8" t="s">
         <v>327</v>
@@ -6668,7 +6689,7 @@
       <c r="BH32" s="2"/>
       <c r="BI32" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ32" s="8" t="s">
         <v>327</v>
@@ -6795,7 +6816,7 @@
       <c r="BH33" s="2"/>
       <c r="BI33" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ33" s="8" t="s">
         <v>327</v>
@@ -6936,7 +6957,7 @@
       <c r="BH34" s="2"/>
       <c r="BI34" s="18">
         <f t="shared" ref="BI34:BI65" ca="1" si="1">NOW()</f>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ34" s="8" t="s">
         <v>327</v>
@@ -7057,7 +7078,7 @@
       <c r="BH35" s="2"/>
       <c r="BI35" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ35" s="8" t="s">
         <v>327</v>
@@ -7182,7 +7203,7 @@
       <c r="BH36" s="2"/>
       <c r="BI36" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ36" s="8" t="s">
         <v>327</v>
@@ -7313,7 +7334,7 @@
       <c r="BH37" s="2"/>
       <c r="BI37" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ37" s="8" t="s">
         <v>327</v>
@@ -7440,7 +7461,7 @@
       <c r="BH38" s="2"/>
       <c r="BI38" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ38" s="8" t="s">
         <v>327</v>
@@ -7569,7 +7590,7 @@
       <c r="BH39" s="2"/>
       <c r="BI39" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ39" s="8" t="s">
         <v>327</v>
@@ -7698,7 +7719,7 @@
       <c r="BH40" s="2"/>
       <c r="BI40" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ40" s="8" t="s">
         <v>327</v>
@@ -7825,7 +7846,7 @@
       <c r="BH41" s="2"/>
       <c r="BI41" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ41" s="8" t="s">
         <v>327</v>
@@ -7962,7 +7983,7 @@
       <c r="BH42" s="2"/>
       <c r="BI42" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ42" s="8" t="s">
         <v>327</v>
@@ -8081,7 +8102,7 @@
       <c r="BH43" s="2"/>
       <c r="BI43" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ43" s="8" t="s">
         <v>327</v>
@@ -8201,7 +8222,7 @@
       <c r="BH44" s="2"/>
       <c r="BI44" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ44" s="8" t="s">
         <v>327</v>
@@ -8323,7 +8344,7 @@
       <c r="BH45" s="2"/>
       <c r="BI45" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ45" s="8" t="s">
         <v>327</v>
@@ -8443,7 +8464,7 @@
       <c r="BH46" s="2"/>
       <c r="BI46" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ46" s="8" t="s">
         <v>327</v>
@@ -8565,7 +8586,7 @@
       <c r="BH47" s="2"/>
       <c r="BI47" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ47" s="8" t="s">
         <v>327</v>
@@ -8685,7 +8706,7 @@
       <c r="BH48" s="2"/>
       <c r="BI48" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ48" s="8" t="s">
         <v>327</v>
@@ -8807,7 +8828,7 @@
       <c r="BH49" s="2"/>
       <c r="BI49" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ49" s="8" t="s">
         <v>327</v>
@@ -8929,7 +8950,7 @@
       <c r="BH50" s="2"/>
       <c r="BI50" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ50" s="8" t="s">
         <v>327</v>
@@ -9049,7 +9070,7 @@
       <c r="BH51" s="2"/>
       <c r="BI51" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ51" s="8" t="s">
         <v>327</v>
@@ -9171,7 +9192,7 @@
       <c r="BH52" s="2"/>
       <c r="BI52" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ52" s="8" t="s">
         <v>327</v>
@@ -9293,7 +9314,7 @@
       <c r="BH53" s="2"/>
       <c r="BI53" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ53" s="8" t="s">
         <v>327</v>
@@ -9419,7 +9440,7 @@
       </c>
       <c r="BI54" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ54" s="8" t="s">
         <v>327</v>
@@ -9546,7 +9567,7 @@
       <c r="BH55" s="24"/>
       <c r="BI55" s="24">
         <f t="shared" ca="1" si="1"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ55" s="8" t="s">
         <v>327</v>
@@ -9683,7 +9704,7 @@
       <c r="BH56" s="24"/>
       <c r="BI56" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ56" s="8" t="s">
         <v>327</v>
@@ -9805,7 +9826,7 @@
       <c r="BH57" s="2"/>
       <c r="BI57" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ57" s="8" t="s">
         <v>327</v>
@@ -9925,7 +9946,7 @@
       <c r="BH58" s="2"/>
       <c r="BI58" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ58" s="8" t="s">
         <v>327</v>
@@ -10047,7 +10068,7 @@
       <c r="BH59" s="2"/>
       <c r="BI59" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ59" s="8" t="s">
         <v>327</v>
@@ -10184,7 +10205,7 @@
       <c r="BH60" s="2"/>
       <c r="BI60" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ60" s="8" t="s">
         <v>327</v>
@@ -10299,7 +10320,7 @@
       <c r="BH61" s="2"/>
       <c r="BI61" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ61" s="8" t="s">
         <v>327</v>
@@ -10419,7 +10440,7 @@
       <c r="BH62" s="2"/>
       <c r="BI62" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ62" s="8" t="s">
         <v>327</v>
@@ -10539,7 +10560,7 @@
       <c r="BH63" s="2"/>
       <c r="BI63" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ63" s="8" t="s">
         <v>327</v>
@@ -10661,7 +10682,7 @@
       <c r="BH64" s="2"/>
       <c r="BI64" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ64" s="8" t="s">
         <v>327</v>
@@ -10786,7 +10807,7 @@
       <c r="BH65" s="2"/>
       <c r="BI65" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ65" s="8" t="s">
         <v>327</v>
@@ -10908,7 +10929,7 @@
       <c r="BH66" s="2"/>
       <c r="BI66" s="18">
         <f t="shared" ref="BI66:BI71" ca="1" si="2">NOW()</f>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ66" s="8" t="s">
         <v>327</v>
@@ -11045,7 +11066,7 @@
       <c r="BH67" s="2"/>
       <c r="BI67" s="18">
         <f t="shared" ca="1" si="2"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ67" s="8" t="s">
         <v>327</v>
@@ -11160,7 +11181,7 @@
       <c r="BH68" s="2"/>
       <c r="BI68" s="18">
         <f t="shared" ca="1" si="2"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ68" s="8" t="s">
         <v>327</v>
@@ -11279,7 +11300,7 @@
       <c r="BH69" s="2"/>
       <c r="BI69" s="18">
         <f t="shared" ca="1" si="2"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ69" s="8" t="s">
         <v>327</v>
@@ -11401,7 +11422,7 @@
       <c r="BH70" s="19"/>
       <c r="BI70" s="33">
         <f t="shared" ca="1" si="2"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ70" s="34" t="s">
         <v>327</v>
@@ -11532,7 +11553,7 @@
       <c r="BH71" s="19"/>
       <c r="BI71" s="33">
         <f t="shared" ca="1" si="2"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ71" s="34" t="s">
         <v>327</v>
@@ -11651,8 +11672,8 @@
       </c>
       <c r="BH72" s="2"/>
       <c r="BI72" s="18">
-        <f t="shared" ref="BI72:BI84" ca="1" si="3">NOW()</f>
-        <v>44224.780693518522</v>
+        <f t="shared" ref="BI72:BI87" ca="1" si="3">NOW()</f>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ72" s="8" t="s">
         <v>327</v>
@@ -11752,7 +11773,7 @@
       <c r="BH73" s="2"/>
       <c r="BI73" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ73" s="8" t="s">
         <v>327</v>
@@ -11874,7 +11895,7 @@
       <c r="BH74" s="2"/>
       <c r="BI74" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ74" s="8" t="s">
         <v>327</v>
@@ -11987,7 +12008,7 @@
       <c r="BH75" s="2"/>
       <c r="BI75" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ75" s="8" t="s">
         <v>327</v>
@@ -12081,7 +12102,7 @@
       <c r="BH76" s="2"/>
       <c r="BI76" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ76" s="8" t="s">
         <v>327</v>
@@ -12216,7 +12237,7 @@
       <c r="BH77" s="2"/>
       <c r="BI77" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ77" s="8" t="s">
         <v>327</v>
@@ -12308,7 +12329,7 @@
       <c r="BH78" s="2"/>
       <c r="BI78" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ78" s="8" t="s">
         <v>327</v>
@@ -12426,7 +12447,7 @@
       <c r="BH79" s="2"/>
       <c r="BI79" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ79" s="8" t="s">
         <v>327</v>
@@ -12520,7 +12541,7 @@
       <c r="BH80" s="2"/>
       <c r="BI80" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ80" s="8" t="s">
         <v>327</v>
@@ -12654,7 +12675,7 @@
       </c>
       <c r="BI81" s="33">
         <f t="shared" ca="1" si="3"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ81" s="34" t="s">
         <v>327</v>
@@ -12753,7 +12774,7 @@
       <c r="BH82" s="19"/>
       <c r="BI82" s="33">
         <f t="shared" ca="1" si="3"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ82" s="34" t="s">
         <v>327</v>
@@ -12873,7 +12894,7 @@
       <c r="BH83" s="2"/>
       <c r="BI83" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ83" s="8" t="s">
         <v>327</v>
@@ -12970,14 +12991,445 @@
       <c r="BH84" s="2"/>
       <c r="BI84" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44224.780693518522</v>
+        <v>44252.634867939814</v>
       </c>
       <c r="BJ84" s="8" t="s">
         <v>327</v>
       </c>
     </row>
+    <row r="85" spans="1:62" ht="28" x14ac:dyDescent="0.15">
+      <c r="A85" s="2" t="s">
+        <v>636</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>529</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E85" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="F85" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="G85" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="H85" s="16">
+        <v>44013</v>
+      </c>
+      <c r="I85" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="J85" s="16">
+        <v>44013</v>
+      </c>
+      <c r="K85" s="16">
+        <v>44378</v>
+      </c>
+      <c r="L85" s="16"/>
+      <c r="M85" s="2">
+        <v>12</v>
+      </c>
+      <c r="N85" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="O85" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="P85" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q85" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="R85" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="S85" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="T85" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="U85" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="V85" s="8" t="s">
+        <v>323</v>
+      </c>
+      <c r="W85" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="X85" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="Y85" s="2"/>
+      <c r="Z85" s="2"/>
+      <c r="AC85" s="2" t="s">
+        <v>561</v>
+      </c>
+      <c r="AD85" s="2" t="s">
+        <v>562</v>
+      </c>
+      <c r="AE85" s="2"/>
+      <c r="AF85" s="2"/>
+      <c r="AG85" s="2"/>
+      <c r="AH85" s="2"/>
+      <c r="AI85" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="AJ85" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="AK85" s="2"/>
+      <c r="AL85" s="2"/>
+      <c r="AO85" s="2" t="s">
+        <v>535</v>
+      </c>
+      <c r="AP85" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="AQ85" s="2"/>
+      <c r="AR85" s="2"/>
+      <c r="AS85" s="2"/>
+      <c r="AT85" s="2"/>
+      <c r="AU85" s="2" t="s">
+        <v>581</v>
+      </c>
+      <c r="AV85" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="AW85" s="2"/>
+      <c r="AX85" s="2"/>
+      <c r="AY85" s="2"/>
+      <c r="AZ85" s="2"/>
+      <c r="BA85" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="BB85" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="BC85" s="2"/>
+      <c r="BD85" s="2"/>
+      <c r="BE85" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="BF85" s="2"/>
+      <c r="BG85" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="BH85" s="2"/>
+      <c r="BI85" s="18">
+        <f t="shared" ca="1" si="3"/>
+        <v>44252.634867939814</v>
+      </c>
+      <c r="BJ85" s="8" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="86" spans="1:62" ht="98" x14ac:dyDescent="0.15">
+      <c r="A86" s="2" t="s">
+        <v>637</v>
+      </c>
+      <c r="B86" s="39" t="s">
+        <v>639</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>640</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E86" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="F86" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="G86" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="H86" s="16">
+        <v>44013</v>
+      </c>
+      <c r="I86" s="9" t="s">
+        <v>370</v>
+      </c>
+      <c r="J86" s="16">
+        <v>44013</v>
+      </c>
+      <c r="K86" s="16">
+        <v>44378</v>
+      </c>
+      <c r="L86" s="16"/>
+      <c r="M86" s="2">
+        <v>12</v>
+      </c>
+      <c r="N86" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="O86" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="P86" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="Q86" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="R86" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="S86" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="T86" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="U86" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="V86" s="8" t="s">
+        <v>371</v>
+      </c>
+      <c r="W86" s="2" t="s">
+        <v>546</v>
+      </c>
+      <c r="X86" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="Y86" s="2"/>
+      <c r="Z86" s="2"/>
+      <c r="AA86" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="AC86" s="2"/>
+      <c r="AD86" s="2"/>
+      <c r="AE86" s="2"/>
+      <c r="AF86" s="2"/>
+      <c r="AG86" s="2"/>
+      <c r="AH86" s="2"/>
+      <c r="AK86" s="2"/>
+      <c r="AL86" s="2"/>
+      <c r="AO86" s="2"/>
+      <c r="AP86" s="2"/>
+      <c r="AQ86" s="2"/>
+      <c r="AR86" s="2"/>
+      <c r="AS86" s="2"/>
+      <c r="AT86" s="2"/>
+      <c r="AU86" s="2"/>
+      <c r="AV86" s="2"/>
+      <c r="AW86" s="2"/>
+      <c r="AX86" s="2"/>
+      <c r="AY86" s="2"/>
+      <c r="AZ86" s="2"/>
+      <c r="BA86" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="BB86" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="BC86" s="2"/>
+      <c r="BD86" s="2"/>
+      <c r="BE86" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="BF86" s="2"/>
+      <c r="BG86" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="BH86" s="2"/>
+      <c r="BI86" s="18">
+        <f t="shared" ca="1" si="3"/>
+        <v>44252.634867939814</v>
+      </c>
+      <c r="BJ86" s="8" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="87" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A87" s="2" t="s">
+        <v>638</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E87" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="F87" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="G87" s="2">
+        <v>35000</v>
+      </c>
+      <c r="H87" s="16">
+        <v>44013</v>
+      </c>
+      <c r="I87" s="8" t="s">
+        <v>434</v>
+      </c>
+      <c r="J87" s="16">
+        <v>44013</v>
+      </c>
+      <c r="K87" s="16">
+        <v>44378</v>
+      </c>
+      <c r="L87" s="16"/>
+      <c r="M87" s="2">
+        <v>12</v>
+      </c>
+      <c r="N87" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="O87" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="P87" s="25" t="s">
+        <v>385</v>
+      </c>
+      <c r="Q87" s="15" t="s">
+        <v>427</v>
+      </c>
+      <c r="R87" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="S87" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="T87" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="U87" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="V87" s="11" t="s">
+        <v>384</v>
+      </c>
+      <c r="W87" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="X87" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="Y87" s="2"/>
+      <c r="Z87" s="2"/>
+      <c r="AA87" s="6" t="s">
+        <v>530</v>
+      </c>
+      <c r="AC87" s="2"/>
+      <c r="AD87" s="2"/>
+      <c r="AE87" s="2"/>
+      <c r="AF87" s="2"/>
+      <c r="AK87" s="2"/>
+      <c r="AL87" s="2"/>
+      <c r="AM87" s="2"/>
+      <c r="AN87" s="2"/>
+      <c r="AO87" s="2"/>
+      <c r="AP87" s="2"/>
+      <c r="AQ87" s="2"/>
+      <c r="AR87" s="2"/>
+      <c r="AU87" s="2"/>
+      <c r="AV87" s="2"/>
+      <c r="AW87" s="2"/>
+      <c r="AX87" s="2"/>
+      <c r="AY87" s="4"/>
+      <c r="AZ87" s="2"/>
+      <c r="BA87" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="BB87" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="BE87" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="BF87" s="2"/>
+      <c r="BG87" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="BH87" s="2"/>
+      <c r="BI87" s="18">
+        <f t="shared" ca="1" si="3"/>
+        <v>44252.634867939814</v>
+      </c>
+      <c r="BJ87" s="8" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="88" spans="1:62" ht="13" x14ac:dyDescent="0.15">
+      <c r="A88" s="2"/>
+      <c r="B88" s="3"/>
+      <c r="C88" s="2"/>
+      <c r="D88" s="2"/>
+      <c r="E88" s="15"/>
+      <c r="F88" s="15"/>
+      <c r="G88" s="15"/>
+      <c r="H88" s="16"/>
+      <c r="I88" s="8"/>
+      <c r="J88" s="16"/>
+      <c r="K88" s="16"/>
+      <c r="L88" s="16"/>
+      <c r="M88" s="2"/>
+      <c r="N88" s="2"/>
+      <c r="O88" s="3"/>
+      <c r="P88" s="15"/>
+      <c r="Q88" s="15"/>
+      <c r="R88" s="2"/>
+      <c r="S88" s="2"/>
+      <c r="T88" s="2"/>
+      <c r="U88" s="3"/>
+      <c r="V88" s="8"/>
+      <c r="W88" s="2"/>
+      <c r="X88" s="2"/>
+      <c r="Y88" s="2"/>
+      <c r="Z88" s="2"/>
+      <c r="AC88" s="2"/>
+      <c r="AD88" s="2"/>
+      <c r="AE88" s="2"/>
+      <c r="AF88" s="2"/>
+      <c r="AG88" s="2"/>
+      <c r="AH88" s="2"/>
+      <c r="AI88" s="2"/>
+      <c r="AJ88" s="2"/>
+      <c r="AK88" s="2"/>
+      <c r="AL88" s="2"/>
+      <c r="AO88" s="2"/>
+      <c r="AP88" s="2"/>
+      <c r="AQ88" s="2"/>
+      <c r="AR88" s="2"/>
+      <c r="AS88" s="2"/>
+      <c r="AT88" s="2"/>
+      <c r="AU88" s="2"/>
+      <c r="AV88" s="2"/>
+      <c r="AW88" s="2"/>
+      <c r="AX88" s="2"/>
+      <c r="AY88" s="2"/>
+      <c r="AZ88" s="2"/>
+      <c r="BA88" s="2"/>
+      <c r="BB88" s="2"/>
+      <c r="BC88" s="2"/>
+      <c r="BD88" s="2"/>
+      <c r="BE88" s="2"/>
+      <c r="BF88" s="2"/>
+      <c r="BG88" s="4"/>
+      <c r="BH88" s="2"/>
+      <c r="BI88" s="18"/>
+      <c r="BJ88" s="8"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:BJ83" xr:uid="{AE487DEF-5BC5-C74D-81B1-9FC54E50B3DD}"/>
+  <autoFilter ref="A1:BJ87" xr:uid="{AE487DEF-5BC5-C74D-81B1-9FC54E50B3DD}"/>
   <phoneticPr fontId="12" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="BJ2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
@@ -13110,8 +13562,15 @@
     <hyperlink ref="I84" r:id="rId128" xr:uid="{021049B8-74B1-2F4E-9BE3-34B3D0F29891}"/>
     <hyperlink ref="V84" r:id="rId129" xr:uid="{C0BA382D-238F-AB46-9209-E01F48AA4036}"/>
     <hyperlink ref="BJ84" r:id="rId130" xr:uid="{DF83E030-E0B8-6540-8979-AD5419CC6E91}"/>
+    <hyperlink ref="I85" r:id="rId131" xr:uid="{A22D5BA3-93AA-6E49-B140-5E9A5C1BCC59}"/>
+    <hyperlink ref="V85" r:id="rId132" xr:uid="{4CFF7C26-D875-C543-AF8C-533BF0C00811}"/>
+    <hyperlink ref="BJ85" r:id="rId133" xr:uid="{59EF6F88-AF4C-3B49-9C21-B32B62F38BB2}"/>
+    <hyperlink ref="V86" r:id="rId134" xr:uid="{93531427-15A7-614E-A75C-3B54E973B5A4}"/>
+    <hyperlink ref="BJ86" r:id="rId135" xr:uid="{A61E0B48-7D1E-9744-9E44-3CFA56C4323E}"/>
+    <hyperlink ref="I87" r:id="rId136" xr:uid="{0C3AF352-EF9A-EA45-B5C8-DFCD5AB4D933}"/>
+    <hyperlink ref="BJ87" r:id="rId137" xr:uid="{54024D96-B6A6-BA4E-89A9-15C22D785419}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId131"/>
+  <legacyDrawing r:id="rId138"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Publish Lily-Jo Project grant data
</commit_message>
<xml_diff>
--- a/open/grants.xlsx
+++ b/open/grants.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/westsi/Documents/GitHub/zing/open/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C8BA1C-F9CD-7B4F-BFD2-3F965DC0DE6B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4650C152-0A1D-BE41-9CBA-C5551616D1EE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="460" yWindow="700" windowWidth="33140" windowHeight="20300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2149" uniqueCount="641">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2171" uniqueCount="652">
   <si>
     <t>Identifier</t>
   </si>
@@ -1993,6 +1993,39 @@
   <si>
     <t xml:space="preserve">Paul Hamlyn Foundation are covering Phase 2 of the MyBestLife project, running design sprints with young people from the user base of UK Youth, The Mix, Leap and Princes Trust. Founders and Coders are the digital partner on this project, and the next phase will be to prototype the most compelling solutions and build through to MVP. This funding is toward the development of these prototypes.
 </t>
+  </si>
+  <si>
+    <t>360G-zing-94</t>
+  </si>
+  <si>
+    <t>Core funding toward curiculum development and growth</t>
+  </si>
+  <si>
+    <t>https://www.thelilyjoproject.com/</t>
+  </si>
+  <si>
+    <t>GB-COH-11603746</t>
+  </si>
+  <si>
+    <t>The Lily-Jo Project CIC</t>
+  </si>
+  <si>
+    <t>Core funding toward the completion of the Lily-Jo project's Key Stage weekly lesson curriculum; alignment to the new mandatory RSHE framework in schools; improving the student, teacher and parent user journeys through their website; and growth, including a campaign to coincide with Mental Health Awareness week.</t>
+  </si>
+  <si>
+    <t>11603746</t>
+  </si>
+  <si>
+    <t>7 Greenbank Avenue</t>
+  </si>
+  <si>
+    <t>Stockport</t>
+  </si>
+  <si>
+    <t>SK4 3BU</t>
+  </si>
+  <si>
+    <t>The Lily-Jo Project is devoted to eliminating the stigma surrounding mental health through music, digital resources, and community engagement. They believe that when exposed to the basic principles of mental health from an early age, kids are empowered to: be proactive about maintaining good mental health into adulthood, and ultimately reach their full potential and achieve their dreams. The Lily-Jo Project offers: a mix of paid and unpaid consistent digital resources in the form of educational curriculum, podcasts, blog articles, and videos; a way to connect with people through the power of music; and an in-person experience (when possible) through gigs and live workshops, enabling us to engage with the community and develop real-world relationships.</t>
   </si>
 </sst>
 </file>
@@ -2919,7 +2952,7 @@
       <c r="BH2" s="2"/>
       <c r="BI2" s="18">
         <f t="shared" ref="BI2:BI33" ca="1" si="0">NOW()</f>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ2" s="8" t="s">
         <v>327</v>
@@ -3044,7 +3077,7 @@
       <c r="BH3" s="2"/>
       <c r="BI3" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ3" s="8" t="s">
         <v>327</v>
@@ -3172,7 +3205,7 @@
       <c r="BH4" s="2"/>
       <c r="BI4" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ4" s="8" t="s">
         <v>327</v>
@@ -3296,7 +3329,7 @@
       <c r="BH5" s="2"/>
       <c r="BI5" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ5" s="8" t="s">
         <v>327</v>
@@ -3424,7 +3457,7 @@
       <c r="BH6" s="2"/>
       <c r="BI6" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ6" s="8" t="s">
         <v>327</v>
@@ -3552,7 +3585,7 @@
       <c r="BH7" s="2"/>
       <c r="BI7" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ7" s="8" t="s">
         <v>327</v>
@@ -3681,7 +3714,7 @@
       <c r="BH8" s="2"/>
       <c r="BI8" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ8" s="8" t="s">
         <v>327</v>
@@ -3806,7 +3839,7 @@
       <c r="BH9" s="2"/>
       <c r="BI9" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ9" s="8" t="s">
         <v>327</v>
@@ -3911,7 +3944,7 @@
       <c r="BH10" s="2"/>
       <c r="BI10" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ10" s="8" t="s">
         <v>327</v>
@@ -4032,7 +4065,7 @@
       <c r="BH11" s="2"/>
       <c r="BI11" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ11" s="8" t="s">
         <v>327</v>
@@ -4159,7 +4192,7 @@
       <c r="BH12" s="2"/>
       <c r="BI12" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ12" s="8" t="s">
         <v>327</v>
@@ -4286,7 +4319,7 @@
       <c r="BH13" s="2"/>
       <c r="BI13" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ13" s="8" t="s">
         <v>327</v>
@@ -4415,7 +4448,7 @@
       <c r="BH14" s="2"/>
       <c r="BI14" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ14" s="8" t="s">
         <v>327</v>
@@ -4540,7 +4573,7 @@
       <c r="BH15" s="2"/>
       <c r="BI15" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ15" s="8" t="s">
         <v>327</v>
@@ -4665,7 +4698,7 @@
       <c r="BH16" s="2"/>
       <c r="BI16" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ16" s="8" t="s">
         <v>327</v>
@@ -4794,7 +4827,7 @@
       <c r="BH17" s="2"/>
       <c r="BI17" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ17" s="8" t="s">
         <v>327</v>
@@ -4923,7 +4956,7 @@
       <c r="BH18" s="2"/>
       <c r="BI18" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ18" s="8" t="s">
         <v>327</v>
@@ -5044,7 +5077,7 @@
       <c r="BH19" s="2"/>
       <c r="BI19" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ19" s="8" t="s">
         <v>327</v>
@@ -5171,7 +5204,7 @@
       <c r="BH20" s="2"/>
       <c r="BI20" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ20" s="8" t="s">
         <v>327</v>
@@ -5300,7 +5333,7 @@
       <c r="BH21" s="2"/>
       <c r="BI21" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ21" s="8" t="s">
         <v>327</v>
@@ -5427,7 +5460,7 @@
       <c r="BH22" s="2"/>
       <c r="BI22" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ22" s="8" t="s">
         <v>327</v>
@@ -5556,7 +5589,7 @@
       <c r="BH23" s="2"/>
       <c r="BI23" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ23" s="8" t="s">
         <v>327</v>
@@ -5681,7 +5714,7 @@
       <c r="BH24" s="2"/>
       <c r="BI24" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ24" s="8" t="s">
         <v>327</v>
@@ -5802,7 +5835,7 @@
       <c r="BH25" s="2"/>
       <c r="BI25" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ25" s="8" t="s">
         <v>327</v>
@@ -5929,7 +5962,7 @@
       <c r="BH26" s="2"/>
       <c r="BI26" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ26" s="8" t="s">
         <v>327</v>
@@ -6058,7 +6091,7 @@
       <c r="BH27" s="2"/>
       <c r="BI27" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ27" s="8" t="s">
         <v>327</v>
@@ -6183,7 +6216,7 @@
       <c r="BH28" s="2"/>
       <c r="BI28" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ28" s="8" t="s">
         <v>327</v>
@@ -6310,7 +6343,7 @@
       <c r="BH29" s="2"/>
       <c r="BI29" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ29" s="8" t="s">
         <v>327</v>
@@ -6435,7 +6468,7 @@
       <c r="BH30" s="2"/>
       <c r="BI30" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ30" s="8" t="s">
         <v>327</v>
@@ -6562,7 +6595,7 @@
       <c r="BH31" s="2"/>
       <c r="BI31" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ31" s="8" t="s">
         <v>327</v>
@@ -6689,7 +6722,7 @@
       <c r="BH32" s="2"/>
       <c r="BI32" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ32" s="8" t="s">
         <v>327</v>
@@ -6816,7 +6849,7 @@
       <c r="BH33" s="2"/>
       <c r="BI33" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ33" s="8" t="s">
         <v>327</v>
@@ -6957,7 +6990,7 @@
       <c r="BH34" s="2"/>
       <c r="BI34" s="18">
         <f t="shared" ref="BI34:BI65" ca="1" si="1">NOW()</f>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ34" s="8" t="s">
         <v>327</v>
@@ -7078,7 +7111,7 @@
       <c r="BH35" s="2"/>
       <c r="BI35" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ35" s="8" t="s">
         <v>327</v>
@@ -7203,7 +7236,7 @@
       <c r="BH36" s="2"/>
       <c r="BI36" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ36" s="8" t="s">
         <v>327</v>
@@ -7334,7 +7367,7 @@
       <c r="BH37" s="2"/>
       <c r="BI37" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ37" s="8" t="s">
         <v>327</v>
@@ -7461,7 +7494,7 @@
       <c r="BH38" s="2"/>
       <c r="BI38" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ38" s="8" t="s">
         <v>327</v>
@@ -7590,7 +7623,7 @@
       <c r="BH39" s="2"/>
       <c r="BI39" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ39" s="8" t="s">
         <v>327</v>
@@ -7719,7 +7752,7 @@
       <c r="BH40" s="2"/>
       <c r="BI40" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ40" s="8" t="s">
         <v>327</v>
@@ -7846,7 +7879,7 @@
       <c r="BH41" s="2"/>
       <c r="BI41" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ41" s="8" t="s">
         <v>327</v>
@@ -7983,7 +8016,7 @@
       <c r="BH42" s="2"/>
       <c r="BI42" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ42" s="8" t="s">
         <v>327</v>
@@ -8102,7 +8135,7 @@
       <c r="BH43" s="2"/>
       <c r="BI43" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ43" s="8" t="s">
         <v>327</v>
@@ -8222,7 +8255,7 @@
       <c r="BH44" s="2"/>
       <c r="BI44" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ44" s="8" t="s">
         <v>327</v>
@@ -8344,7 +8377,7 @@
       <c r="BH45" s="2"/>
       <c r="BI45" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ45" s="8" t="s">
         <v>327</v>
@@ -8464,7 +8497,7 @@
       <c r="BH46" s="2"/>
       <c r="BI46" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ46" s="8" t="s">
         <v>327</v>
@@ -8586,7 +8619,7 @@
       <c r="BH47" s="2"/>
       <c r="BI47" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ47" s="8" t="s">
         <v>327</v>
@@ -8706,7 +8739,7 @@
       <c r="BH48" s="2"/>
       <c r="BI48" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ48" s="8" t="s">
         <v>327</v>
@@ -8828,7 +8861,7 @@
       <c r="BH49" s="2"/>
       <c r="BI49" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ49" s="8" t="s">
         <v>327</v>
@@ -8950,7 +8983,7 @@
       <c r="BH50" s="2"/>
       <c r="BI50" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ50" s="8" t="s">
         <v>327</v>
@@ -9070,7 +9103,7 @@
       <c r="BH51" s="2"/>
       <c r="BI51" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ51" s="8" t="s">
         <v>327</v>
@@ -9192,7 +9225,7 @@
       <c r="BH52" s="2"/>
       <c r="BI52" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ52" s="8" t="s">
         <v>327</v>
@@ -9314,7 +9347,7 @@
       <c r="BH53" s="2"/>
       <c r="BI53" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ53" s="8" t="s">
         <v>327</v>
@@ -9440,7 +9473,7 @@
       </c>
       <c r="BI54" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ54" s="8" t="s">
         <v>327</v>
@@ -9567,7 +9600,7 @@
       <c r="BH55" s="24"/>
       <c r="BI55" s="24">
         <f t="shared" ca="1" si="1"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ55" s="8" t="s">
         <v>327</v>
@@ -9704,7 +9737,7 @@
       <c r="BH56" s="24"/>
       <c r="BI56" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ56" s="8" t="s">
         <v>327</v>
@@ -9826,7 +9859,7 @@
       <c r="BH57" s="2"/>
       <c r="BI57" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ57" s="8" t="s">
         <v>327</v>
@@ -9946,7 +9979,7 @@
       <c r="BH58" s="2"/>
       <c r="BI58" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ58" s="8" t="s">
         <v>327</v>
@@ -10068,7 +10101,7 @@
       <c r="BH59" s="2"/>
       <c r="BI59" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ59" s="8" t="s">
         <v>327</v>
@@ -10205,7 +10238,7 @@
       <c r="BH60" s="2"/>
       <c r="BI60" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ60" s="8" t="s">
         <v>327</v>
@@ -10320,7 +10353,7 @@
       <c r="BH61" s="2"/>
       <c r="BI61" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ61" s="8" t="s">
         <v>327</v>
@@ -10440,7 +10473,7 @@
       <c r="BH62" s="2"/>
       <c r="BI62" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ62" s="8" t="s">
         <v>327</v>
@@ -10560,7 +10593,7 @@
       <c r="BH63" s="2"/>
       <c r="BI63" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ63" s="8" t="s">
         <v>327</v>
@@ -10682,7 +10715,7 @@
       <c r="BH64" s="2"/>
       <c r="BI64" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ64" s="8" t="s">
         <v>327</v>
@@ -10807,7 +10840,7 @@
       <c r="BH65" s="2"/>
       <c r="BI65" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ65" s="8" t="s">
         <v>327</v>
@@ -10929,7 +10962,7 @@
       <c r="BH66" s="2"/>
       <c r="BI66" s="18">
         <f t="shared" ref="BI66:BI71" ca="1" si="2">NOW()</f>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ66" s="8" t="s">
         <v>327</v>
@@ -11066,7 +11099,7 @@
       <c r="BH67" s="2"/>
       <c r="BI67" s="18">
         <f t="shared" ca="1" si="2"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ67" s="8" t="s">
         <v>327</v>
@@ -11181,7 +11214,7 @@
       <c r="BH68" s="2"/>
       <c r="BI68" s="18">
         <f t="shared" ca="1" si="2"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ68" s="8" t="s">
         <v>327</v>
@@ -11300,7 +11333,7 @@
       <c r="BH69" s="2"/>
       <c r="BI69" s="18">
         <f t="shared" ca="1" si="2"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ69" s="8" t="s">
         <v>327</v>
@@ -11422,7 +11455,7 @@
       <c r="BH70" s="19"/>
       <c r="BI70" s="33">
         <f t="shared" ca="1" si="2"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ70" s="34" t="s">
         <v>327</v>
@@ -11553,7 +11586,7 @@
       <c r="BH71" s="19"/>
       <c r="BI71" s="33">
         <f t="shared" ca="1" si="2"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ71" s="34" t="s">
         <v>327</v>
@@ -11672,8 +11705,8 @@
       </c>
       <c r="BH72" s="2"/>
       <c r="BI72" s="18">
-        <f t="shared" ref="BI72:BI87" ca="1" si="3">NOW()</f>
-        <v>44252.634867939814</v>
+        <f t="shared" ref="BI72:BI88" ca="1" si="3">NOW()</f>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ72" s="8" t="s">
         <v>327</v>
@@ -11773,7 +11806,7 @@
       <c r="BH73" s="2"/>
       <c r="BI73" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ73" s="8" t="s">
         <v>327</v>
@@ -11895,7 +11928,7 @@
       <c r="BH74" s="2"/>
       <c r="BI74" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ74" s="8" t="s">
         <v>327</v>
@@ -11935,7 +11968,9 @@
       <c r="K75" s="16">
         <v>44287</v>
       </c>
-      <c r="L75" s="16"/>
+      <c r="L75" s="16">
+        <v>44287</v>
+      </c>
       <c r="M75" s="2">
         <v>12</v>
       </c>
@@ -12008,7 +12043,7 @@
       <c r="BH75" s="2"/>
       <c r="BI75" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ75" s="8" t="s">
         <v>327</v>
@@ -12046,7 +12081,10 @@
         <v>43922</v>
       </c>
       <c r="K76" s="16">
-        <v>43922</v>
+        <v>44287</v>
+      </c>
+      <c r="L76" s="16">
+        <v>44287</v>
       </c>
       <c r="M76" s="6">
         <v>12</v>
@@ -12102,7 +12140,7 @@
       <c r="BH76" s="2"/>
       <c r="BI76" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ76" s="8" t="s">
         <v>327</v>
@@ -12142,7 +12180,9 @@
       <c r="K77" s="16">
         <v>44287</v>
       </c>
-      <c r="L77" s="16"/>
+      <c r="L77" s="16">
+        <v>44287</v>
+      </c>
       <c r="M77" s="2">
         <v>12</v>
       </c>
@@ -12237,7 +12277,7 @@
       <c r="BH77" s="2"/>
       <c r="BI77" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ77" s="8" t="s">
         <v>327</v>
@@ -12329,7 +12369,7 @@
       <c r="BH78" s="2"/>
       <c r="BI78" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ78" s="8" t="s">
         <v>327</v>
@@ -12447,7 +12487,7 @@
       <c r="BH79" s="2"/>
       <c r="BI79" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ79" s="8" t="s">
         <v>327</v>
@@ -12541,7 +12581,7 @@
       <c r="BH80" s="2"/>
       <c r="BI80" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ80" s="8" t="s">
         <v>327</v>
@@ -12675,7 +12715,7 @@
       </c>
       <c r="BI81" s="33">
         <f t="shared" ca="1" si="3"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ81" s="34" t="s">
         <v>327</v>
@@ -12774,7 +12814,7 @@
       <c r="BH82" s="19"/>
       <c r="BI82" s="33">
         <f t="shared" ca="1" si="3"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ82" s="34" t="s">
         <v>327</v>
@@ -12894,7 +12934,7 @@
       <c r="BH83" s="2"/>
       <c r="BI83" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ83" s="8" t="s">
         <v>327</v>
@@ -12991,7 +13031,7 @@
       <c r="BH84" s="2"/>
       <c r="BI84" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ84" s="8" t="s">
         <v>327</v>
@@ -13126,7 +13166,7 @@
       <c r="BH85" s="2"/>
       <c r="BI85" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ85" s="8" t="s">
         <v>327</v>
@@ -13246,13 +13286,13 @@
       <c r="BH86" s="2"/>
       <c r="BI86" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ86" s="8" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="87" spans="1:62" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:62" ht="56" x14ac:dyDescent="0.15">
       <c r="A87" s="2" t="s">
         <v>638</v>
       </c>
@@ -13362,36 +13402,78 @@
       <c r="BH87" s="2"/>
       <c r="BI87" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44252.634867939814</v>
+        <v>44302.781457291669</v>
       </c>
       <c r="BJ87" s="8" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="88" spans="1:62" ht="13" x14ac:dyDescent="0.15">
-      <c r="A88" s="2"/>
-      <c r="B88" s="3"/>
-      <c r="C88" s="2"/>
-      <c r="D88" s="2"/>
-      <c r="E88" s="15"/>
-      <c r="F88" s="15"/>
-      <c r="G88" s="15"/>
-      <c r="H88" s="16"/>
-      <c r="I88" s="8"/>
-      <c r="J88" s="16"/>
-      <c r="K88" s="16"/>
+    <row r="88" spans="1:62" ht="84" x14ac:dyDescent="0.15">
+      <c r="A88" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>646</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E88" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="F88" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="G88" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="H88" s="16">
+        <v>44287</v>
+      </c>
+      <c r="I88" s="8" t="s">
+        <v>643</v>
+      </c>
+      <c r="J88" s="16">
+        <v>44287</v>
+      </c>
+      <c r="K88" s="16">
+        <v>44652</v>
+      </c>
       <c r="L88" s="16"/>
-      <c r="M88" s="2"/>
-      <c r="N88" s="2"/>
-      <c r="O88" s="3"/>
+      <c r="M88" s="2">
+        <v>12</v>
+      </c>
+      <c r="N88" s="2" t="s">
+        <v>644</v>
+      </c>
+      <c r="O88" s="3" t="s">
+        <v>645</v>
+      </c>
       <c r="P88" s="15"/>
-      <c r="Q88" s="15"/>
-      <c r="R88" s="2"/>
-      <c r="S88" s="2"/>
-      <c r="T88" s="2"/>
-      <c r="U88" s="3"/>
-      <c r="V88" s="8"/>
-      <c r="W88" s="2"/>
+      <c r="Q88" s="15" t="s">
+        <v>647</v>
+      </c>
+      <c r="R88" s="2" t="s">
+        <v>648</v>
+      </c>
+      <c r="S88" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="T88" s="2" t="s">
+        <v>650</v>
+      </c>
+      <c r="U88" s="3" t="s">
+        <v>651</v>
+      </c>
+      <c r="V88" s="8" t="s">
+        <v>643</v>
+      </c>
+      <c r="W88" s="2" t="s">
+        <v>541</v>
+      </c>
       <c r="X88" s="2"/>
       <c r="Y88" s="2"/>
       <c r="Z88" s="2"/>
@@ -13417,16 +13499,27 @@
       <c r="AX88" s="2"/>
       <c r="AY88" s="2"/>
       <c r="AZ88" s="2"/>
-      <c r="BA88" s="2"/>
-      <c r="BB88" s="2"/>
-      <c r="BC88" s="2"/>
-      <c r="BD88" s="2"/>
-      <c r="BE88" s="2"/>
+      <c r="BA88" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="BB88" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="BE88" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="BF88" s="2"/>
-      <c r="BG88" s="4"/>
+      <c r="BG88" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="BH88" s="2"/>
-      <c r="BI88" s="18"/>
-      <c r="BJ88" s="8"/>
+      <c r="BI88" s="18">
+        <f t="shared" ca="1" si="3"/>
+        <v>44302.781457291669</v>
+      </c>
+      <c r="BJ88" s="8" t="s">
+        <v>327</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:BJ87" xr:uid="{AE487DEF-5BC5-C74D-81B1-9FC54E50B3DD}"/>
@@ -13569,8 +13662,11 @@
     <hyperlink ref="BJ86" r:id="rId135" xr:uid="{A61E0B48-7D1E-9744-9E44-3CFA56C4323E}"/>
     <hyperlink ref="I87" r:id="rId136" xr:uid="{0C3AF352-EF9A-EA45-B5C8-DFCD5AB4D933}"/>
     <hyperlink ref="BJ87" r:id="rId137" xr:uid="{54024D96-B6A6-BA4E-89A9-15C22D785419}"/>
+    <hyperlink ref="I88" r:id="rId138" xr:uid="{7D68488F-A43B-AE43-AE9F-143DD94A0FCF}"/>
+    <hyperlink ref="V88" r:id="rId139" xr:uid="{4D13C756-0C91-E446-AA2D-61D67EAC0A85}"/>
+    <hyperlink ref="BJ88" r:id="rId140" xr:uid="{8F94CCD7-FAE8-474E-A7F6-65692D57572C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId138"/>
+  <legacyDrawing r:id="rId141"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated 360 Giving grants data, and copy corrections
</commit_message>
<xml_diff>
--- a/open/grants.xlsx
+++ b/open/grants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/westsi/Documents/GitHub/zing/open/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4650C152-0A1D-BE41-9CBA-C5551616D1EE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E554CD-75B4-074E-A4A7-46872BF96FBE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="460" yWindow="700" windowWidth="33140" windowHeight="20300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2171" uniqueCount="652">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2192" uniqueCount="656">
   <si>
     <t>Identifier</t>
   </si>
@@ -1652,9 +1652,6 @@
     <t>BH20 6DD</t>
   </si>
   <si>
-    <t>Learning with Parent's mission is to motivate and empower families to have enjoyable learning experiences together. Through their programmes, they partner with schools to drive and monitor effective parental engagement and to support disadvantaged families,  and partner with organisations to champion parental engagement as a means to narrow the disadvantage gap.</t>
-  </si>
-  <si>
     <t>Core funding in response to COVID19, toward coverage of a shortage in event fundraising, which was due to run during the UK lockdown.</t>
   </si>
   <si>
@@ -2026,6 +2023,21 @@
   </si>
   <si>
     <t>The Lily-Jo Project is devoted to eliminating the stigma surrounding mental health through music, digital resources, and community engagement. They believe that when exposed to the basic principles of mental health from an early age, kids are empowered to: be proactive about maintaining good mental health into adulthood, and ultimately reach their full potential and achieve their dreams. The Lily-Jo Project offers: a mix of paid and unpaid consistent digital resources in the form of educational curriculum, podcasts, blog articles, and videos; a way to connect with people through the power of music; and an in-person experience (when possible) through gigs and live workshops, enabling us to engage with the community and develop real-world relationships.</t>
+  </si>
+  <si>
+    <t>360G-zing-95</t>
+  </si>
+  <si>
+    <t>GB-CHC-1189812</t>
+  </si>
+  <si>
+    <t>Learning with Parent's mission is to motivate and empower families to have enjoyable learning experiences together. Through their programmes, they partner with schools to drive and monitor effective parental engagement and to support disadvantaged families, and partner with organisations to champion parental engagement as a means to narrow the disadvantage gap.</t>
+  </si>
+  <si>
+    <t>Core funding toward the redevelopment of the Learning with Parents platform</t>
+  </si>
+  <si>
+    <t>Learning with Parents are establishing themselves as the thought and action leader on embedding parental engagement in all aspects of school curriculum. To cope with increased demand on their services, our last round of funding supported the hiring of a CTO, and improvements to the back-end platform (in response to sudden increased demand during Covid-19 lockdowns), with further in-kind support under our digital stream. The team have since rebuilt their back-end platform, and this funding round is toward to its continued development, related digital projects, and other core costs.</t>
   </si>
 </sst>
 </file>
@@ -2576,7 +2588,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:BJ88"/>
+  <dimension ref="A1:BJ89"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="120" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -2710,94 +2722,94 @@
         <v>21</v>
       </c>
       <c r="W1" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>547</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>548</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>549</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>550</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>551</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>552</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>553</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>554</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>555</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>556</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>557</v>
       </c>
-      <c r="AH1" s="1" t="s">
-        <v>558</v>
-      </c>
       <c r="AI1" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
         <v>563</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>564</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>565</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>566</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>567</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>568</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>569</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>570</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>571</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>572</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>573</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>574</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>576</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>577</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>578</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>579</v>
-      </c>
-      <c r="AZ1" s="1" t="s">
-        <v>580</v>
       </c>
       <c r="BA1" s="1" t="s">
         <v>22</v>
@@ -2901,15 +2913,15 @@
         <v>40</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
       <c r="AA2" s="6" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="AC2" s="2"/>
       <c r="AD2" s="2"/>
@@ -2952,7 +2964,7 @@
       <c r="BH2" s="2"/>
       <c r="BI2" s="18">
         <f t="shared" ref="BI2:BI33" ca="1" si="0">NOW()</f>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ2" s="8" t="s">
         <v>327</v>
@@ -3026,10 +3038,10 @@
         <v>323</v>
       </c>
       <c r="W3" s="2" t="s">
+        <v>532</v>
+      </c>
+      <c r="X3" s="2" t="s">
         <v>533</v>
-      </c>
-      <c r="X3" s="2" t="s">
-        <v>534</v>
       </c>
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
@@ -3077,7 +3089,7 @@
       <c r="BH3" s="2"/>
       <c r="BI3" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ3" s="8" t="s">
         <v>327</v>
@@ -3154,15 +3166,15 @@
         <v>40</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y4" s="2"/>
       <c r="Z4" s="2"/>
       <c r="AA4" s="6" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="AB4" s="2" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="AC4" s="2"/>
       <c r="AD4" s="2"/>
@@ -3205,7 +3217,7 @@
       <c r="BH4" s="2"/>
       <c r="BI4" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ4" s="8" t="s">
         <v>327</v>
@@ -3279,10 +3291,10 @@
         <v>72</v>
       </c>
       <c r="W5" s="6" t="s">
+        <v>534</v>
+      </c>
+      <c r="X5" s="2" t="s">
         <v>535</v>
-      </c>
-      <c r="X5" s="2" t="s">
-        <v>536</v>
       </c>
       <c r="Y5" s="2"/>
       <c r="Z5" s="2"/>
@@ -3329,7 +3341,7 @@
       <c r="BH5" s="2"/>
       <c r="BI5" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ5" s="8" t="s">
         <v>327</v>
@@ -3406,15 +3418,15 @@
         <v>40</v>
       </c>
       <c r="X6" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y6" s="2"/>
       <c r="Z6" s="2"/>
       <c r="AA6" s="6" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="AB6" s="2" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="AC6" s="2"/>
       <c r="AD6" s="2"/>
@@ -3457,7 +3469,7 @@
       <c r="BH6" s="2"/>
       <c r="BI6" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ6" s="8" t="s">
         <v>327</v>
@@ -3534,15 +3546,15 @@
         <v>40</v>
       </c>
       <c r="X7" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y7" s="2"/>
       <c r="Z7" s="2"/>
       <c r="AA7" s="6" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="AB7" s="2" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="AC7" s="2"/>
       <c r="AD7" s="2"/>
@@ -3585,7 +3597,7 @@
       <c r="BH7" s="2"/>
       <c r="BI7" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ7" s="8" t="s">
         <v>327</v>
@@ -3659,20 +3671,20 @@
         <v>323</v>
       </c>
       <c r="W8" s="6" t="s">
+        <v>532</v>
+      </c>
+      <c r="X8" s="2" t="s">
         <v>533</v>
-      </c>
-      <c r="X8" s="2" t="s">
-        <v>534</v>
       </c>
       <c r="Y8" s="2"/>
       <c r="Z8" s="2"/>
       <c r="AA8" s="2"/>
       <c r="AB8" s="2"/>
       <c r="AC8" s="6" t="s">
+        <v>534</v>
+      </c>
+      <c r="AD8" s="2" t="s">
         <v>535</v>
-      </c>
-      <c r="AD8" s="2" t="s">
-        <v>536</v>
       </c>
       <c r="AE8" s="2"/>
       <c r="AF8" s="2"/>
@@ -3714,7 +3726,7 @@
       <c r="BH8" s="2"/>
       <c r="BI8" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ8" s="8" t="s">
         <v>327</v>
@@ -3786,15 +3798,15 @@
         <v>351</v>
       </c>
       <c r="W9" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="X9" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y9" s="2"/>
       <c r="Z9" s="2"/>
       <c r="AA9" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="AB9" s="2"/>
       <c r="AC9" s="2"/>
@@ -3839,7 +3851,7 @@
       <c r="BH9" s="2"/>
       <c r="BI9" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ9" s="8" t="s">
         <v>327</v>
@@ -3913,10 +3925,10 @@
         <v>351</v>
       </c>
       <c r="W10" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X10" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="Y10" s="2"/>
       <c r="Z10" s="2"/>
@@ -3944,7 +3956,7 @@
       <c r="BH10" s="2"/>
       <c r="BI10" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ10" s="8" t="s">
         <v>327</v>
@@ -4016,7 +4028,7 @@
         <v>375</v>
       </c>
       <c r="W11" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="X11" s="2"/>
       <c r="Y11" s="2"/>
@@ -4065,7 +4077,7 @@
       <c r="BH11" s="2"/>
       <c r="BI11" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ11" s="8" t="s">
         <v>327</v>
@@ -4139,15 +4151,15 @@
         <v>392</v>
       </c>
       <c r="W12" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="X12" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y12" s="2"/>
       <c r="Z12" s="2"/>
       <c r="AA12" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="AB12" s="2"/>
       <c r="AC12" s="2"/>
@@ -4192,7 +4204,7 @@
       <c r="BH12" s="2"/>
       <c r="BI12" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ12" s="8" t="s">
         <v>327</v>
@@ -4258,24 +4270,24 @@
         <v>117</v>
       </c>
       <c r="U13" s="2" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="V13" s="7" t="s">
         <v>394</v>
       </c>
       <c r="W13" s="2" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="X13" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y13" s="2"/>
       <c r="Z13" s="2"/>
       <c r="AA13" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="AB13" s="2" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="AC13" s="2"/>
       <c r="AD13" s="2"/>
@@ -4319,7 +4331,7 @@
       <c r="BH13" s="2"/>
       <c r="BI13" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ13" s="8" t="s">
         <v>327</v>
@@ -4393,20 +4405,20 @@
         <v>323</v>
       </c>
       <c r="W14" s="6" t="s">
+        <v>532</v>
+      </c>
+      <c r="X14" s="2" t="s">
         <v>533</v>
-      </c>
-      <c r="X14" s="2" t="s">
-        <v>534</v>
       </c>
       <c r="Y14" s="2"/>
       <c r="Z14" s="2"/>
       <c r="AA14" s="2"/>
       <c r="AB14" s="2"/>
       <c r="AC14" s="6" t="s">
+        <v>534</v>
+      </c>
+      <c r="AD14" s="2" t="s">
         <v>535</v>
-      </c>
-      <c r="AD14" s="2" t="s">
-        <v>536</v>
       </c>
       <c r="AE14" s="2"/>
       <c r="AF14" s="2"/>
@@ -4448,7 +4460,7 @@
       <c r="BH14" s="2"/>
       <c r="BI14" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ14" s="8" t="s">
         <v>327</v>
@@ -4520,15 +4532,15 @@
         <v>351</v>
       </c>
       <c r="W15" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="X15" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y15" s="2"/>
       <c r="Z15" s="2"/>
       <c r="AA15" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="AB15" s="2"/>
       <c r="AC15" s="2"/>
@@ -4573,7 +4585,7 @@
       <c r="BH15" s="2"/>
       <c r="BI15" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ15" s="8" t="s">
         <v>327</v>
@@ -4645,15 +4657,15 @@
         <v>351</v>
       </c>
       <c r="W16" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="X16" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y16" s="2"/>
       <c r="Z16" s="2"/>
       <c r="AA16" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="AB16" s="2"/>
       <c r="AC16" s="2"/>
@@ -4698,7 +4710,7 @@
       <c r="BH16" s="2"/>
       <c r="BI16" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ16" s="8" t="s">
         <v>327</v>
@@ -4775,15 +4787,15 @@
         <v>40</v>
       </c>
       <c r="X17" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y17" s="2"/>
       <c r="Z17" s="2"/>
       <c r="AA17" s="6" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="AB17" s="2" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="AC17" s="2"/>
       <c r="AD17" s="2"/>
@@ -4827,7 +4839,7 @@
       <c r="BH17" s="2"/>
       <c r="BI17" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ17" s="8" t="s">
         <v>327</v>
@@ -4904,15 +4916,15 @@
         <v>40</v>
       </c>
       <c r="X18" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y18" s="2"/>
       <c r="Z18" s="2"/>
       <c r="AA18" s="6" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="AB18" s="2" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="AC18" s="2"/>
       <c r="AD18" s="2"/>
@@ -4956,7 +4968,7 @@
       <c r="BH18" s="2"/>
       <c r="BI18" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ18" s="8" t="s">
         <v>327</v>
@@ -5028,7 +5040,7 @@
         <v>375</v>
       </c>
       <c r="W19" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="X19" s="2"/>
       <c r="Y19" s="2"/>
@@ -5077,7 +5089,7 @@
       <c r="BH19" s="2"/>
       <c r="BI19" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ19" s="8" t="s">
         <v>327</v>
@@ -5152,15 +5164,15 @@
         <v>40</v>
       </c>
       <c r="X20" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y20" s="2"/>
       <c r="Z20" s="2"/>
       <c r="AA20" s="6" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="AB20" s="2" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="AC20" s="2"/>
       <c r="AD20" s="2"/>
@@ -5204,7 +5216,7 @@
       <c r="BH20" s="2"/>
       <c r="BI20" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ20" s="8" t="s">
         <v>327</v>
@@ -5281,15 +5293,15 @@
         <v>40</v>
       </c>
       <c r="X21" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y21" s="2"/>
       <c r="Z21" s="2"/>
       <c r="AA21" s="6" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="AB21" s="2" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="AC21" s="2"/>
       <c r="AD21" s="2"/>
@@ -5333,7 +5345,7 @@
       <c r="BH21" s="2"/>
       <c r="BI21" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ21" s="8" t="s">
         <v>327</v>
@@ -5408,15 +5420,15 @@
         <v>40</v>
       </c>
       <c r="X22" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y22" s="2"/>
       <c r="Z22" s="2"/>
       <c r="AA22" s="6" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="AB22" s="2" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="AC22" s="2"/>
       <c r="AD22" s="2"/>
@@ -5460,7 +5472,7 @@
       <c r="BH22" s="2"/>
       <c r="BI22" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ22" s="8" t="s">
         <v>327</v>
@@ -5537,15 +5549,15 @@
         <v>40</v>
       </c>
       <c r="X23" s="19" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y23" s="19"/>
       <c r="Z23" s="19"/>
       <c r="AA23" s="12" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="AB23" s="19" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="AC23" s="2"/>
       <c r="AD23" s="2"/>
@@ -5589,7 +5601,7 @@
       <c r="BH23" s="2"/>
       <c r="BI23" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ23" s="8" t="s">
         <v>327</v>
@@ -5663,10 +5675,10 @@
         <v>323</v>
       </c>
       <c r="W24" s="2" t="s">
+        <v>532</v>
+      </c>
+      <c r="X24" s="2" t="s">
         <v>533</v>
-      </c>
-      <c r="X24" s="2" t="s">
-        <v>534</v>
       </c>
       <c r="Y24" s="2"/>
       <c r="Z24" s="2"/>
@@ -5714,7 +5726,7 @@
       <c r="BH24" s="2"/>
       <c r="BI24" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ24" s="8" t="s">
         <v>327</v>
@@ -5786,7 +5798,7 @@
         <v>375</v>
       </c>
       <c r="W25" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="X25" s="2"/>
       <c r="Y25" s="2"/>
@@ -5835,7 +5847,7 @@
       <c r="BH25" s="2"/>
       <c r="BI25" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ25" s="8" t="s">
         <v>327</v>
@@ -5909,15 +5921,15 @@
         <v>392</v>
       </c>
       <c r="W26" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="X26" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y26" s="2"/>
       <c r="Z26" s="2"/>
       <c r="AA26" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="AB26" s="2"/>
       <c r="AC26" s="2"/>
@@ -5962,7 +5974,7 @@
       <c r="BH26" s="2"/>
       <c r="BI26" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ26" s="8" t="s">
         <v>327</v>
@@ -6039,15 +6051,15 @@
         <v>40</v>
       </c>
       <c r="X27" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y27" s="2"/>
       <c r="Z27" s="2"/>
       <c r="AA27" s="6" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="AB27" s="2" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="AC27" s="2"/>
       <c r="AD27" s="2"/>
@@ -6091,7 +6103,7 @@
       <c r="BH27" s="2"/>
       <c r="BI27" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ27" s="8" t="s">
         <v>327</v>
@@ -6163,15 +6175,15 @@
         <v>174</v>
       </c>
       <c r="W28" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="X28" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y28" s="2"/>
       <c r="Z28" s="2"/>
       <c r="AA28" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="AB28" s="2"/>
       <c r="AC28" s="2"/>
@@ -6216,7 +6228,7 @@
       <c r="BH28" s="2"/>
       <c r="BI28" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ28" s="8" t="s">
         <v>327</v>
@@ -6290,15 +6302,15 @@
         <v>186</v>
       </c>
       <c r="W29" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="X29" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y29" s="2"/>
       <c r="Z29" s="2"/>
       <c r="AA29" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="AB29" s="2"/>
       <c r="AC29" s="2"/>
@@ -6343,7 +6355,7 @@
       <c r="BH29" s="2"/>
       <c r="BI29" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ29" s="8" t="s">
         <v>327</v>
@@ -6415,15 +6427,15 @@
         <v>196</v>
       </c>
       <c r="W30" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="X30" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y30" s="2"/>
       <c r="Z30" s="2"/>
       <c r="AA30" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="AB30" s="2"/>
       <c r="AC30" s="2"/>
@@ -6468,7 +6480,7 @@
       <c r="BH30" s="2"/>
       <c r="BI30" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ30" s="8" t="s">
         <v>327</v>
@@ -6542,15 +6554,15 @@
         <v>345</v>
       </c>
       <c r="W31" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="X31" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y31" s="2"/>
       <c r="Z31" s="2"/>
       <c r="AA31" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="AB31" s="2"/>
       <c r="AC31" s="2"/>
@@ -6595,7 +6607,7 @@
       <c r="BH31" s="2"/>
       <c r="BI31" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ31" s="8" t="s">
         <v>327</v>
@@ -6669,15 +6681,15 @@
         <v>371</v>
       </c>
       <c r="W32" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="X32" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y32" s="2"/>
       <c r="Z32" s="2"/>
       <c r="AA32" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="AB32" s="2"/>
       <c r="AC32" s="2"/>
@@ -6722,7 +6734,7 @@
       <c r="BH32" s="2"/>
       <c r="BI32" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ32" s="8" t="s">
         <v>327</v>
@@ -6796,15 +6808,15 @@
         <v>382</v>
       </c>
       <c r="W33" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="X33" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y33" s="2"/>
       <c r="Z33" s="2"/>
       <c r="AA33" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="AB33" s="2"/>
       <c r="AC33" s="2"/>
@@ -6849,7 +6861,7 @@
       <c r="BH33" s="2"/>
       <c r="BI33" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ33" s="8" t="s">
         <v>327</v>
@@ -6923,50 +6935,50 @@
         <v>323</v>
       </c>
       <c r="W34" s="2" t="s">
+        <v>558</v>
+      </c>
+      <c r="X34" s="2" t="s">
         <v>559</v>
-      </c>
-      <c r="X34" s="2" t="s">
-        <v>560</v>
       </c>
       <c r="Y34" s="2"/>
       <c r="Z34" s="2"/>
       <c r="AA34" s="2"/>
       <c r="AB34" s="2"/>
       <c r="AC34" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="AD34" s="2" t="s">
         <v>561</v>
-      </c>
-      <c r="AD34" s="2" t="s">
-        <v>562</v>
       </c>
       <c r="AE34" s="2"/>
       <c r="AF34" s="2"/>
       <c r="AG34" s="2"/>
       <c r="AH34" s="2"/>
       <c r="AI34" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="AJ34" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="AK34" s="2"/>
       <c r="AL34" s="2"/>
       <c r="AM34" s="2"/>
       <c r="AN34" s="2"/>
       <c r="AO34" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="AP34" s="2" t="s">
         <v>535</v>
-      </c>
-      <c r="AP34" s="2" t="s">
-        <v>536</v>
       </c>
       <c r="AQ34" s="2"/>
       <c r="AR34" s="2"/>
       <c r="AS34" s="2"/>
       <c r="AT34" s="2"/>
       <c r="AU34" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="AV34" s="2" t="s">
         <v>581</v>
-      </c>
-      <c r="AV34" s="2" t="s">
-        <v>582</v>
       </c>
       <c r="AW34" s="2"/>
       <c r="AX34" s="2"/>
@@ -6990,7 +7002,7 @@
       <c r="BH34" s="2"/>
       <c r="BI34" s="18">
         <f t="shared" ref="BI34:BI65" ca="1" si="1">NOW()</f>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ34" s="8" t="s">
         <v>327</v>
@@ -7062,7 +7074,7 @@
         <v>227</v>
       </c>
       <c r="W35" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="X35" s="2"/>
       <c r="Y35" s="2"/>
@@ -7111,7 +7123,7 @@
       <c r="BH35" s="2"/>
       <c r="BI35" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ35" s="8" t="s">
         <v>327</v>
@@ -7185,10 +7197,10 @@
         <v>72</v>
       </c>
       <c r="W36" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X36" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="Y36" s="2"/>
       <c r="Z36" s="2"/>
@@ -7236,7 +7248,7 @@
       <c r="BH36" s="2"/>
       <c r="BI36" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ36" s="8" t="s">
         <v>327</v>
@@ -7308,30 +7320,30 @@
         <v>340</v>
       </c>
       <c r="W37" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="X37" s="2" t="s">
         <v>535</v>
-      </c>
-      <c r="X37" s="2" t="s">
-        <v>536</v>
       </c>
       <c r="Y37" s="2"/>
       <c r="Z37" s="2"/>
       <c r="AA37" s="2"/>
       <c r="AB37" s="2"/>
       <c r="AC37" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="AD37" s="2" t="s">
         <v>583</v>
-      </c>
-      <c r="AD37" s="2" t="s">
-        <v>584</v>
       </c>
       <c r="AE37" s="2"/>
       <c r="AF37" s="2"/>
       <c r="AG37" s="2"/>
       <c r="AH37" s="2"/>
       <c r="AI37" s="2" t="s">
+        <v>558</v>
+      </c>
+      <c r="AJ37" s="2" t="s">
         <v>559</v>
-      </c>
-      <c r="AJ37" s="2" t="s">
-        <v>560</v>
       </c>
       <c r="AK37" s="2"/>
       <c r="AL37" s="2"/>
@@ -7367,7 +7379,7 @@
       <c r="BH37" s="2"/>
       <c r="BI37" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ37" s="8" t="s">
         <v>327</v>
@@ -7435,21 +7447,21 @@
         <v>248</v>
       </c>
       <c r="U38" s="2" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="V38" s="7" t="s">
         <v>249</v>
       </c>
       <c r="W38" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="X38" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y38" s="2"/>
       <c r="Z38" s="2"/>
       <c r="AA38" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="AB38" s="2"/>
       <c r="AC38" s="2"/>
@@ -7494,7 +7506,7 @@
       <c r="BH38" s="2"/>
       <c r="BI38" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ38" s="8" t="s">
         <v>327</v>
@@ -7571,15 +7583,15 @@
         <v>40</v>
       </c>
       <c r="X39" s="19" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y39" s="19"/>
       <c r="Z39" s="19"/>
       <c r="AA39" s="12" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="AB39" s="19" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="AC39" s="2"/>
       <c r="AD39" s="2"/>
@@ -7623,7 +7635,7 @@
       <c r="BH39" s="2"/>
       <c r="BI39" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ39" s="8" t="s">
         <v>327</v>
@@ -7700,15 +7712,15 @@
         <v>40</v>
       </c>
       <c r="X40" s="19" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y40" s="19"/>
       <c r="Z40" s="19"/>
       <c r="AA40" s="12" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="AB40" s="19" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="AC40" s="2"/>
       <c r="AD40" s="2"/>
@@ -7752,7 +7764,7 @@
       <c r="BH40" s="2"/>
       <c r="BI40" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ40" s="8" t="s">
         <v>327</v>
@@ -7826,15 +7838,15 @@
         <v>363</v>
       </c>
       <c r="W41" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="X41" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y41" s="2"/>
       <c r="Z41" s="2"/>
       <c r="AA41" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="AB41" s="2"/>
       <c r="AC41" s="2"/>
@@ -7879,7 +7891,7 @@
       <c r="BH41" s="2"/>
       <c r="BI41" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ41" s="8" t="s">
         <v>327</v>
@@ -7953,46 +7965,46 @@
         <v>323</v>
       </c>
       <c r="W42" s="2" t="s">
+        <v>558</v>
+      </c>
+      <c r="X42" s="2" t="s">
         <v>559</v>
-      </c>
-      <c r="X42" s="2" t="s">
-        <v>560</v>
       </c>
       <c r="Y42" s="2"/>
       <c r="Z42" s="2"/>
       <c r="AC42" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="AD42" s="2" t="s">
         <v>561</v>
-      </c>
-      <c r="AD42" s="2" t="s">
-        <v>562</v>
       </c>
       <c r="AE42" s="2"/>
       <c r="AF42" s="2"/>
       <c r="AG42" s="2"/>
       <c r="AH42" s="2"/>
       <c r="AI42" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="AJ42" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="AK42" s="2"/>
       <c r="AL42" s="2"/>
       <c r="AO42" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="AP42" s="2" t="s">
         <v>535</v>
-      </c>
-      <c r="AP42" s="2" t="s">
-        <v>536</v>
       </c>
       <c r="AQ42" s="2"/>
       <c r="AR42" s="2"/>
       <c r="AS42" s="2"/>
       <c r="AT42" s="2"/>
       <c r="AU42" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="AV42" s="2" t="s">
         <v>581</v>
-      </c>
-      <c r="AV42" s="2" t="s">
-        <v>582</v>
       </c>
       <c r="AW42" s="2"/>
       <c r="AX42" s="2"/>
@@ -8016,7 +8028,7 @@
       <c r="BH42" s="2"/>
       <c r="BI42" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ42" s="8" t="s">
         <v>327</v>
@@ -8090,10 +8102,10 @@
         <v>72</v>
       </c>
       <c r="W43" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="X43" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="Y43" s="2"/>
       <c r="Z43" s="2"/>
@@ -8135,7 +8147,7 @@
       <c r="BH43" s="2"/>
       <c r="BI43" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ43" s="8" t="s">
         <v>327</v>
@@ -8207,15 +8219,15 @@
         <v>351</v>
       </c>
       <c r="W44" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="X44" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y44" s="2"/>
       <c r="Z44" s="2"/>
       <c r="AA44" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="AC44" s="2"/>
       <c r="AD44" s="2"/>
@@ -8255,7 +8267,7 @@
       <c r="BH44" s="2"/>
       <c r="BI44" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ44" s="8" t="s">
         <v>327</v>
@@ -8329,15 +8341,15 @@
         <v>186</v>
       </c>
       <c r="W45" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="X45" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y45" s="2"/>
       <c r="Z45" s="2"/>
       <c r="AA45" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="AC45" s="2"/>
       <c r="AD45" s="2"/>
@@ -8377,7 +8389,7 @@
       <c r="BH45" s="2"/>
       <c r="BI45" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ45" s="8" t="s">
         <v>327</v>
@@ -8449,15 +8461,15 @@
         <v>196</v>
       </c>
       <c r="W46" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="X46" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y46" s="2"/>
       <c r="Z46" s="2"/>
       <c r="AA46" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="AC46" s="2"/>
       <c r="AD46" s="2"/>
@@ -8497,7 +8509,7 @@
       <c r="BH46" s="2"/>
       <c r="BI46" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ46" s="8" t="s">
         <v>327</v>
@@ -8565,21 +8577,21 @@
         <v>248</v>
       </c>
       <c r="U47" s="2" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="V47" s="7" t="s">
         <v>249</v>
       </c>
       <c r="W47" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="X47" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y47" s="2"/>
       <c r="Z47" s="2"/>
       <c r="AA47" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="AC47" s="2"/>
       <c r="AD47" s="2"/>
@@ -8619,7 +8631,7 @@
       <c r="BH47" s="2"/>
       <c r="BI47" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ47" s="8" t="s">
         <v>327</v>
@@ -8691,15 +8703,15 @@
         <v>174</v>
       </c>
       <c r="W48" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="X48" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y48" s="2"/>
       <c r="Z48" s="2"/>
       <c r="AA48" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="AC48" s="2"/>
       <c r="AD48" s="2"/>
@@ -8739,7 +8751,7 @@
       <c r="BH48" s="2"/>
       <c r="BI48" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ48" s="8" t="s">
         <v>327</v>
@@ -8807,21 +8819,21 @@
         <v>248</v>
       </c>
       <c r="U49" s="2" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="V49" s="7" t="s">
         <v>249</v>
       </c>
       <c r="W49" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="X49" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y49" s="2"/>
       <c r="Z49" s="2"/>
       <c r="AA49" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="AC49" s="2"/>
       <c r="AD49" s="2"/>
@@ -8861,7 +8873,7 @@
       <c r="BH49" s="2"/>
       <c r="BI49" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ49" s="8" t="s">
         <v>327</v>
@@ -8935,15 +8947,15 @@
         <v>382</v>
       </c>
       <c r="W50" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="X50" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y50" s="2"/>
       <c r="Z50" s="2"/>
       <c r="AA50" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="AC50" s="2"/>
       <c r="AD50" s="2"/>
@@ -8983,7 +8995,7 @@
       <c r="BH50" s="2"/>
       <c r="BI50" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ50" s="8" t="s">
         <v>327</v>
@@ -9055,15 +9067,15 @@
         <v>351</v>
       </c>
       <c r="W51" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="X51" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y51" s="2"/>
       <c r="Z51" s="2"/>
       <c r="AA51" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="AC51" s="2"/>
       <c r="AD51" s="2"/>
@@ -9103,7 +9115,7 @@
       <c r="BH51" s="2"/>
       <c r="BI51" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ51" s="8" t="s">
         <v>327</v>
@@ -9177,15 +9189,15 @@
         <v>371</v>
       </c>
       <c r="W52" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="X52" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y52" s="2"/>
       <c r="Z52" s="2"/>
       <c r="AA52" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="AC52" s="2"/>
       <c r="AD52" s="2"/>
@@ -9225,7 +9237,7 @@
       <c r="BH52" s="2"/>
       <c r="BI52" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ52" s="8" t="s">
         <v>327</v>
@@ -9299,15 +9311,15 @@
         <v>285</v>
       </c>
       <c r="W53" s="2" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="X53" s="6" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y53" s="2"/>
       <c r="Z53" s="2"/>
       <c r="AA53" s="2" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="AC53" s="2"/>
       <c r="AD53" s="2"/>
@@ -9347,7 +9359,7 @@
       <c r="BH53" s="2"/>
       <c r="BI53" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ53" s="8" t="s">
         <v>327</v>
@@ -9419,28 +9431,28 @@
         <v>340</v>
       </c>
       <c r="W54" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="X54" s="2" t="s">
         <v>535</v>
-      </c>
-      <c r="X54" s="2" t="s">
-        <v>536</v>
       </c>
       <c r="Y54" s="2"/>
       <c r="Z54" s="2"/>
       <c r="AC54" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="AD54" s="2" t="s">
         <v>583</v>
-      </c>
-      <c r="AD54" s="2" t="s">
-        <v>584</v>
       </c>
       <c r="AE54" s="2"/>
       <c r="AF54" s="2"/>
       <c r="AG54" s="2"/>
       <c r="AH54" s="2"/>
       <c r="AI54" s="2" t="s">
+        <v>558</v>
+      </c>
+      <c r="AJ54" s="2" t="s">
         <v>559</v>
-      </c>
-      <c r="AJ54" s="2" t="s">
-        <v>560</v>
       </c>
       <c r="AK54" s="2"/>
       <c r="AL54" s="2"/>
@@ -9473,7 +9485,7 @@
       </c>
       <c r="BI54" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ54" s="8" t="s">
         <v>327</v>
@@ -9545,28 +9557,28 @@
         <v>340</v>
       </c>
       <c r="W55" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="X55" s="2" t="s">
         <v>535</v>
-      </c>
-      <c r="X55" s="2" t="s">
-        <v>536</v>
       </c>
       <c r="Y55" s="4"/>
       <c r="Z55" s="4"/>
       <c r="AC55" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="AD55" s="2" t="s">
         <v>583</v>
-      </c>
-      <c r="AD55" s="2" t="s">
-        <v>584</v>
       </c>
       <c r="AE55" s="4"/>
       <c r="AF55" s="4"/>
       <c r="AG55" s="4"/>
       <c r="AH55" s="4"/>
       <c r="AI55" s="2" t="s">
+        <v>558</v>
+      </c>
+      <c r="AJ55" s="2" t="s">
         <v>559</v>
-      </c>
-      <c r="AJ55" s="2" t="s">
-        <v>560</v>
       </c>
       <c r="AK55" s="4"/>
       <c r="AL55" s="4"/>
@@ -9600,7 +9612,7 @@
       <c r="BH55" s="24"/>
       <c r="BI55" s="24">
         <f t="shared" ca="1" si="1"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ55" s="8" t="s">
         <v>327</v>
@@ -9674,46 +9686,46 @@
         <v>323</v>
       </c>
       <c r="W56" s="2" t="s">
+        <v>558</v>
+      </c>
+      <c r="X56" s="2" t="s">
         <v>559</v>
-      </c>
-      <c r="X56" s="2" t="s">
-        <v>560</v>
       </c>
       <c r="Y56" s="2"/>
       <c r="Z56" s="2"/>
       <c r="AC56" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="AD56" s="2" t="s">
         <v>561</v>
-      </c>
-      <c r="AD56" s="2" t="s">
-        <v>562</v>
       </c>
       <c r="AE56" s="2"/>
       <c r="AF56" s="2"/>
       <c r="AG56" s="2"/>
       <c r="AH56" s="2"/>
       <c r="AI56" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="AJ56" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="AK56" s="2"/>
       <c r="AL56" s="2"/>
       <c r="AO56" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="AP56" s="2" t="s">
         <v>535</v>
-      </c>
-      <c r="AP56" s="2" t="s">
-        <v>536</v>
       </c>
       <c r="AQ56" s="2"/>
       <c r="AR56" s="2"/>
       <c r="AS56" s="2"/>
       <c r="AT56" s="2"/>
       <c r="AU56" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="AV56" s="2" t="s">
         <v>581</v>
-      </c>
-      <c r="AV56" s="2" t="s">
-        <v>582</v>
       </c>
       <c r="AW56" s="2"/>
       <c r="AX56" s="2"/>
@@ -9737,7 +9749,7 @@
       <c r="BH56" s="24"/>
       <c r="BI56" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ56" s="8" t="s">
         <v>327</v>
@@ -9805,21 +9817,21 @@
         <v>248</v>
       </c>
       <c r="U57" s="2" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="V57" s="7" t="s">
         <v>249</v>
       </c>
       <c r="W57" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="X57" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y57" s="2"/>
       <c r="Z57" s="2"/>
       <c r="AA57" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="AC57" s="2"/>
       <c r="AD57" s="2"/>
@@ -9859,7 +9871,7 @@
       <c r="BH57" s="2"/>
       <c r="BI57" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ57" s="8" t="s">
         <v>327</v>
@@ -9931,15 +9943,15 @@
         <v>372</v>
       </c>
       <c r="W58" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="X58" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y58" s="2"/>
       <c r="Z58" s="2"/>
       <c r="AA58" s="6" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="AC58" s="2"/>
       <c r="AD58" s="2"/>
@@ -9979,7 +9991,7 @@
       <c r="BH58" s="2"/>
       <c r="BI58" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ58" s="8" t="s">
         <v>327</v>
@@ -10053,15 +10065,15 @@
         <v>384</v>
       </c>
       <c r="W59" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="X59" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y59" s="2"/>
       <c r="Z59" s="2"/>
       <c r="AA59" s="6" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="AC59" s="2"/>
       <c r="AD59" s="2"/>
@@ -10101,7 +10113,7 @@
       <c r="BH59" s="2"/>
       <c r="BI59" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ59" s="8" t="s">
         <v>327</v>
@@ -10175,46 +10187,46 @@
         <v>323</v>
       </c>
       <c r="W60" s="2" t="s">
+        <v>558</v>
+      </c>
+      <c r="X60" s="2" t="s">
         <v>559</v>
-      </c>
-      <c r="X60" s="2" t="s">
-        <v>560</v>
       </c>
       <c r="Y60" s="2"/>
       <c r="Z60" s="2"/>
       <c r="AC60" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="AD60" s="2" t="s">
         <v>561</v>
-      </c>
-      <c r="AD60" s="2" t="s">
-        <v>562</v>
       </c>
       <c r="AE60" s="2"/>
       <c r="AF60" s="2"/>
       <c r="AG60" s="2"/>
       <c r="AH60" s="2"/>
       <c r="AI60" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="AJ60" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="AK60" s="2"/>
       <c r="AL60" s="2"/>
       <c r="AO60" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="AP60" s="2" t="s">
         <v>535</v>
-      </c>
-      <c r="AP60" s="2" t="s">
-        <v>536</v>
       </c>
       <c r="AQ60" s="2"/>
       <c r="AR60" s="2"/>
       <c r="AS60" s="2"/>
       <c r="AT60" s="2"/>
       <c r="AU60" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="AV60" s="2" t="s">
         <v>581</v>
-      </c>
-      <c r="AV60" s="2" t="s">
-        <v>582</v>
       </c>
       <c r="AW60" s="2"/>
       <c r="AX60" s="2"/>
@@ -10238,7 +10250,7 @@
       <c r="BH60" s="2"/>
       <c r="BI60" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ60" s="8" t="s">
         <v>327</v>
@@ -10310,7 +10322,7 @@
         <v>405</v>
       </c>
       <c r="W61" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="X61" s="2"/>
       <c r="Y61" s="2"/>
@@ -10353,7 +10365,7 @@
       <c r="BH61" s="2"/>
       <c r="BI61" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ61" s="8" t="s">
         <v>327</v>
@@ -10425,15 +10437,15 @@
         <v>407</v>
       </c>
       <c r="W62" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="X62" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y62" s="2"/>
       <c r="Z62" s="2"/>
       <c r="AA62" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="AC62" s="2"/>
       <c r="AD62" s="2"/>
@@ -10473,7 +10485,7 @@
       <c r="BH62" s="2"/>
       <c r="BI62" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ62" s="8" t="s">
         <v>327</v>
@@ -10545,15 +10557,15 @@
         <v>418</v>
       </c>
       <c r="W63" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="X63" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y63" s="2"/>
       <c r="Z63" s="2"/>
       <c r="AA63" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="AC63" s="2"/>
       <c r="AD63" s="2"/>
@@ -10593,7 +10605,7 @@
       <c r="BH63" s="2"/>
       <c r="BI63" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ63" s="8" t="s">
         <v>327</v>
@@ -10667,15 +10679,15 @@
         <v>437</v>
       </c>
       <c r="W64" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="X64" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y64" s="2"/>
       <c r="Z64" s="2"/>
       <c r="AA64" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="AC64" s="2"/>
       <c r="AD64" s="2"/>
@@ -10715,7 +10727,7 @@
       <c r="BH64" s="2"/>
       <c r="BI64" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ64" s="8" t="s">
         <v>327</v>
@@ -10789,18 +10801,18 @@
         <v>446</v>
       </c>
       <c r="W65" s="2" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="X65" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y65" s="2"/>
       <c r="Z65" s="2"/>
       <c r="AA65" s="6" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="AB65" s="6" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="AC65" s="2"/>
       <c r="AD65" s="2"/>
@@ -10840,7 +10852,7 @@
       <c r="BH65" s="2"/>
       <c r="BI65" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ65" s="8" t="s">
         <v>327</v>
@@ -10917,12 +10929,12 @@
         <v>40</v>
       </c>
       <c r="X66" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y66" s="2"/>
       <c r="Z66" s="2"/>
       <c r="AA66" s="6" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="AC66" s="2"/>
       <c r="AD66" s="2"/>
@@ -10962,7 +10974,7 @@
       <c r="BH66" s="2"/>
       <c r="BI66" s="18">
         <f t="shared" ref="BI66:BI71" ca="1" si="2">NOW()</f>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ66" s="8" t="s">
         <v>327</v>
@@ -11036,46 +11048,46 @@
         <v>323</v>
       </c>
       <c r="W67" s="2" t="s">
+        <v>558</v>
+      </c>
+      <c r="X67" s="2" t="s">
         <v>559</v>
-      </c>
-      <c r="X67" s="2" t="s">
-        <v>560</v>
       </c>
       <c r="Y67" s="2"/>
       <c r="Z67" s="2"/>
       <c r="AC67" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="AD67" s="2" t="s">
         <v>561</v>
-      </c>
-      <c r="AD67" s="2" t="s">
-        <v>562</v>
       </c>
       <c r="AE67" s="2"/>
       <c r="AF67" s="2"/>
       <c r="AG67" s="2"/>
       <c r="AH67" s="2"/>
       <c r="AI67" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="AJ67" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="AK67" s="2"/>
       <c r="AL67" s="2"/>
       <c r="AO67" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="AP67" s="2" t="s">
         <v>535</v>
-      </c>
-      <c r="AP67" s="2" t="s">
-        <v>536</v>
       </c>
       <c r="AQ67" s="2"/>
       <c r="AR67" s="2"/>
       <c r="AS67" s="2"/>
       <c r="AT67" s="2"/>
       <c r="AU67" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="AV67" s="2" t="s">
         <v>581</v>
-      </c>
-      <c r="AV67" s="2" t="s">
-        <v>582</v>
       </c>
       <c r="AW67" s="2"/>
       <c r="AX67" s="2"/>
@@ -11099,7 +11111,7 @@
       <c r="BH67" s="2"/>
       <c r="BI67" s="18">
         <f t="shared" ca="1" si="2"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ67" s="8" t="s">
         <v>327</v>
@@ -11171,7 +11183,7 @@
         <v>372</v>
       </c>
       <c r="W68" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="X68" s="2"/>
       <c r="Y68" s="2"/>
@@ -11214,7 +11226,7 @@
       <c r="BH68" s="2"/>
       <c r="BI68" s="18">
         <f t="shared" ca="1" si="2"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ68" s="8" t="s">
         <v>327</v>
@@ -11285,15 +11297,15 @@
         <v>480</v>
       </c>
       <c r="W69" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="X69" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y69" s="2"/>
       <c r="Z69" s="2"/>
       <c r="AA69" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="AC69" s="2"/>
       <c r="AD69" s="2"/>
@@ -11333,7 +11345,7 @@
       <c r="BH69" s="2"/>
       <c r="BI69" s="18">
         <f t="shared" ca="1" si="2"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ69" s="8" t="s">
         <v>327</v>
@@ -11407,15 +11419,15 @@
         <v>308</v>
       </c>
       <c r="W70" s="19" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="X70" s="19" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y70" s="19"/>
       <c r="Z70" s="19"/>
       <c r="AA70" s="12" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="AC70" s="19"/>
       <c r="AD70" s="19"/>
@@ -11455,7 +11467,7 @@
       <c r="BH70" s="19"/>
       <c r="BI70" s="33">
         <f t="shared" ca="1" si="2"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ70" s="34" t="s">
         <v>327</v>
@@ -11530,29 +11542,29 @@
         <v>40</v>
       </c>
       <c r="X71" s="19" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y71" s="19"/>
       <c r="Z71" s="19"/>
       <c r="AA71" s="12" t="s">
+        <v>529</v>
+      </c>
+      <c r="AB71" s="12" t="s">
+        <v>531</v>
+      </c>
+      <c r="AC71" s="19" t="s">
+        <v>589</v>
+      </c>
+      <c r="AD71" s="19" t="s">
         <v>530</v>
-      </c>
-      <c r="AB71" s="12" t="s">
-        <v>532</v>
-      </c>
-      <c r="AC71" s="19" t="s">
-        <v>590</v>
-      </c>
-      <c r="AD71" s="19" t="s">
-        <v>531</v>
       </c>
       <c r="AE71" s="19"/>
       <c r="AF71" s="19"/>
       <c r="AG71" s="19" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="AH71" s="19" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="AK71" s="19"/>
       <c r="AL71" s="19"/>
@@ -11586,7 +11598,7 @@
       <c r="BH71" s="19"/>
       <c r="BI71" s="33">
         <f t="shared" ca="1" si="2"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ71" s="34" t="s">
         <v>327</v>
@@ -11618,7 +11630,7 @@
         <v>43831</v>
       </c>
       <c r="I72" s="8" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="J72" s="16">
         <v>43831</v>
@@ -11655,18 +11667,18 @@
         <v>512</v>
       </c>
       <c r="V72" s="8" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="W72" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="X72" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y72" s="2"/>
       <c r="Z72" s="2"/>
       <c r="AA72" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="AC72" s="2"/>
       <c r="AD72" s="2"/>
@@ -11705,8 +11717,8 @@
       </c>
       <c r="BH72" s="2"/>
       <c r="BI72" s="18">
-        <f t="shared" ref="BI72:BI88" ca="1" si="3">NOW()</f>
-        <v>44302.781457291669</v>
+        <f t="shared" ref="BI72:BI89" ca="1" si="3">NOW()</f>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ72" s="8" t="s">
         <v>327</v>
@@ -11780,13 +11792,13 @@
         <v>508</v>
       </c>
       <c r="W73" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="X73" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="AA73" s="6" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="BA73" s="2" t="s">
         <v>43</v>
@@ -11806,7 +11818,7 @@
       <c r="BH73" s="2"/>
       <c r="BI73" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ73" s="8" t="s">
         <v>327</v>
@@ -11859,7 +11871,7 @@
         <v>419</v>
       </c>
       <c r="P74" s="26" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="Q74" s="17" t="s">
         <v>420</v>
@@ -11880,15 +11892,15 @@
         <v>418</v>
       </c>
       <c r="W74" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="X74" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y74" s="2"/>
       <c r="Z74" s="2"/>
       <c r="AA74" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="AC74" s="2"/>
       <c r="AD74" s="2"/>
@@ -11928,7 +11940,7 @@
       <c r="BH74" s="2"/>
       <c r="BI74" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ74" s="8" t="s">
         <v>327</v>
@@ -12000,7 +12012,7 @@
         <v>372</v>
       </c>
       <c r="W75" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="X75" s="2"/>
       <c r="Y75" s="2"/>
@@ -12043,7 +12055,7 @@
       <c r="BH75" s="2"/>
       <c r="BI75" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ75" s="8" t="s">
         <v>327</v>
@@ -12108,19 +12120,19 @@
         <v>526</v>
       </c>
       <c r="U76" s="6" t="s">
-        <v>527</v>
+        <v>653</v>
       </c>
       <c r="V76" s="8" t="s">
         <v>521</v>
       </c>
       <c r="W76" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="X76" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="AA76" s="6" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="BA76" s="2" t="s">
         <v>43</v>
@@ -12140,7 +12152,7 @@
       <c r="BH76" s="2"/>
       <c r="BI76" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ76" s="8" t="s">
         <v>327</v>
@@ -12151,10 +12163,10 @@
         <v>499</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>34</v>
@@ -12214,46 +12226,46 @@
         <v>323</v>
       </c>
       <c r="W77" s="2" t="s">
+        <v>558</v>
+      </c>
+      <c r="X77" s="2" t="s">
         <v>559</v>
-      </c>
-      <c r="X77" s="2" t="s">
-        <v>560</v>
       </c>
       <c r="Y77" s="2"/>
       <c r="Z77" s="2"/>
       <c r="AC77" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="AD77" s="2" t="s">
         <v>561</v>
-      </c>
-      <c r="AD77" s="2" t="s">
-        <v>562</v>
       </c>
       <c r="AE77" s="2"/>
       <c r="AF77" s="2"/>
       <c r="AG77" s="2"/>
       <c r="AH77" s="2"/>
       <c r="AI77" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="AJ77" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="AK77" s="2"/>
       <c r="AL77" s="2"/>
       <c r="AO77" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="AP77" s="2" t="s">
         <v>535</v>
-      </c>
-      <c r="AP77" s="2" t="s">
-        <v>536</v>
       </c>
       <c r="AQ77" s="2"/>
       <c r="AR77" s="2"/>
       <c r="AS77" s="2"/>
       <c r="AT77" s="2"/>
       <c r="AU77" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="AV77" s="2" t="s">
         <v>581</v>
-      </c>
-      <c r="AV77" s="2" t="s">
-        <v>582</v>
       </c>
       <c r="AW77" s="2"/>
       <c r="AX77" s="2"/>
@@ -12277,7 +12289,7 @@
       <c r="BH77" s="2"/>
       <c r="BI77" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ77" s="8" t="s">
         <v>327</v>
@@ -12285,13 +12297,13 @@
     </row>
     <row r="78" spans="1:62" ht="70" x14ac:dyDescent="0.15">
       <c r="A78" s="2" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="C78" s="12" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="D78" s="6" t="s">
         <v>34</v>
@@ -12309,7 +12321,7 @@
         <v>44075</v>
       </c>
       <c r="I78" s="8" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="J78" s="16">
         <v>44075</v>
@@ -12321,37 +12333,37 @@
         <v>12</v>
       </c>
       <c r="N78" s="6" t="s">
+        <v>595</v>
+      </c>
+      <c r="O78" s="6" t="s">
+        <v>594</v>
+      </c>
+      <c r="Q78" s="30" t="s">
         <v>596</v>
       </c>
-      <c r="O78" s="6" t="s">
-        <v>595</v>
-      </c>
-      <c r="Q78" s="30" t="s">
-        <v>597</v>
-      </c>
       <c r="R78" s="6" t="s">
+        <v>609</v>
+      </c>
+      <c r="S78" s="6" t="s">
+        <v>607</v>
+      </c>
+      <c r="T78" s="6" t="s">
+        <v>608</v>
+      </c>
+      <c r="U78" s="6" t="s">
         <v>610</v>
       </c>
-      <c r="S78" s="6" t="s">
-        <v>608</v>
-      </c>
-      <c r="T78" s="6" t="s">
-        <v>609</v>
-      </c>
-      <c r="U78" s="6" t="s">
-        <v>611</v>
-      </c>
       <c r="V78" s="8" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="W78" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="X78" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="AA78" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="BA78" s="2" t="s">
         <v>43</v>
@@ -12369,7 +12381,7 @@
       <c r="BH78" s="2"/>
       <c r="BI78" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ78" s="8" t="s">
         <v>327</v>
@@ -12377,13 +12389,13 @@
     </row>
     <row r="79" spans="1:62" ht="42" x14ac:dyDescent="0.15">
       <c r="A79" s="6" t="s">
+        <v>599</v>
+      </c>
+      <c r="B79" s="2" t="s">
         <v>600</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="C79" s="3" t="s">
         <v>601</v>
-      </c>
-      <c r="C79" s="3" t="s">
-        <v>602</v>
       </c>
       <c r="D79" s="3" t="s">
         <v>34</v>
@@ -12414,40 +12426,40 @@
         <v>12</v>
       </c>
       <c r="N79" s="3" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="O79" s="3" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="P79" s="28"/>
       <c r="Q79" s="6">
         <v>12611737</v>
       </c>
       <c r="R79" s="17" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="S79" s="3" t="s">
         <v>40</v>
       </c>
       <c r="T79" s="3" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="U79" s="3" t="s">
         <v>479</v>
       </c>
       <c r="V79" s="8" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="W79" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="X79" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y79" s="2"/>
       <c r="Z79" s="2"/>
       <c r="AA79" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="AC79" s="2"/>
       <c r="AD79" s="2"/>
@@ -12487,7 +12499,7 @@
       <c r="BH79" s="2"/>
       <c r="BI79" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ79" s="8" t="s">
         <v>327</v>
@@ -12495,13 +12507,13 @@
     </row>
     <row r="80" spans="1:62" ht="56" x14ac:dyDescent="0.15">
       <c r="A80" s="6" t="s">
+        <v>612</v>
+      </c>
+      <c r="B80" s="6" t="s">
         <v>613</v>
       </c>
-      <c r="B80" s="6" t="s">
-        <v>614</v>
-      </c>
       <c r="C80" s="6" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="D80" s="6" t="s">
         <v>34</v>
@@ -12519,7 +12531,7 @@
         <v>44075</v>
       </c>
       <c r="I80" s="8" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="J80" s="16">
         <v>44075</v>
@@ -12549,19 +12561,19 @@
         <v>478</v>
       </c>
       <c r="U80" s="6" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="V80" s="8" t="s">
         <v>480</v>
       </c>
       <c r="W80" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="X80" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="AA80" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="BA80" s="2" t="s">
         <v>43</v>
@@ -12581,7 +12593,7 @@
       <c r="BH80" s="2"/>
       <c r="BI80" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ80" s="8" t="s">
         <v>327</v>
@@ -12589,13 +12601,13 @@
     </row>
     <row r="81" spans="1:62" ht="126" x14ac:dyDescent="0.15">
       <c r="A81" s="6" t="s">
+        <v>617</v>
+      </c>
+      <c r="B81" s="6" t="s">
+        <v>619</v>
+      </c>
+      <c r="C81" s="6" t="s">
         <v>618</v>
-      </c>
-      <c r="B81" s="6" t="s">
-        <v>620</v>
-      </c>
-      <c r="C81" s="6" t="s">
-        <v>619</v>
       </c>
       <c r="D81" s="6" t="s">
         <v>34</v>
@@ -12650,56 +12662,56 @@
         <v>485</v>
       </c>
       <c r="W81" s="35" t="s">
+        <v>621</v>
+      </c>
+      <c r="X81" s="32" t="s">
+        <v>530</v>
+      </c>
+      <c r="AA81" s="6" t="s">
+        <v>620</v>
+      </c>
+      <c r="AB81" s="32" t="s">
+        <v>531</v>
+      </c>
+      <c r="AC81" s="32" t="s">
         <v>622</v>
       </c>
-      <c r="X81" s="32" t="s">
+      <c r="AD81" s="32" t="s">
+        <v>530</v>
+      </c>
+      <c r="AG81" s="32" t="s">
+        <v>623</v>
+      </c>
+      <c r="AH81" s="32" t="s">
         <v>531</v>
-      </c>
-      <c r="AA81" s="6" t="s">
-        <v>621</v>
-      </c>
-      <c r="AB81" s="32" t="s">
-        <v>532</v>
-      </c>
-      <c r="AC81" s="32" t="s">
-        <v>623</v>
-      </c>
-      <c r="AD81" s="32" t="s">
-        <v>531</v>
-      </c>
-      <c r="AG81" s="32" t="s">
-        <v>624</v>
-      </c>
-      <c r="AH81" s="32" t="s">
-        <v>532</v>
       </c>
       <c r="AI81" s="19" t="s">
         <v>40</v>
       </c>
       <c r="AJ81" s="19" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="AK81" s="19"/>
       <c r="AL81" s="19"/>
       <c r="AM81" s="12" t="s">
+        <v>529</v>
+      </c>
+      <c r="AN81" s="12" t="s">
+        <v>531</v>
+      </c>
+      <c r="AO81" s="19" t="s">
+        <v>589</v>
+      </c>
+      <c r="AP81" s="19" t="s">
         <v>530</v>
-      </c>
-      <c r="AN81" s="12" t="s">
-        <v>532</v>
-      </c>
-      <c r="AO81" s="19" t="s">
-        <v>590</v>
-      </c>
-      <c r="AP81" s="19" t="s">
-        <v>531</v>
       </c>
       <c r="AQ81" s="19"/>
       <c r="AR81" s="19"/>
       <c r="AS81" s="19" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="AT81" s="19" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="BA81" s="19" t="s">
         <v>43</v>
@@ -12715,7 +12727,7 @@
       </c>
       <c r="BI81" s="33">
         <f t="shared" ca="1" si="3"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ81" s="34" t="s">
         <v>327</v>
@@ -12723,13 +12735,13 @@
     </row>
     <row r="82" spans="1:62" ht="56" x14ac:dyDescent="0.15">
       <c r="A82" s="32" t="s">
+        <v>624</v>
+      </c>
+      <c r="B82" s="32" t="s">
+        <v>626</v>
+      </c>
+      <c r="C82" s="32" t="s">
         <v>625</v>
-      </c>
-      <c r="B82" s="32" t="s">
-        <v>627</v>
-      </c>
-      <c r="C82" s="32" t="s">
-        <v>626</v>
       </c>
       <c r="D82" s="32" t="s">
         <v>34</v>
@@ -12786,15 +12798,15 @@
         <v>308</v>
       </c>
       <c r="W82" s="19" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="X82" s="19" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y82" s="19"/>
       <c r="Z82" s="19"/>
       <c r="AA82" s="12" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="BA82" s="19" t="s">
         <v>43</v>
@@ -12814,7 +12826,7 @@
       <c r="BH82" s="19"/>
       <c r="BI82" s="33">
         <f t="shared" ca="1" si="3"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ82" s="34" t="s">
         <v>327</v>
@@ -12822,13 +12834,13 @@
     </row>
     <row r="83" spans="1:62" ht="42" x14ac:dyDescent="0.15">
       <c r="A83" s="3" t="s">
+        <v>627</v>
+      </c>
+      <c r="B83" s="6" t="s">
+        <v>629</v>
+      </c>
+      <c r="C83" s="6" t="s">
         <v>628</v>
-      </c>
-      <c r="B83" s="6" t="s">
-        <v>630</v>
-      </c>
-      <c r="C83" s="6" t="s">
-        <v>629</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>34</v>
@@ -12862,7 +12874,7 @@
         <v>244</v>
       </c>
       <c r="O83" s="2" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="P83" s="15" t="s">
         <v>245</v>
@@ -12871,30 +12883,30 @@
         <v>246</v>
       </c>
       <c r="R83" s="2" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="S83" s="2" t="s">
         <v>40</v>
       </c>
       <c r="T83" s="2" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="U83" s="2" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="V83" s="7" t="s">
         <v>249</v>
       </c>
       <c r="W83" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="X83" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y83" s="2"/>
       <c r="Z83" s="2"/>
       <c r="AA83" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="AC83" s="2"/>
       <c r="AD83" s="2"/>
@@ -12934,7 +12946,7 @@
       <c r="BH83" s="2"/>
       <c r="BI83" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ83" s="8" t="s">
         <v>327</v>
@@ -12942,13 +12954,13 @@
     </row>
     <row r="84" spans="1:62" ht="56" x14ac:dyDescent="0.15">
       <c r="A84" s="2" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B84" s="6" t="s">
         <v>510</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="D84" s="6" t="s">
         <v>34</v>
@@ -13005,13 +13017,13 @@
         <v>508</v>
       </c>
       <c r="W84" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="X84" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="AA84" s="6" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="BA84" s="2" t="s">
         <v>43</v>
@@ -13031,7 +13043,7 @@
       <c r="BH84" s="2"/>
       <c r="BI84" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ84" s="8" t="s">
         <v>327</v>
@@ -13039,13 +13051,13 @@
     </row>
     <row r="85" spans="1:62" ht="28" x14ac:dyDescent="0.15">
       <c r="A85" s="2" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>34</v>
@@ -13103,46 +13115,46 @@
         <v>323</v>
       </c>
       <c r="W85" s="2" t="s">
+        <v>558</v>
+      </c>
+      <c r="X85" s="2" t="s">
         <v>559</v>
-      </c>
-      <c r="X85" s="2" t="s">
-        <v>560</v>
       </c>
       <c r="Y85" s="2"/>
       <c r="Z85" s="2"/>
       <c r="AC85" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="AD85" s="2" t="s">
         <v>561</v>
-      </c>
-      <c r="AD85" s="2" t="s">
-        <v>562</v>
       </c>
       <c r="AE85" s="2"/>
       <c r="AF85" s="2"/>
       <c r="AG85" s="2"/>
       <c r="AH85" s="2"/>
       <c r="AI85" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="AJ85" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="AK85" s="2"/>
       <c r="AL85" s="2"/>
       <c r="AO85" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="AP85" s="2" t="s">
         <v>535</v>
-      </c>
-      <c r="AP85" s="2" t="s">
-        <v>536</v>
       </c>
       <c r="AQ85" s="2"/>
       <c r="AR85" s="2"/>
       <c r="AS85" s="2"/>
       <c r="AT85" s="2"/>
       <c r="AU85" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="AV85" s="2" t="s">
         <v>581</v>
-      </c>
-      <c r="AV85" s="2" t="s">
-        <v>582</v>
       </c>
       <c r="AW85" s="2"/>
       <c r="AX85" s="2"/>
@@ -13166,7 +13178,7 @@
       <c r="BH85" s="2"/>
       <c r="BI85" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ85" s="8" t="s">
         <v>327</v>
@@ -13174,13 +13186,13 @@
     </row>
     <row r="86" spans="1:62" ht="98" x14ac:dyDescent="0.15">
       <c r="A86" s="2" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B86" s="39" t="s">
+        <v>638</v>
+      </c>
+      <c r="C86" s="2" t="s">
         <v>639</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>640</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>34</v>
@@ -13238,15 +13250,15 @@
         <v>371</v>
       </c>
       <c r="W86" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="X86" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y86" s="2"/>
       <c r="Z86" s="2"/>
       <c r="AA86" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="AC86" s="2"/>
       <c r="AD86" s="2"/>
@@ -13286,7 +13298,7 @@
       <c r="BH86" s="2"/>
       <c r="BI86" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ86" s="8" t="s">
         <v>327</v>
@@ -13294,7 +13306,7 @@
     </row>
     <row r="87" spans="1:62" ht="56" x14ac:dyDescent="0.15">
       <c r="A87" s="2" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>433</v>
@@ -13361,12 +13373,12 @@
         <v>40</v>
       </c>
       <c r="X87" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="Y87" s="2"/>
       <c r="Z87" s="2"/>
       <c r="AA87" s="6" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="AC87" s="2"/>
       <c r="AD87" s="2"/>
@@ -13402,7 +13414,7 @@
       <c r="BH87" s="2"/>
       <c r="BI87" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ87" s="8" t="s">
         <v>327</v>
@@ -13410,13 +13422,13 @@
     </row>
     <row r="88" spans="1:62" ht="84" x14ac:dyDescent="0.15">
       <c r="A88" s="2" t="s">
+        <v>640</v>
+      </c>
+      <c r="B88" s="3" t="s">
         <v>641</v>
       </c>
-      <c r="B88" s="3" t="s">
-        <v>642</v>
-      </c>
       <c r="C88" s="2" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>34</v>
@@ -13434,7 +13446,7 @@
         <v>44287</v>
       </c>
       <c r="I88" s="8" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="J88" s="16">
         <v>44287</v>
@@ -13447,32 +13459,32 @@
         <v>12</v>
       </c>
       <c r="N88" s="2" t="s">
+        <v>643</v>
+      </c>
+      <c r="O88" s="3" t="s">
         <v>644</v>
-      </c>
-      <c r="O88" s="3" t="s">
-        <v>645</v>
       </c>
       <c r="P88" s="15"/>
       <c r="Q88" s="15" t="s">
+        <v>646</v>
+      </c>
+      <c r="R88" s="2" t="s">
         <v>647</v>
       </c>
-      <c r="R88" s="2" t="s">
+      <c r="S88" s="2" t="s">
         <v>648</v>
       </c>
-      <c r="S88" s="2" t="s">
+      <c r="T88" s="2" t="s">
         <v>649</v>
       </c>
-      <c r="T88" s="2" t="s">
+      <c r="U88" s="3" t="s">
         <v>650</v>
       </c>
-      <c r="U88" s="3" t="s">
-        <v>651</v>
-      </c>
       <c r="V88" s="8" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="W88" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="X88" s="2"/>
       <c r="Y88" s="2"/>
@@ -13515,9 +13527,107 @@
       <c r="BH88" s="2"/>
       <c r="BI88" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44302.781457291669</v>
+        <v>44330.826532060186</v>
       </c>
       <c r="BJ88" s="8" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="89" spans="1:62" ht="70" x14ac:dyDescent="0.15">
+      <c r="A89" s="2" t="s">
+        <v>651</v>
+      </c>
+      <c r="B89" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="C89" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="D89" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E89" s="6">
+        <v>35000</v>
+      </c>
+      <c r="F89" s="6">
+        <v>35000</v>
+      </c>
+      <c r="G89" s="6">
+        <v>35000</v>
+      </c>
+      <c r="H89" s="16">
+        <v>44287</v>
+      </c>
+      <c r="I89" s="8" t="s">
+        <v>521</v>
+      </c>
+      <c r="J89" s="16">
+        <v>44287</v>
+      </c>
+      <c r="K89" s="16">
+        <v>44652</v>
+      </c>
+      <c r="L89" s="16"/>
+      <c r="M89" s="6">
+        <v>12</v>
+      </c>
+      <c r="N89" s="6" t="s">
+        <v>652</v>
+      </c>
+      <c r="O89" s="6" t="s">
+        <v>502</v>
+      </c>
+      <c r="P89" s="6">
+        <v>1189812</v>
+      </c>
+      <c r="Q89" s="15" t="s">
+        <v>523</v>
+      </c>
+      <c r="R89" s="6" t="s">
+        <v>524</v>
+      </c>
+      <c r="S89" s="6" t="s">
+        <v>525</v>
+      </c>
+      <c r="T89" s="6" t="s">
+        <v>526</v>
+      </c>
+      <c r="U89" s="6" t="s">
+        <v>653</v>
+      </c>
+      <c r="V89" s="8" t="s">
+        <v>521</v>
+      </c>
+      <c r="W89" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="X89" s="2" t="s">
+        <v>530</v>
+      </c>
+      <c r="AA89" s="6" t="s">
+        <v>541</v>
+      </c>
+      <c r="BA89" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="BB89" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="BC89" s="2"/>
+      <c r="BD89" s="2"/>
+      <c r="BE89" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="BF89" s="2"/>
+      <c r="BG89" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="BH89" s="2"/>
+      <c r="BI89" s="18">
+        <f t="shared" ca="1" si="3"/>
+        <v>44330.826532060186</v>
+      </c>
+      <c r="BJ89" s="8" t="s">
         <v>327</v>
       </c>
     </row>
@@ -13665,8 +13775,11 @@
     <hyperlink ref="I88" r:id="rId138" xr:uid="{7D68488F-A43B-AE43-AE9F-143DD94A0FCF}"/>
     <hyperlink ref="V88" r:id="rId139" xr:uid="{4D13C756-0C91-E446-AA2D-61D67EAC0A85}"/>
     <hyperlink ref="BJ88" r:id="rId140" xr:uid="{8F94CCD7-FAE8-474E-A7F6-65692D57572C}"/>
+    <hyperlink ref="BJ89" r:id="rId141" xr:uid="{B5962B40-521B-6E48-8E4E-03CBC5EC10E5}"/>
+    <hyperlink ref="I89" r:id="rId142" xr:uid="{2E84DC81-1217-FB4C-BD66-0B2497A04FEF}"/>
+    <hyperlink ref="V89" r:id="rId143" xr:uid="{2E335074-DC5E-9647-92F0-33F6B8E71A09}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId141"/>
+  <legacyDrawing r:id="rId144"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Publish 360 Giving Update
Reconnect London grant.
</commit_message>
<xml_diff>
--- a/open/grants.xlsx
+++ b/open/grants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/westsi/Documents/GitHub/zing/open/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E554CD-75B4-074E-A4A7-46872BF96FBE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{832B864A-648F-7743-A25F-4B52B3F91475}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="460" yWindow="700" windowWidth="33140" windowHeight="20300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2192" uniqueCount="656">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2214" uniqueCount="660">
   <si>
     <t>Identifier</t>
   </si>
@@ -2038,6 +2038,20 @@
   </si>
   <si>
     <t>Learning with Parents are establishing themselves as the thought and action leader on embedding parental engagement in all aspects of school curriculum. To cope with increased demand on their services, our last round of funding supported the hiring of a CTO, and improvements to the back-end platform (in response to sudden increased demand during Covid-19 lockdowns), with further in-kind support under our digital stream. The team have since rebuilt their back-end platform, and this funding round is toward to its continued development, related digital projects, and other core costs.</t>
+  </si>
+  <si>
+    <t>360G-zing-96</t>
+  </si>
+  <si>
+    <t>https://www.reconnectlondon.org/</t>
+  </si>
+  <si>
+    <t>Funding toward the startup of Reconnect London</t>
+  </si>
+  <si>
+    <t>Incubated by The Difference, London Reconnect is a collaborative group of London-wide school system-leaders, who have joined together to address learning loss caused by the Covid-19 pandemic. The network spans the system. Local authority, foundation and MAT schools as well as government, philanthropists, corporate and third sector organisations are driven by a pledge: to quickly bring about change for disadvantaged and vulnerable young Londoners and make up lost ground in the wake of the pandemic. 
+Hundreds of thousands of Londonʼs children have faced food poverty and fallen on the wrong side of the digital divide. Hungry, and struggling to access education online, social isolation has worsened the picture. Serious mental health problems have risen during the pandemic; as have domestic violence reports, and reports of teenage criminal exploitation.
+This funding is unrestricted, including funding toward a project director.</t>
   </si>
 </sst>
 </file>
@@ -2588,13 +2602,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:BJ89"/>
+  <dimension ref="A1:BJ90"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="120" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A90" sqref="A90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2964,7 +2978,7 @@
       <c r="BH2" s="2"/>
       <c r="BI2" s="18">
         <f t="shared" ref="BI2:BI33" ca="1" si="0">NOW()</f>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ2" s="8" t="s">
         <v>327</v>
@@ -3089,7 +3103,7 @@
       <c r="BH3" s="2"/>
       <c r="BI3" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ3" s="8" t="s">
         <v>327</v>
@@ -3217,7 +3231,7 @@
       <c r="BH4" s="2"/>
       <c r="BI4" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ4" s="8" t="s">
         <v>327</v>
@@ -3341,7 +3355,7 @@
       <c r="BH5" s="2"/>
       <c r="BI5" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ5" s="8" t="s">
         <v>327</v>
@@ -3469,7 +3483,7 @@
       <c r="BH6" s="2"/>
       <c r="BI6" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ6" s="8" t="s">
         <v>327</v>
@@ -3597,7 +3611,7 @@
       <c r="BH7" s="2"/>
       <c r="BI7" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ7" s="8" t="s">
         <v>327</v>
@@ -3726,7 +3740,7 @@
       <c r="BH8" s="2"/>
       <c r="BI8" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ8" s="8" t="s">
         <v>327</v>
@@ -3851,7 +3865,7 @@
       <c r="BH9" s="2"/>
       <c r="BI9" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ9" s="8" t="s">
         <v>327</v>
@@ -3956,7 +3970,7 @@
       <c r="BH10" s="2"/>
       <c r="BI10" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ10" s="8" t="s">
         <v>327</v>
@@ -4077,7 +4091,7 @@
       <c r="BH11" s="2"/>
       <c r="BI11" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ11" s="8" t="s">
         <v>327</v>
@@ -4204,7 +4218,7 @@
       <c r="BH12" s="2"/>
       <c r="BI12" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ12" s="8" t="s">
         <v>327</v>
@@ -4331,7 +4345,7 @@
       <c r="BH13" s="2"/>
       <c r="BI13" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ13" s="8" t="s">
         <v>327</v>
@@ -4460,7 +4474,7 @@
       <c r="BH14" s="2"/>
       <c r="BI14" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ14" s="8" t="s">
         <v>327</v>
@@ -4585,7 +4599,7 @@
       <c r="BH15" s="2"/>
       <c r="BI15" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ15" s="8" t="s">
         <v>327</v>
@@ -4710,7 +4724,7 @@
       <c r="BH16" s="2"/>
       <c r="BI16" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ16" s="8" t="s">
         <v>327</v>
@@ -4839,7 +4853,7 @@
       <c r="BH17" s="2"/>
       <c r="BI17" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ17" s="8" t="s">
         <v>327</v>
@@ -4968,7 +4982,7 @@
       <c r="BH18" s="2"/>
       <c r="BI18" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ18" s="8" t="s">
         <v>327</v>
@@ -5089,7 +5103,7 @@
       <c r="BH19" s="2"/>
       <c r="BI19" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ19" s="8" t="s">
         <v>327</v>
@@ -5216,7 +5230,7 @@
       <c r="BH20" s="2"/>
       <c r="BI20" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ20" s="8" t="s">
         <v>327</v>
@@ -5345,7 +5359,7 @@
       <c r="BH21" s="2"/>
       <c r="BI21" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ21" s="8" t="s">
         <v>327</v>
@@ -5472,7 +5486,7 @@
       <c r="BH22" s="2"/>
       <c r="BI22" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ22" s="8" t="s">
         <v>327</v>
@@ -5601,7 +5615,7 @@
       <c r="BH23" s="2"/>
       <c r="BI23" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ23" s="8" t="s">
         <v>327</v>
@@ -5726,7 +5740,7 @@
       <c r="BH24" s="2"/>
       <c r="BI24" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ24" s="8" t="s">
         <v>327</v>
@@ -5847,7 +5861,7 @@
       <c r="BH25" s="2"/>
       <c r="BI25" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ25" s="8" t="s">
         <v>327</v>
@@ -5974,7 +5988,7 @@
       <c r="BH26" s="2"/>
       <c r="BI26" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ26" s="8" t="s">
         <v>327</v>
@@ -6103,7 +6117,7 @@
       <c r="BH27" s="2"/>
       <c r="BI27" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ27" s="8" t="s">
         <v>327</v>
@@ -6228,7 +6242,7 @@
       <c r="BH28" s="2"/>
       <c r="BI28" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ28" s="8" t="s">
         <v>327</v>
@@ -6355,7 +6369,7 @@
       <c r="BH29" s="2"/>
       <c r="BI29" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ29" s="8" t="s">
         <v>327</v>
@@ -6480,7 +6494,7 @@
       <c r="BH30" s="2"/>
       <c r="BI30" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ30" s="8" t="s">
         <v>327</v>
@@ -6607,7 +6621,7 @@
       <c r="BH31" s="2"/>
       <c r="BI31" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ31" s="8" t="s">
         <v>327</v>
@@ -6734,7 +6748,7 @@
       <c r="BH32" s="2"/>
       <c r="BI32" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ32" s="8" t="s">
         <v>327</v>
@@ -6861,7 +6875,7 @@
       <c r="BH33" s="2"/>
       <c r="BI33" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ33" s="8" t="s">
         <v>327</v>
@@ -7002,7 +7016,7 @@
       <c r="BH34" s="2"/>
       <c r="BI34" s="18">
         <f t="shared" ref="BI34:BI65" ca="1" si="1">NOW()</f>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ34" s="8" t="s">
         <v>327</v>
@@ -7123,7 +7137,7 @@
       <c r="BH35" s="2"/>
       <c r="BI35" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ35" s="8" t="s">
         <v>327</v>
@@ -7248,7 +7262,7 @@
       <c r="BH36" s="2"/>
       <c r="BI36" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ36" s="8" t="s">
         <v>327</v>
@@ -7379,7 +7393,7 @@
       <c r="BH37" s="2"/>
       <c r="BI37" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ37" s="8" t="s">
         <v>327</v>
@@ -7506,7 +7520,7 @@
       <c r="BH38" s="2"/>
       <c r="BI38" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ38" s="8" t="s">
         <v>327</v>
@@ -7635,7 +7649,7 @@
       <c r="BH39" s="2"/>
       <c r="BI39" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ39" s="8" t="s">
         <v>327</v>
@@ -7764,7 +7778,7 @@
       <c r="BH40" s="2"/>
       <c r="BI40" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ40" s="8" t="s">
         <v>327</v>
@@ -7891,7 +7905,7 @@
       <c r="BH41" s="2"/>
       <c r="BI41" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ41" s="8" t="s">
         <v>327</v>
@@ -8028,7 +8042,7 @@
       <c r="BH42" s="2"/>
       <c r="BI42" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ42" s="8" t="s">
         <v>327</v>
@@ -8147,7 +8161,7 @@
       <c r="BH43" s="2"/>
       <c r="BI43" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ43" s="8" t="s">
         <v>327</v>
@@ -8267,7 +8281,7 @@
       <c r="BH44" s="2"/>
       <c r="BI44" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ44" s="8" t="s">
         <v>327</v>
@@ -8389,7 +8403,7 @@
       <c r="BH45" s="2"/>
       <c r="BI45" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ45" s="8" t="s">
         <v>327</v>
@@ -8509,7 +8523,7 @@
       <c r="BH46" s="2"/>
       <c r="BI46" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ46" s="8" t="s">
         <v>327</v>
@@ -8631,7 +8645,7 @@
       <c r="BH47" s="2"/>
       <c r="BI47" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ47" s="8" t="s">
         <v>327</v>
@@ -8751,7 +8765,7 @@
       <c r="BH48" s="2"/>
       <c r="BI48" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ48" s="8" t="s">
         <v>327</v>
@@ -8873,7 +8887,7 @@
       <c r="BH49" s="2"/>
       <c r="BI49" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ49" s="8" t="s">
         <v>327</v>
@@ -8995,7 +9009,7 @@
       <c r="BH50" s="2"/>
       <c r="BI50" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ50" s="8" t="s">
         <v>327</v>
@@ -9115,7 +9129,7 @@
       <c r="BH51" s="2"/>
       <c r="BI51" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ51" s="8" t="s">
         <v>327</v>
@@ -9237,7 +9251,7 @@
       <c r="BH52" s="2"/>
       <c r="BI52" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ52" s="8" t="s">
         <v>327</v>
@@ -9359,7 +9373,7 @@
       <c r="BH53" s="2"/>
       <c r="BI53" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ53" s="8" t="s">
         <v>327</v>
@@ -9485,7 +9499,7 @@
       </c>
       <c r="BI54" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ54" s="8" t="s">
         <v>327</v>
@@ -9612,7 +9626,7 @@
       <c r="BH55" s="24"/>
       <c r="BI55" s="24">
         <f t="shared" ca="1" si="1"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ55" s="8" t="s">
         <v>327</v>
@@ -9749,7 +9763,7 @@
       <c r="BH56" s="24"/>
       <c r="BI56" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ56" s="8" t="s">
         <v>327</v>
@@ -9871,7 +9885,7 @@
       <c r="BH57" s="2"/>
       <c r="BI57" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ57" s="8" t="s">
         <v>327</v>
@@ -9991,7 +10005,7 @@
       <c r="BH58" s="2"/>
       <c r="BI58" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ58" s="8" t="s">
         <v>327</v>
@@ -10113,7 +10127,7 @@
       <c r="BH59" s="2"/>
       <c r="BI59" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ59" s="8" t="s">
         <v>327</v>
@@ -10250,7 +10264,7 @@
       <c r="BH60" s="2"/>
       <c r="BI60" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ60" s="8" t="s">
         <v>327</v>
@@ -10365,7 +10379,7 @@
       <c r="BH61" s="2"/>
       <c r="BI61" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ61" s="8" t="s">
         <v>327</v>
@@ -10485,7 +10499,7 @@
       <c r="BH62" s="2"/>
       <c r="BI62" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ62" s="8" t="s">
         <v>327</v>
@@ -10605,7 +10619,7 @@
       <c r="BH63" s="2"/>
       <c r="BI63" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ63" s="8" t="s">
         <v>327</v>
@@ -10727,7 +10741,7 @@
       <c r="BH64" s="2"/>
       <c r="BI64" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ64" s="8" t="s">
         <v>327</v>
@@ -10852,7 +10866,7 @@
       <c r="BH65" s="2"/>
       <c r="BI65" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ65" s="8" t="s">
         <v>327</v>
@@ -10974,7 +10988,7 @@
       <c r="BH66" s="2"/>
       <c r="BI66" s="18">
         <f t="shared" ref="BI66:BI71" ca="1" si="2">NOW()</f>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ66" s="8" t="s">
         <v>327</v>
@@ -11111,7 +11125,7 @@
       <c r="BH67" s="2"/>
       <c r="BI67" s="18">
         <f t="shared" ca="1" si="2"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ67" s="8" t="s">
         <v>327</v>
@@ -11226,7 +11240,7 @@
       <c r="BH68" s="2"/>
       <c r="BI68" s="18">
         <f t="shared" ca="1" si="2"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ68" s="8" t="s">
         <v>327</v>
@@ -11345,7 +11359,7 @@
       <c r="BH69" s="2"/>
       <c r="BI69" s="18">
         <f t="shared" ca="1" si="2"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ69" s="8" t="s">
         <v>327</v>
@@ -11467,7 +11481,7 @@
       <c r="BH70" s="19"/>
       <c r="BI70" s="33">
         <f t="shared" ca="1" si="2"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ70" s="34" t="s">
         <v>327</v>
@@ -11598,7 +11612,7 @@
       <c r="BH71" s="19"/>
       <c r="BI71" s="33">
         <f t="shared" ca="1" si="2"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ71" s="34" t="s">
         <v>327</v>
@@ -11717,8 +11731,8 @@
       </c>
       <c r="BH72" s="2"/>
       <c r="BI72" s="18">
-        <f t="shared" ref="BI72:BI89" ca="1" si="3">NOW()</f>
-        <v>44330.826532060186</v>
+        <f t="shared" ref="BI72:BI90" ca="1" si="3">NOW()</f>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ72" s="8" t="s">
         <v>327</v>
@@ -11818,7 +11832,7 @@
       <c r="BH73" s="2"/>
       <c r="BI73" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ73" s="8" t="s">
         <v>327</v>
@@ -11940,7 +11954,7 @@
       <c r="BH74" s="2"/>
       <c r="BI74" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ74" s="8" t="s">
         <v>327</v>
@@ -12055,7 +12069,7 @@
       <c r="BH75" s="2"/>
       <c r="BI75" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ75" s="8" t="s">
         <v>327</v>
@@ -12152,7 +12166,7 @@
       <c r="BH76" s="2"/>
       <c r="BI76" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ76" s="8" t="s">
         <v>327</v>
@@ -12289,7 +12303,7 @@
       <c r="BH77" s="2"/>
       <c r="BI77" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ77" s="8" t="s">
         <v>327</v>
@@ -12381,7 +12395,7 @@
       <c r="BH78" s="2"/>
       <c r="BI78" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ78" s="8" t="s">
         <v>327</v>
@@ -12499,7 +12513,7 @@
       <c r="BH79" s="2"/>
       <c r="BI79" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ79" s="8" t="s">
         <v>327</v>
@@ -12593,7 +12607,7 @@
       <c r="BH80" s="2"/>
       <c r="BI80" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ80" s="8" t="s">
         <v>327</v>
@@ -12727,7 +12741,7 @@
       </c>
       <c r="BI81" s="33">
         <f t="shared" ca="1" si="3"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ81" s="34" t="s">
         <v>327</v>
@@ -12826,7 +12840,7 @@
       <c r="BH82" s="19"/>
       <c r="BI82" s="33">
         <f t="shared" ca="1" si="3"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ82" s="34" t="s">
         <v>327</v>
@@ -12946,7 +12960,7 @@
       <c r="BH83" s="2"/>
       <c r="BI83" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ83" s="8" t="s">
         <v>327</v>
@@ -13043,7 +13057,7 @@
       <c r="BH84" s="2"/>
       <c r="BI84" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ84" s="8" t="s">
         <v>327</v>
@@ -13178,7 +13192,7 @@
       <c r="BH85" s="2"/>
       <c r="BI85" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ85" s="8" t="s">
         <v>327</v>
@@ -13298,7 +13312,7 @@
       <c r="BH86" s="2"/>
       <c r="BI86" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ86" s="8" t="s">
         <v>327</v>
@@ -13414,7 +13428,7 @@
       <c r="BH87" s="2"/>
       <c r="BI87" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ87" s="8" t="s">
         <v>327</v>
@@ -13527,7 +13541,7 @@
       <c r="BH88" s="2"/>
       <c r="BI88" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ88" s="8" t="s">
         <v>327</v>
@@ -13625,9 +13639,108 @@
       <c r="BH89" s="2"/>
       <c r="BI89" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44330.826532060186</v>
+        <v>44341.506390972223</v>
       </c>
       <c r="BJ89" s="8" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="90" spans="1:62" ht="140" x14ac:dyDescent="0.15">
+      <c r="A90" s="2" t="s">
+        <v>656</v>
+      </c>
+      <c r="B90" s="6" t="s">
+        <v>658</v>
+      </c>
+      <c r="C90" s="6" t="s">
+        <v>659</v>
+      </c>
+      <c r="D90" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E90" s="6">
+        <v>20000</v>
+      </c>
+      <c r="F90" s="6">
+        <v>20000</v>
+      </c>
+      <c r="G90" s="6">
+        <v>20000</v>
+      </c>
+      <c r="H90" s="36">
+        <v>44228</v>
+      </c>
+      <c r="I90" s="34" t="s">
+        <v>657</v>
+      </c>
+      <c r="J90" s="36">
+        <v>44348</v>
+      </c>
+      <c r="K90" s="36">
+        <v>44713</v>
+      </c>
+      <c r="M90" s="6">
+        <v>12</v>
+      </c>
+      <c r="N90" s="5" t="s">
+        <v>467</v>
+      </c>
+      <c r="O90" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="P90" s="29" t="s">
+        <v>466</v>
+      </c>
+      <c r="Q90" s="37" t="s">
+        <v>469</v>
+      </c>
+      <c r="R90" s="5" t="s">
+        <v>471</v>
+      </c>
+      <c r="S90" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="T90" s="5" t="s">
+        <v>470</v>
+      </c>
+      <c r="U90" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="V90" s="34" t="s">
+        <v>308</v>
+      </c>
+      <c r="W90" s="19" t="s">
+        <v>545</v>
+      </c>
+      <c r="X90" s="19" t="s">
+        <v>530</v>
+      </c>
+      <c r="Y90" s="19"/>
+      <c r="Z90" s="19"/>
+      <c r="AA90" s="12" t="s">
+        <v>541</v>
+      </c>
+      <c r="BA90" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="BB90" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="BC90" s="19"/>
+      <c r="BD90" s="19"/>
+      <c r="BE90" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="BF90" s="19"/>
+      <c r="BG90" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="BH90" s="19"/>
+      <c r="BI90" s="33">
+        <f t="shared" ca="1" si="3"/>
+        <v>44341.506390972223</v>
+      </c>
+      <c r="BJ90" s="34" t="s">
         <v>327</v>
       </c>
     </row>
@@ -13778,8 +13891,10 @@
     <hyperlink ref="BJ89" r:id="rId141" xr:uid="{B5962B40-521B-6E48-8E4E-03CBC5EC10E5}"/>
     <hyperlink ref="I89" r:id="rId142" xr:uid="{2E84DC81-1217-FB4C-BD66-0B2497A04FEF}"/>
     <hyperlink ref="V89" r:id="rId143" xr:uid="{2E335074-DC5E-9647-92F0-33F6B8E71A09}"/>
+    <hyperlink ref="V90" r:id="rId144" xr:uid="{F449B04D-237B-7546-BC43-6E3FC8872799}"/>
+    <hyperlink ref="BJ90" r:id="rId145" xr:uid="{F6A2BA07-9F11-2245-A9FE-ED659C43DEAC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId144"/>
+  <legacyDrawing r:id="rId146"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Publish new grants data
</commit_message>
<xml_diff>
--- a/open/grants.xlsx
+++ b/open/grants.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/westsi/Documents/GitHub/zing/open/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{832B864A-648F-7743-A25F-4B52B3F91475}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96F9B7A-1493-A04A-91A0-445C4DC7F351}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="460" yWindow="700" windowWidth="33140" windowHeight="20300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="grants" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">grants!$A$1:$BJ$87</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">grants!$A$1:$BJ$91</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2214" uniqueCount="660">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2236" uniqueCount="662">
   <si>
     <t>Identifier</t>
   </si>
@@ -2052,6 +2052,12 @@
     <t>Incubated by The Difference, London Reconnect is a collaborative group of London-wide school system-leaders, who have joined together to address learning loss caused by the Covid-19 pandemic. The network spans the system. Local authority, foundation and MAT schools as well as government, philanthropists, corporate and third sector organisations are driven by a pledge: to quickly bring about change for disadvantaged and vulnerable young Londoners and make up lost ground in the wake of the pandemic. 
 Hundreds of thousands of Londonʼs children have faced food poverty and fallen on the wrong side of the digital divide. Hungry, and struggling to access education online, social isolation has worsened the picture. Serious mental health problems have risen during the pandemic; as have domestic violence reports, and reports of teenage criminal exploitation.
 This funding is unrestricted, including funding toward a project director.</t>
+  </si>
+  <si>
+    <t>360G-zing-97</t>
+  </si>
+  <si>
+    <t>A third grant to support the core costs of recruitment, development and technology for the opening of Lighthouse's first children's home, planned for fall 2021.</t>
   </si>
 </sst>
 </file>
@@ -2602,13 +2608,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:BJ90"/>
+  <dimension ref="A1:BJ91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="120" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A90" sqref="A90"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2978,7 +2984,7 @@
       <c r="BH2" s="2"/>
       <c r="BI2" s="18">
         <f t="shared" ref="BI2:BI33" ca="1" si="0">NOW()</f>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ2" s="8" t="s">
         <v>327</v>
@@ -3103,7 +3109,7 @@
       <c r="BH3" s="2"/>
       <c r="BI3" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ3" s="8" t="s">
         <v>327</v>
@@ -3231,7 +3237,7 @@
       <c r="BH4" s="2"/>
       <c r="BI4" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ4" s="8" t="s">
         <v>327</v>
@@ -3355,7 +3361,7 @@
       <c r="BH5" s="2"/>
       <c r="BI5" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ5" s="8" t="s">
         <v>327</v>
@@ -3483,7 +3489,7 @@
       <c r="BH6" s="2"/>
       <c r="BI6" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ6" s="8" t="s">
         <v>327</v>
@@ -3611,7 +3617,7 @@
       <c r="BH7" s="2"/>
       <c r="BI7" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ7" s="8" t="s">
         <v>327</v>
@@ -3740,7 +3746,7 @@
       <c r="BH8" s="2"/>
       <c r="BI8" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ8" s="8" t="s">
         <v>327</v>
@@ -3865,7 +3871,7 @@
       <c r="BH9" s="2"/>
       <c r="BI9" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ9" s="8" t="s">
         <v>327</v>
@@ -3970,7 +3976,7 @@
       <c r="BH10" s="2"/>
       <c r="BI10" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ10" s="8" t="s">
         <v>327</v>
@@ -4091,7 +4097,7 @@
       <c r="BH11" s="2"/>
       <c r="BI11" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ11" s="8" t="s">
         <v>327</v>
@@ -4218,7 +4224,7 @@
       <c r="BH12" s="2"/>
       <c r="BI12" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ12" s="8" t="s">
         <v>327</v>
@@ -4345,7 +4351,7 @@
       <c r="BH13" s="2"/>
       <c r="BI13" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ13" s="8" t="s">
         <v>327</v>
@@ -4474,7 +4480,7 @@
       <c r="BH14" s="2"/>
       <c r="BI14" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ14" s="8" t="s">
         <v>327</v>
@@ -4599,7 +4605,7 @@
       <c r="BH15" s="2"/>
       <c r="BI15" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ15" s="8" t="s">
         <v>327</v>
@@ -4724,7 +4730,7 @@
       <c r="BH16" s="2"/>
       <c r="BI16" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ16" s="8" t="s">
         <v>327</v>
@@ -4853,7 +4859,7 @@
       <c r="BH17" s="2"/>
       <c r="BI17" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ17" s="8" t="s">
         <v>327</v>
@@ -4982,7 +4988,7 @@
       <c r="BH18" s="2"/>
       <c r="BI18" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ18" s="8" t="s">
         <v>327</v>
@@ -5103,7 +5109,7 @@
       <c r="BH19" s="2"/>
       <c r="BI19" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ19" s="8" t="s">
         <v>327</v>
@@ -5230,7 +5236,7 @@
       <c r="BH20" s="2"/>
       <c r="BI20" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ20" s="8" t="s">
         <v>327</v>
@@ -5359,7 +5365,7 @@
       <c r="BH21" s="2"/>
       <c r="BI21" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ21" s="8" t="s">
         <v>327</v>
@@ -5486,7 +5492,7 @@
       <c r="BH22" s="2"/>
       <c r="BI22" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ22" s="8" t="s">
         <v>327</v>
@@ -5615,7 +5621,7 @@
       <c r="BH23" s="2"/>
       <c r="BI23" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ23" s="8" t="s">
         <v>327</v>
@@ -5740,7 +5746,7 @@
       <c r="BH24" s="2"/>
       <c r="BI24" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ24" s="8" t="s">
         <v>327</v>
@@ -5861,7 +5867,7 @@
       <c r="BH25" s="2"/>
       <c r="BI25" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ25" s="8" t="s">
         <v>327</v>
@@ -5988,7 +5994,7 @@
       <c r="BH26" s="2"/>
       <c r="BI26" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ26" s="8" t="s">
         <v>327</v>
@@ -6117,7 +6123,7 @@
       <c r="BH27" s="2"/>
       <c r="BI27" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ27" s="8" t="s">
         <v>327</v>
@@ -6242,7 +6248,7 @@
       <c r="BH28" s="2"/>
       <c r="BI28" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ28" s="8" t="s">
         <v>327</v>
@@ -6369,7 +6375,7 @@
       <c r="BH29" s="2"/>
       <c r="BI29" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ29" s="8" t="s">
         <v>327</v>
@@ -6494,7 +6500,7 @@
       <c r="BH30" s="2"/>
       <c r="BI30" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ30" s="8" t="s">
         <v>327</v>
@@ -6621,7 +6627,7 @@
       <c r="BH31" s="2"/>
       <c r="BI31" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ31" s="8" t="s">
         <v>327</v>
@@ -6748,7 +6754,7 @@
       <c r="BH32" s="2"/>
       <c r="BI32" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ32" s="8" t="s">
         <v>327</v>
@@ -6875,7 +6881,7 @@
       <c r="BH33" s="2"/>
       <c r="BI33" s="18">
         <f t="shared" ca="1" si="0"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ33" s="8" t="s">
         <v>327</v>
@@ -7016,7 +7022,7 @@
       <c r="BH34" s="2"/>
       <c r="BI34" s="18">
         <f t="shared" ref="BI34:BI65" ca="1" si="1">NOW()</f>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ34" s="8" t="s">
         <v>327</v>
@@ -7137,7 +7143,7 @@
       <c r="BH35" s="2"/>
       <c r="BI35" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ35" s="8" t="s">
         <v>327</v>
@@ -7262,7 +7268,7 @@
       <c r="BH36" s="2"/>
       <c r="BI36" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ36" s="8" t="s">
         <v>327</v>
@@ -7393,7 +7399,7 @@
       <c r="BH37" s="2"/>
       <c r="BI37" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ37" s="8" t="s">
         <v>327</v>
@@ -7520,7 +7526,7 @@
       <c r="BH38" s="2"/>
       <c r="BI38" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ38" s="8" t="s">
         <v>327</v>
@@ -7649,7 +7655,7 @@
       <c r="BH39" s="2"/>
       <c r="BI39" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ39" s="8" t="s">
         <v>327</v>
@@ -7778,7 +7784,7 @@
       <c r="BH40" s="2"/>
       <c r="BI40" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ40" s="8" t="s">
         <v>327</v>
@@ -7905,7 +7911,7 @@
       <c r="BH41" s="2"/>
       <c r="BI41" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ41" s="8" t="s">
         <v>327</v>
@@ -8042,7 +8048,7 @@
       <c r="BH42" s="2"/>
       <c r="BI42" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ42" s="8" t="s">
         <v>327</v>
@@ -8161,7 +8167,7 @@
       <c r="BH43" s="2"/>
       <c r="BI43" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ43" s="8" t="s">
         <v>327</v>
@@ -8281,7 +8287,7 @@
       <c r="BH44" s="2"/>
       <c r="BI44" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ44" s="8" t="s">
         <v>327</v>
@@ -8403,7 +8409,7 @@
       <c r="BH45" s="2"/>
       <c r="BI45" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ45" s="8" t="s">
         <v>327</v>
@@ -8523,7 +8529,7 @@
       <c r="BH46" s="2"/>
       <c r="BI46" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ46" s="8" t="s">
         <v>327</v>
@@ -8645,7 +8651,7 @@
       <c r="BH47" s="2"/>
       <c r="BI47" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ47" s="8" t="s">
         <v>327</v>
@@ -8765,7 +8771,7 @@
       <c r="BH48" s="2"/>
       <c r="BI48" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ48" s="8" t="s">
         <v>327</v>
@@ -8887,7 +8893,7 @@
       <c r="BH49" s="2"/>
       <c r="BI49" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ49" s="8" t="s">
         <v>327</v>
@@ -9009,7 +9015,7 @@
       <c r="BH50" s="2"/>
       <c r="BI50" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ50" s="8" t="s">
         <v>327</v>
@@ -9129,7 +9135,7 @@
       <c r="BH51" s="2"/>
       <c r="BI51" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ51" s="8" t="s">
         <v>327</v>
@@ -9251,7 +9257,7 @@
       <c r="BH52" s="2"/>
       <c r="BI52" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ52" s="8" t="s">
         <v>327</v>
@@ -9373,7 +9379,7 @@
       <c r="BH53" s="2"/>
       <c r="BI53" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ53" s="8" t="s">
         <v>327</v>
@@ -9499,7 +9505,7 @@
       </c>
       <c r="BI54" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ54" s="8" t="s">
         <v>327</v>
@@ -9626,7 +9632,7 @@
       <c r="BH55" s="24"/>
       <c r="BI55" s="24">
         <f t="shared" ca="1" si="1"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ55" s="8" t="s">
         <v>327</v>
@@ -9763,7 +9769,7 @@
       <c r="BH56" s="24"/>
       <c r="BI56" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ56" s="8" t="s">
         <v>327</v>
@@ -9885,7 +9891,7 @@
       <c r="BH57" s="2"/>
       <c r="BI57" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ57" s="8" t="s">
         <v>327</v>
@@ -10005,7 +10011,7 @@
       <c r="BH58" s="2"/>
       <c r="BI58" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ58" s="8" t="s">
         <v>327</v>
@@ -10127,7 +10133,7 @@
       <c r="BH59" s="2"/>
       <c r="BI59" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ59" s="8" t="s">
         <v>327</v>
@@ -10264,7 +10270,7 @@
       <c r="BH60" s="2"/>
       <c r="BI60" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ60" s="8" t="s">
         <v>327</v>
@@ -10379,7 +10385,7 @@
       <c r="BH61" s="2"/>
       <c r="BI61" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ61" s="8" t="s">
         <v>327</v>
@@ -10499,7 +10505,7 @@
       <c r="BH62" s="2"/>
       <c r="BI62" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ62" s="8" t="s">
         <v>327</v>
@@ -10619,7 +10625,7 @@
       <c r="BH63" s="2"/>
       <c r="BI63" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ63" s="8" t="s">
         <v>327</v>
@@ -10741,7 +10747,7 @@
       <c r="BH64" s="2"/>
       <c r="BI64" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ64" s="8" t="s">
         <v>327</v>
@@ -10866,7 +10872,7 @@
       <c r="BH65" s="2"/>
       <c r="BI65" s="18">
         <f t="shared" ca="1" si="1"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ65" s="8" t="s">
         <v>327</v>
@@ -10988,7 +10994,7 @@
       <c r="BH66" s="2"/>
       <c r="BI66" s="18">
         <f t="shared" ref="BI66:BI71" ca="1" si="2">NOW()</f>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ66" s="8" t="s">
         <v>327</v>
@@ -11125,7 +11131,7 @@
       <c r="BH67" s="2"/>
       <c r="BI67" s="18">
         <f t="shared" ca="1" si="2"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ67" s="8" t="s">
         <v>327</v>
@@ -11240,7 +11246,7 @@
       <c r="BH68" s="2"/>
       <c r="BI68" s="18">
         <f t="shared" ca="1" si="2"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ68" s="8" t="s">
         <v>327</v>
@@ -11359,7 +11365,7 @@
       <c r="BH69" s="2"/>
       <c r="BI69" s="18">
         <f t="shared" ca="1" si="2"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ69" s="8" t="s">
         <v>327</v>
@@ -11481,7 +11487,7 @@
       <c r="BH70" s="19"/>
       <c r="BI70" s="33">
         <f t="shared" ca="1" si="2"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ70" s="34" t="s">
         <v>327</v>
@@ -11612,7 +11618,7 @@
       <c r="BH71" s="19"/>
       <c r="BI71" s="33">
         <f t="shared" ca="1" si="2"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ71" s="34" t="s">
         <v>327</v>
@@ -11731,8 +11737,8 @@
       </c>
       <c r="BH72" s="2"/>
       <c r="BI72" s="18">
-        <f t="shared" ref="BI72:BI90" ca="1" si="3">NOW()</f>
-        <v>44341.506390972223</v>
+        <f t="shared" ref="BI72:BI91" ca="1" si="3">NOW()</f>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ72" s="8" t="s">
         <v>327</v>
@@ -11832,7 +11838,7 @@
       <c r="BH73" s="2"/>
       <c r="BI73" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ73" s="8" t="s">
         <v>327</v>
@@ -11954,7 +11960,7 @@
       <c r="BH74" s="2"/>
       <c r="BI74" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ74" s="8" t="s">
         <v>327</v>
@@ -12069,7 +12075,7 @@
       <c r="BH75" s="2"/>
       <c r="BI75" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ75" s="8" t="s">
         <v>327</v>
@@ -12166,7 +12172,7 @@
       <c r="BH76" s="2"/>
       <c r="BI76" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ76" s="8" t="s">
         <v>327</v>
@@ -12303,7 +12309,7 @@
       <c r="BH77" s="2"/>
       <c r="BI77" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ77" s="8" t="s">
         <v>327</v>
@@ -12395,7 +12401,7 @@
       <c r="BH78" s="2"/>
       <c r="BI78" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ78" s="8" t="s">
         <v>327</v>
@@ -12513,7 +12519,7 @@
       <c r="BH79" s="2"/>
       <c r="BI79" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ79" s="8" t="s">
         <v>327</v>
@@ -12607,7 +12613,7 @@
       <c r="BH80" s="2"/>
       <c r="BI80" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ80" s="8" t="s">
         <v>327</v>
@@ -12741,7 +12747,7 @@
       </c>
       <c r="BI81" s="33">
         <f t="shared" ca="1" si="3"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ81" s="34" t="s">
         <v>327</v>
@@ -12840,7 +12846,7 @@
       <c r="BH82" s="19"/>
       <c r="BI82" s="33">
         <f t="shared" ca="1" si="3"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ82" s="34" t="s">
         <v>327</v>
@@ -12960,7 +12966,7 @@
       <c r="BH83" s="2"/>
       <c r="BI83" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ83" s="8" t="s">
         <v>327</v>
@@ -13057,7 +13063,7 @@
       <c r="BH84" s="2"/>
       <c r="BI84" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ84" s="8" t="s">
         <v>327</v>
@@ -13192,7 +13198,7 @@
       <c r="BH85" s="2"/>
       <c r="BI85" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ85" s="8" t="s">
         <v>327</v>
@@ -13312,7 +13318,7 @@
       <c r="BH86" s="2"/>
       <c r="BI86" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ86" s="8" t="s">
         <v>327</v>
@@ -13352,7 +13358,9 @@
       <c r="K87" s="16">
         <v>44378</v>
       </c>
-      <c r="L87" s="16"/>
+      <c r="L87" s="16">
+        <v>44378</v>
+      </c>
       <c r="M87" s="2">
         <v>12</v>
       </c>
@@ -13428,7 +13436,7 @@
       <c r="BH87" s="2"/>
       <c r="BI87" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ87" s="8" t="s">
         <v>327</v>
@@ -13541,7 +13549,7 @@
       <c r="BH88" s="2"/>
       <c r="BI88" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ88" s="8" t="s">
         <v>327</v>
@@ -13639,7 +13647,7 @@
       <c r="BH89" s="2"/>
       <c r="BI89" s="18">
         <f t="shared" ca="1" si="3"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ89" s="8" t="s">
         <v>327</v>
@@ -13738,14 +13746,109 @@
       <c r="BH90" s="19"/>
       <c r="BI90" s="33">
         <f t="shared" ca="1" si="3"/>
-        <v>44341.506390972223</v>
+        <v>44365.714328240741</v>
       </c>
       <c r="BJ90" s="34" t="s">
         <v>327</v>
       </c>
     </row>
+    <row r="91" spans="1:62" ht="56" x14ac:dyDescent="0.15">
+      <c r="A91" s="2" t="s">
+        <v>660</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>661</v>
+      </c>
+      <c r="D91" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E91" s="6">
+        <v>35000</v>
+      </c>
+      <c r="F91" s="6">
+        <v>35000</v>
+      </c>
+      <c r="G91" s="6">
+        <v>35000</v>
+      </c>
+      <c r="H91" s="36">
+        <v>44358</v>
+      </c>
+      <c r="I91" s="8" t="s">
+        <v>434</v>
+      </c>
+      <c r="J91" s="16">
+        <v>44378</v>
+      </c>
+      <c r="K91" s="16">
+        <v>44743</v>
+      </c>
+      <c r="M91" s="6">
+        <v>12</v>
+      </c>
+      <c r="N91" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="O91" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="P91" s="25" t="s">
+        <v>385</v>
+      </c>
+      <c r="Q91" s="15" t="s">
+        <v>427</v>
+      </c>
+      <c r="R91" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="S91" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="T91" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="U91" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="V91" s="11" t="s">
+        <v>384</v>
+      </c>
+      <c r="W91" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="X91" s="2" t="s">
+        <v>530</v>
+      </c>
+      <c r="AA91" s="6" t="s">
+        <v>529</v>
+      </c>
+      <c r="BA91" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="BB91" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="BE91" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="BF91" s="2"/>
+      <c r="BG91" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="BH91" s="2"/>
+      <c r="BI91" s="18">
+        <f t="shared" ca="1" si="3"/>
+        <v>44365.714328240741</v>
+      </c>
+      <c r="BJ91" s="8" t="s">
+        <v>327</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:BJ87" xr:uid="{AE487DEF-5BC5-C74D-81B1-9FC54E50B3DD}"/>
+  <autoFilter ref="A1:BJ91" xr:uid="{AE487DEF-5BC5-C74D-81B1-9FC54E50B3DD}"/>
   <phoneticPr fontId="12" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="BJ2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
@@ -13893,8 +13996,10 @@
     <hyperlink ref="V89" r:id="rId143" xr:uid="{2E335074-DC5E-9647-92F0-33F6B8E71A09}"/>
     <hyperlink ref="V90" r:id="rId144" xr:uid="{F449B04D-237B-7546-BC43-6E3FC8872799}"/>
     <hyperlink ref="BJ90" r:id="rId145" xr:uid="{F6A2BA07-9F11-2245-A9FE-ED659C43DEAC}"/>
+    <hyperlink ref="I91" r:id="rId146" xr:uid="{F940ECC7-DC95-3C45-BB63-08166F970DE7}"/>
+    <hyperlink ref="BJ91" r:id="rId147" xr:uid="{3C2E58A6-7831-3143-88AB-62D53ED219BB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId146"/>
+  <legacyDrawing r:id="rId148"/>
 </worksheet>
 </file>
</xml_diff>